<commit_message>
Show Emp who does not have Account+ Hide Password
</commit_message>
<xml_diff>
--- a/Tasks.xlsx
+++ b/Tasks.xlsx
@@ -11,12 +11,15 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
+  <definedNames>
+    <definedName name="LOCAL_MYSQL_DATE_FORMAT" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
+  </definedNames>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="66">
   <si>
     <t>Login</t>
   </si>
@@ -108,12 +111,6 @@
     <t>عرض الموظفين الذين ليس لهم حساب فقط في Auto-Complete</t>
   </si>
   <si>
-    <t>عند اختيار موظف من Auto-Complete يتم تعبئة الرقم الوظيفي</t>
-  </si>
-  <si>
-    <t>عند مسح او تغير اسم الموظف يتم مسح او تغيير الرقم الوظيفي</t>
-  </si>
-  <si>
     <t>Encrypt Password</t>
   </si>
   <si>
@@ -178,13 +175,55 @@
   </si>
   <si>
     <t>Update Password</t>
+  </si>
+  <si>
+    <t>Prevent Arabic Char in Username</t>
+  </si>
+  <si>
+    <t>عند اختيار موظف من Auto-Complete يتم تعبئة Primary Key للموظف</t>
+  </si>
+  <si>
+    <t>عند مسح او تغير اسم الموظف يتم مسح او تغيير رقم الموظف</t>
+  </si>
+  <si>
+    <t>Bug</t>
+  </si>
+  <si>
+    <t>عرض الرقم الوظيفي بدلا من ال Primary Key واخفاء ال Primary Key في hdn</t>
+  </si>
+  <si>
+    <t>Fix Number of Filtered Row</t>
+  </si>
+  <si>
+    <t>User Permition</t>
+  </si>
+  <si>
+    <t>Redesign the page</t>
+  </si>
+  <si>
+    <t>Get Users Types</t>
+  </si>
+  <si>
+    <t>عند اختيار نوع المستخدم -&gt; يتم عرض الصلاحيات</t>
+  </si>
+  <si>
+    <t>Get Unpermited Pages</t>
+  </si>
+  <si>
+    <t>Get Permeted Pages</t>
+  </si>
+  <si>
+    <t>Delete Permition onClick Permitied Page</t>
+  </si>
+  <si>
+    <t>Add Permition onClick Unpermited Page</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -223,6 +262,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="5"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -256,14 +303,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -273,15 +314,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -289,12 +321,58 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD7D7D7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+      <tableStyleElement type="wholeTable" dxfId="1"/>
+      <tableStyleElement type="headerRow" dxfId="0"/>
+    </tableStyle>
+  </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -590,584 +668,733 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D62"/>
+  <dimension ref="A1:D78"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="A64" sqref="A64"/>
+    <sheetView tabSelected="1" topLeftCell="A53" workbookViewId="0">
+      <selection activeCell="A68" sqref="A68:XFD68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="3"/>
+    <col min="1" max="1" width="9.140625" style="1"/>
     <col min="2" max="2" width="59" customWidth="1"/>
-    <col min="3" max="3" width="14.5703125" style="5" customWidth="1"/>
+    <col min="3" max="3" width="14.5703125" style="3" customWidth="1"/>
     <col min="4" max="4" width="10.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="3">
+      <c r="A2" s="1">
         <v>1</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="2" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="3">
-        <v>2</v>
-      </c>
-      <c r="B3" s="3" t="s">
+      <c r="A3" s="1">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="3">
+      <c r="A4" s="1">
         <v>3</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="1" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="3">
+      <c r="A5" s="1">
         <v>4</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="1" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="8" t="s">
+      <c r="A7" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="7"/>
-      <c r="C7" s="7"/>
-      <c r="D7" s="7"/>
+      <c r="B7" s="10"/>
+      <c r="C7" s="10"/>
+      <c r="D7" s="10"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="3">
+      <c r="A8" s="1">
         <v>1</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B8" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="4" t="s">
+      <c r="C8" s="2" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="3">
-        <v>2</v>
-      </c>
-      <c r="B9" s="3" t="s">
+      <c r="A9" s="1">
+        <v>2</v>
+      </c>
+      <c r="B9" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="4" t="s">
+      <c r="C9" s="2" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="3">
+      <c r="A10" s="1">
         <v>3</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="B10" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C10" s="4" t="s">
+      <c r="C10" s="2" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="3">
+      <c r="A11" s="1">
         <v>4</v>
       </c>
-      <c r="B11" s="3" t="s">
+      <c r="B11" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C11" s="4" t="s">
+      <c r="C11" s="2" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="3">
+      <c r="A12" s="1">
         <v>5</v>
       </c>
-      <c r="B12" s="3" t="s">
+      <c r="B12" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C12" s="4" t="s">
+      <c r="C12" s="2" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="3">
+      <c r="A13" s="1">
         <v>6</v>
       </c>
-      <c r="B13" s="3" t="s">
+      <c r="B13" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C13" s="4" t="s">
+      <c r="C13" s="2" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="3">
+      <c r="A14" s="1">
         <v>7</v>
       </c>
-      <c r="B14" s="3" t="s">
+      <c r="B14" s="1" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="3">
+      <c r="A15" s="1">
         <v>8</v>
       </c>
-      <c r="B15" s="3" t="s">
+      <c r="B15" s="1" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="8" t="s">
+      <c r="A17" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="B17" s="6"/>
-      <c r="C17" s="6"/>
-      <c r="D17" s="6"/>
+      <c r="B17" s="11"/>
+      <c r="C17" s="11"/>
+      <c r="D17" s="11"/>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="9" t="s">
+      <c r="A18" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="B18" s="10" t="s">
+      <c r="B18" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C18" s="9"/>
-      <c r="D18" s="11"/>
+      <c r="C18" s="4"/>
+      <c r="D18" s="6"/>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="3">
+      <c r="A19" s="1">
         <v>1</v>
       </c>
       <c r="B19" t="s">
         <v>18</v>
       </c>
-      <c r="C19" s="4" t="s">
+      <c r="C19" s="2" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="3">
+      <c r="A20" s="1">
         <v>2</v>
       </c>
       <c r="B20" t="s">
         <v>26</v>
       </c>
-      <c r="C20" s="4" t="s">
+      <c r="C20" s="2" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="3">
+      <c r="A21" s="1">
         <v>3</v>
       </c>
       <c r="B21" t="s">
         <v>19</v>
       </c>
-      <c r="C21" s="4" t="s">
+      <c r="C21" s="2" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="3">
+      <c r="A22" s="1">
         <v>4</v>
       </c>
       <c r="B22" t="s">
         <v>21</v>
       </c>
-      <c r="C22" s="4" t="s">
+      <c r="C22" s="2" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="3">
+      <c r="A23" s="1">
         <v>5</v>
       </c>
       <c r="B23" t="s">
         <v>20</v>
       </c>
-      <c r="C23" s="4" t="s">
+      <c r="C23" s="2" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="3">
+      <c r="A24" s="1">
         <v>6</v>
       </c>
       <c r="B24" t="s">
-        <v>46</v>
-      </c>
-      <c r="C24" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="C24" s="2" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="3">
+      <c r="A25" s="1">
         <v>7</v>
       </c>
       <c r="B25" t="s">
-        <v>47</v>
-      </c>
-      <c r="C25" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="C25" s="2" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="3">
+      <c r="A26" s="1">
         <v>8</v>
       </c>
       <c r="B26" t="s">
         <v>22</v>
       </c>
-      <c r="C26" s="4" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="9" t="s">
+      <c r="C26" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" s="1">
+        <v>9</v>
+      </c>
+      <c r="B27" t="s">
+        <v>57</v>
+      </c>
+      <c r="C27" s="2"/>
+      <c r="D27" s="12" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="B28" s="10" t="s">
+      <c r="B29" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="C28" s="9"/>
-      <c r="D28" s="11"/>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="3">
+      <c r="C29" s="4"/>
+      <c r="D29" s="6"/>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" s="1">
         <v>1</v>
       </c>
-      <c r="B29" t="s">
+      <c r="B30" t="s">
         <v>25</v>
       </c>
-      <c r="C29" s="4" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="3">
-        <v>2</v>
-      </c>
-      <c r="B30" t="s">
+      <c r="C30" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" s="1">
+        <v>2</v>
+      </c>
+      <c r="B31" t="s">
+        <v>31</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" s="1">
+        <v>3</v>
+      </c>
+      <c r="B32" t="s">
+        <v>14</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="1">
+        <v>4</v>
+      </c>
+      <c r="B33" t="s">
+        <v>27</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" s="1">
+        <v>5</v>
+      </c>
+      <c r="B34" t="s">
+        <v>28</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" s="1">
+        <v>6</v>
+      </c>
+      <c r="B35" t="s">
+        <v>29</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" s="1">
+        <v>7</v>
+      </c>
+      <c r="B36" t="s">
+        <v>53</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" s="1">
+        <v>8</v>
+      </c>
+      <c r="B37" t="s">
+        <v>54</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" s="1">
+        <v>9</v>
+      </c>
+      <c r="B38" t="s">
+        <v>30</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" s="1">
+        <v>10</v>
+      </c>
+      <c r="B39" t="s">
+        <v>35</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" s="1">
+        <v>11</v>
+      </c>
+      <c r="B40" t="s">
+        <v>52</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" s="1">
+        <v>11</v>
+      </c>
+      <c r="B41" t="s">
+        <v>32</v>
+      </c>
+      <c r="C41" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42" s="1">
+        <v>12</v>
+      </c>
+      <c r="B42" t="s">
         <v>33</v>
       </c>
-      <c r="C30" s="4" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="3">
+      <c r="C42" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43" s="1">
+        <v>13</v>
+      </c>
+      <c r="B43" t="s">
+        <v>34</v>
+      </c>
+      <c r="C43" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44" s="1">
+        <v>14</v>
+      </c>
+      <c r="B44" t="s">
+        <v>43</v>
+      </c>
+      <c r="C44" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45" s="1">
+        <v>15</v>
+      </c>
+      <c r="B45" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46" s="1">
+        <v>16</v>
+      </c>
+      <c r="B46" t="s">
+        <v>56</v>
+      </c>
+      <c r="C46" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D46" s="12" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A48" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="B48" s="9"/>
+      <c r="C48" s="9"/>
+      <c r="D48" s="9"/>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A49" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B49" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="C49" s="4"/>
+      <c r="D49" s="6"/>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A50" s="1">
+        <v>1</v>
+      </c>
+      <c r="B50" t="s">
+        <v>39</v>
+      </c>
+      <c r="C50" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A51" s="1">
+        <v>2</v>
+      </c>
+      <c r="B51" t="s">
+        <v>26</v>
+      </c>
+      <c r="C51" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A52" s="1">
         <v>3</v>
       </c>
-      <c r="B31" t="s">
+      <c r="B52" t="s">
+        <v>40</v>
+      </c>
+      <c r="C52" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A53" s="1">
+        <v>4</v>
+      </c>
+      <c r="B53" t="s">
+        <v>21</v>
+      </c>
+      <c r="C53" s="2"/>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A54" s="1">
+        <v>5</v>
+      </c>
+      <c r="B54" t="s">
+        <v>57</v>
+      </c>
+      <c r="C54" s="2"/>
+      <c r="D54" s="12" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A56" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B56" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="C56" s="4"/>
+      <c r="D56" s="6"/>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A57" s="1">
+        <v>1</v>
+      </c>
+      <c r="B57" t="s">
+        <v>42</v>
+      </c>
+      <c r="C57" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A58" s="1">
+        <v>2</v>
+      </c>
+      <c r="B58" t="s">
+        <v>31</v>
+      </c>
+      <c r="C58" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A59" s="1">
+        <v>3</v>
+      </c>
+      <c r="B59" t="s">
         <v>14</v>
       </c>
-      <c r="C31" s="4" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="3">
+      <c r="C59" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A60" s="1">
         <v>4</v>
       </c>
-      <c r="B32" t="s">
-        <v>27</v>
-      </c>
-      <c r="C32" s="4" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="3">
+      <c r="B60" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A61" s="1">
         <v>5</v>
       </c>
-      <c r="B33" t="s">
-        <v>28</v>
-      </c>
-      <c r="C33" s="4" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" s="3">
+      <c r="B61" t="s">
+        <v>47</v>
+      </c>
+      <c r="C61" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A62" s="1">
         <v>6</v>
       </c>
-      <c r="B34" t="s">
-        <v>29</v>
-      </c>
-      <c r="C34" s="4"/>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" s="3">
+      <c r="B62" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A63" s="1">
         <v>7</v>
       </c>
-      <c r="B35" t="s">
-        <v>30</v>
-      </c>
-      <c r="C35" s="4" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" s="3">
+      <c r="B63" t="s">
+        <v>43</v>
+      </c>
+      <c r="C63" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A64" s="1">
         <v>8</v>
       </c>
-      <c r="B36" t="s">
-        <v>31</v>
-      </c>
-      <c r="C36" s="4" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" s="3">
-        <v>9</v>
-      </c>
-      <c r="B37" t="s">
-        <v>32</v>
-      </c>
-      <c r="C37" s="4" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38" s="3">
-        <v>10</v>
-      </c>
-      <c r="B38" t="s">
-        <v>37</v>
-      </c>
-      <c r="C38" s="4"/>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" s="3">
-        <v>11</v>
-      </c>
-      <c r="B39" t="s">
-        <v>34</v>
-      </c>
-      <c r="C39" s="4" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A40" s="3">
-        <v>12</v>
-      </c>
-      <c r="B40" t="s">
-        <v>35</v>
-      </c>
-      <c r="C40" s="4" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A41" s="3">
-        <v>13</v>
-      </c>
-      <c r="B41" t="s">
+      <c r="B64" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A42" s="3">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A66" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="B66" s="9"/>
+      <c r="C66" s="9"/>
+      <c r="D66" s="9"/>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A67" s="1">
+        <v>1</v>
+      </c>
+      <c r="B67" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A68" s="1">
+        <v>2</v>
+      </c>
+      <c r="B68" t="s">
         <v>14</v>
       </c>
-      <c r="B42" t="s">
-        <v>45</v>
-      </c>
-      <c r="C42" s="4" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A43" s="3">
-        <v>15</v>
-      </c>
-      <c r="B43" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A45" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="B45" s="8"/>
-      <c r="C45" s="8"/>
-      <c r="D45" s="8"/>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A46" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="B46" s="10" t="s">
-        <v>40</v>
-      </c>
-      <c r="C46" s="9"/>
-      <c r="D46" s="11"/>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A47" s="3">
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A69" s="1">
+        <v>3</v>
+      </c>
+      <c r="B69" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A71" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="B71" s="9"/>
+      <c r="C71" s="9"/>
+      <c r="D71" s="9"/>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A72" s="1">
         <v>1</v>
       </c>
-      <c r="B47" t="s">
-        <v>41</v>
-      </c>
-      <c r="C47" s="4" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A48" s="3">
-        <v>2</v>
-      </c>
-      <c r="B48" t="s">
-        <v>26</v>
-      </c>
-      <c r="C48" s="4" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A49" s="3">
+      <c r="B72" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A73" s="1">
+        <v>2</v>
+      </c>
+      <c r="B73" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A74" s="1">
         <v>3</v>
       </c>
-      <c r="B49" t="s">
-        <v>42</v>
-      </c>
-      <c r="C49" s="4" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A51" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="B51" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="C51" s="9"/>
-      <c r="D51" s="11"/>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A52" s="3">
-        <v>1</v>
-      </c>
-      <c r="B52" t="s">
-        <v>44</v>
-      </c>
-      <c r="C52" s="4" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A53" s="3">
-        <v>2</v>
-      </c>
-      <c r="B53" t="s">
-        <v>33</v>
-      </c>
-      <c r="C53" s="4" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A54" s="3">
-        <v>3</v>
-      </c>
-      <c r="B54" t="s">
-        <v>14</v>
-      </c>
-      <c r="C54" s="4" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A55" s="3">
+      <c r="B74" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A75" s="1">
         <v>4</v>
       </c>
-      <c r="B55" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A56" s="3">
+      <c r="B75" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A76" s="1">
         <v>5</v>
       </c>
-      <c r="B56" t="s">
-        <v>49</v>
-      </c>
-      <c r="C56" s="4" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A57" s="3">
+      <c r="B76" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A77" s="1">
         <v>6</v>
       </c>
-      <c r="B57" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A59" s="8" t="s">
-        <v>51</v>
-      </c>
-      <c r="B59" s="8"/>
-      <c r="C59" s="8"/>
-      <c r="D59" s="8"/>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A60" s="3">
-        <v>1</v>
-      </c>
-      <c r="B60" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A61" s="3">
-        <v>2</v>
-      </c>
-      <c r="B61" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A62" s="3">
-        <v>3</v>
-      </c>
-      <c r="B62" t="s">
-        <v>53</v>
+      <c r="B77" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A78" s="1">
+        <v>7</v>
+      </c>
+      <c r="B78" t="s">
+        <v>64</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="6">
+    <mergeCell ref="A71:D71"/>
     <mergeCell ref="A1:D1"/>
     <mergeCell ref="A7:D7"/>
     <mergeCell ref="A17:D17"/>
-    <mergeCell ref="A45:D45"/>
-    <mergeCell ref="A59:D59"/>
+    <mergeCell ref="A48:D48"/>
+    <mergeCell ref="A66:D66"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
fix employee flter search count
</commit_message>
<xml_diff>
--- a/Tasks.xlsx
+++ b/Tasks.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="66">
   <si>
     <t>Login</t>
   </si>
@@ -671,7 +671,7 @@
   <dimension ref="A1:D78"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A39" workbookViewId="0">
-      <selection activeCell="C62" sqref="C62"/>
+      <selection activeCell="C54" sqref="C54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1197,7 +1197,9 @@
       <c r="B54" t="s">
         <v>57</v>
       </c>
-      <c r="C54" s="2"/>
+      <c r="C54" s="2" t="s">
+        <v>2</v>
+      </c>
       <c r="D54" s="7" t="s">
         <v>55</v>
       </c>

</xml_diff>

<commit_message>
Insert & Delete User Type Permission
</commit_message>
<xml_diff>
--- a/Tasks.xlsx
+++ b/Tasks.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="66">
   <si>
     <t>Login</t>
   </si>
@@ -671,7 +671,7 @@
   <dimension ref="A1:D78"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A56" workbookViewId="0">
-      <selection activeCell="C74" sqref="C74"/>
+      <selection activeCell="C64" sqref="C64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1398,6 +1398,9 @@
       <c r="B77" t="s">
         <v>65</v>
       </c>
+      <c r="C77" s="2" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" s="1">
@@ -1405,6 +1408,9 @@
       </c>
       <c r="B78" t="s">
         <v>64</v>
+      </c>
+      <c r="C78" s="2" t="s">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add Recommendation to Survey
</commit_message>
<xml_diff>
--- a/Tasks.xlsx
+++ b/Tasks.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505"/>
+    <workbookView xWindow="480" yWindow="120" windowWidth="18195" windowHeight="8445"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -15,11 +15,12 @@
     <definedName name="LOCAL_MYSQL_DATE_FORMAT" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
   </definedNames>
   <calcPr calcId="144525"/>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="317" uniqueCount="163">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="481" uniqueCount="233">
   <si>
     <t>Login</t>
   </si>
@@ -871,9 +872,6 @@
     <t>Change DB (Create Master Table for Elder Disease)</t>
   </si>
   <si>
-    <t>Add Elder Desiease Details</t>
-  </si>
-  <si>
     <t>If Elder_Desiease_Id (Master) IS NOT EXIST Insert Elder_Desiease</t>
   </si>
   <si>
@@ -883,9 +881,6 @@
     <t>Disable Inserted Disease &amp; Enable Inserted Disease</t>
   </si>
   <si>
-    <t>Add Elder Disease Det وصف الحالة المرضية</t>
-  </si>
-  <si>
     <t>If Elder_Desiease_Id (Master) IS EXIST Update  وصف الحالة المرضية</t>
   </si>
   <si>
@@ -926,6 +921,222 @@
   </si>
   <si>
     <t>Step 4: Elder Room</t>
+  </si>
+  <si>
+    <t>Change DB (Add organization_id column)</t>
+  </si>
+  <si>
+    <t>Add Income Details (If income_id "Master"  IS NOT EXIST Add income_resource)</t>
+  </si>
+  <si>
+    <t>Delete Income Details</t>
+  </si>
+  <si>
+    <t>Disable Inserted resource except (NGOs)</t>
+  </si>
+  <si>
+    <t>Enable Deleted resource</t>
+  </si>
+  <si>
+    <t>When NGOs selected -&gt; NGO Drplst Appear</t>
+  </si>
+  <si>
+    <t>Add Income resource (Master) اجمالي الدخل + حصة المسن</t>
+  </si>
+  <si>
+    <t>Update Income resource (Master) اجمالي الدخل + حصة المسن</t>
+  </si>
+  <si>
+    <t>Drow Total Row at the end of the table</t>
+  </si>
+  <si>
+    <t>Create Drow Fun in Controler</t>
+  </si>
+  <si>
+    <t>Change DB دمج الحاجة الى صيانة والحاجة الى ترميم في حقل واحد للغرفة والحمام</t>
+  </si>
+  <si>
+    <t xml:space="preserve">اظهار حقل تحديد نوع الصيانة والترميم في حال كانت الغرفة بحاجة الى صيانة </t>
+  </si>
+  <si>
+    <t xml:space="preserve">اظهار حقل تحديد نوع الصيانة والترميم في حال كانت الحمام بحاجة الى صيانة </t>
+  </si>
+  <si>
+    <t>Insert Elder Desiease Details</t>
+  </si>
+  <si>
+    <t>Insert Elder Disease Det وصف الحالة المرضية</t>
+  </si>
+  <si>
+    <t>Insert Elder Room</t>
+  </si>
+  <si>
+    <t>Update Elder Room</t>
+  </si>
+  <si>
+    <t>VIII</t>
+  </si>
+  <si>
+    <t>Step 4: Elder Medication</t>
+  </si>
+  <si>
+    <t>Insert Medication Availability</t>
+  </si>
+  <si>
+    <t>Delete Medication Availability</t>
+  </si>
+  <si>
+    <t>Insert Medication Needs</t>
+  </si>
+  <si>
+    <t>Delete Medication Needs</t>
+  </si>
+  <si>
+    <t>Disable Inserted Need</t>
+  </si>
+  <si>
+    <t>IX</t>
+  </si>
+  <si>
+    <t>Change DB (no_provision_needs,legal_advice,legal_advice_reason)</t>
+  </si>
+  <si>
+    <t>Step 4: Family Elder Relationship</t>
+  </si>
+  <si>
+    <t>Insert Family_Elder_Relationship</t>
+  </si>
+  <si>
+    <t>Update Family_Elder_Relationship</t>
+  </si>
+  <si>
+    <t>Make no provision needs Visible "عند اختيار توفير الاحتيادات = لا"</t>
+  </si>
+  <si>
+    <t>Make legal advice reason Visible "عند اختيار الحاجة الى عيادة قان ونية=نعم"</t>
+  </si>
+  <si>
+    <t>X</t>
+  </si>
+  <si>
+    <t>Step 4: Elder Behaviour</t>
+  </si>
+  <si>
+    <t>Change DB (elder_pariah_tb)</t>
+  </si>
+  <si>
+    <t>Insert Elder Behaviour</t>
+  </si>
+  <si>
+    <t>If Behaviour = pariah SHOW Reason Div</t>
+  </si>
+  <si>
+    <t>Insert pariah reason</t>
+  </si>
+  <si>
+    <t>Disable Inserted pariah reason</t>
+  </si>
+  <si>
+    <t>Disable Inserted Elder Behaviour</t>
+  </si>
+  <si>
+    <t>Delete pariah reason</t>
+  </si>
+  <si>
+    <t>Enable Deleted pariah reason</t>
+  </si>
+  <si>
+    <t>Delete Elder Behaviour</t>
+  </si>
+  <si>
+    <t>If Deleted Behaviour = pariah Delete Reason + Hide Div</t>
+  </si>
+  <si>
+    <t>Enable Deleted Elder Behaviour</t>
+  </si>
+  <si>
+    <t>XI</t>
+  </si>
+  <si>
+    <t>Step 4: Family Psycho</t>
+  </si>
+  <si>
+    <t>Insert Family Psycho</t>
+  </si>
+  <si>
+    <t>Disable Inserted Family Psycho</t>
+  </si>
+  <si>
+    <t>Delete Family Psycho</t>
+  </si>
+  <si>
+    <t>Enable Inserted Family Psycho</t>
+  </si>
+  <si>
+    <t>XII</t>
+  </si>
+  <si>
+    <t>Step 4: Life Improvement</t>
+  </si>
+  <si>
+    <t>Fix DB Error (Family Member Id FK Sub Constant)</t>
+  </si>
+  <si>
+    <t>Insert Life Improvement</t>
+  </si>
+  <si>
+    <t>Update Life Improvement</t>
+  </si>
+  <si>
+    <t>XIII</t>
+  </si>
+  <si>
+    <t>Step 4: Aids Recommendation</t>
+  </si>
+  <si>
+    <t>Insert Aids Recommendations</t>
+  </si>
+  <si>
+    <t>Update Aids Recommendations</t>
+  </si>
+  <si>
+    <t>Insert Medical Aids Recommendations</t>
+  </si>
+  <si>
+    <t>Delete Medical Aids Recommendations</t>
+  </si>
+  <si>
+    <t>Disable Inserted Medical Aids Recommendations</t>
+  </si>
+  <si>
+    <t>Enable Deleted Medical Aids Recommendations</t>
+  </si>
+  <si>
+    <t>Insert Home Aids Recommendations</t>
+  </si>
+  <si>
+    <t>Disable Inserted Home Aids Recommendations</t>
+  </si>
+  <si>
+    <t>Delete Home Aids Recommendations</t>
+  </si>
+  <si>
+    <t>Enable Deleted Home Aids Recommendations</t>
+  </si>
+  <si>
+    <t>تعديل دعم نفسي  الى تكست</t>
+  </si>
+  <si>
+    <t>تعديل دعم اجتماعي الى تكست</t>
+  </si>
+  <si>
+    <t>تعديل ترفيه الى تكست</t>
+  </si>
+  <si>
+    <t>اضافة حقل Details لوضع الاجار وتفاصيل اشياء اخرى في جدول Home Aids Recommendations</t>
+  </si>
+  <si>
+    <t>اظهار حقل Details عند اختيار الاجار أواشياء اخرى</t>
   </si>
 </sst>
 </file>
@@ -1405,16 +1616,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D194"/>
+  <dimension ref="A1:D291"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A184" workbookViewId="0">
-      <selection activeCell="B194" sqref="B194"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="1"/>
-    <col min="2" max="2" width="59" customWidth="1"/>
+    <col min="2" max="2" width="60.140625" customWidth="1"/>
     <col min="3" max="3" width="14.5703125" style="3" customWidth="1"/>
     <col min="4" max="4" width="10.85546875" customWidth="1"/>
   </cols>
@@ -1540,7 +1751,7 @@
       <c r="A14" s="1">
         <v>7</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="B14" s="3" t="s">
         <v>12</v>
       </c>
     </row>
@@ -3019,7 +3230,7 @@
         <v>3</v>
       </c>
       <c r="B168" t="s">
-        <v>144</v>
+        <v>174</v>
       </c>
       <c r="C168" s="2" t="s">
         <v>2</v>
@@ -3030,7 +3241,7 @@
         <v>4</v>
       </c>
       <c r="B169" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C169" s="2" t="s">
         <v>2</v>
@@ -3041,7 +3252,7 @@
         <v>5</v>
       </c>
       <c r="B170" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C170" s="2" t="s">
         <v>2</v>
@@ -3052,7 +3263,7 @@
         <v>6</v>
       </c>
       <c r="B171" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C171" s="2" t="s">
         <v>2</v>
@@ -3063,7 +3274,7 @@
         <v>7</v>
       </c>
       <c r="B172" t="s">
-        <v>148</v>
+        <v>175</v>
       </c>
       <c r="C172" s="2" t="s">
         <v>2</v>
@@ -3074,7 +3285,7 @@
         <v>8</v>
       </c>
       <c r="B173" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="C173" s="2" t="s">
         <v>2</v>
@@ -3114,33 +3325,53 @@
     </row>
     <row r="178" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A178" s="4" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B178" s="5" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="C178" s="4"/>
       <c r="D178" s="6"/>
     </row>
     <row r="179" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C179" s="2"/>
+      <c r="A179" s="1">
+        <v>1</v>
+      </c>
+      <c r="B179" t="s">
+        <v>125</v>
+      </c>
+      <c r="C179" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="180" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A180" s="1">
+        <v>2</v>
+      </c>
+      <c r="B180" t="s">
+        <v>161</v>
+      </c>
+      <c r="C180" s="2" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="181" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A181" s="4" t="s">
-        <v>159</v>
-      </c>
-      <c r="B181" s="5" t="s">
-        <v>151</v>
-      </c>
-      <c r="C181" s="4"/>
-      <c r="D181" s="6"/>
+      <c r="A181" s="1">
+        <v>3</v>
+      </c>
+      <c r="B181" t="s">
+        <v>162</v>
+      </c>
+      <c r="C181" s="2" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="182" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A182" s="1">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="B182" t="s">
-        <v>152</v>
+        <v>164</v>
       </c>
       <c r="C182" s="2" t="s">
         <v>2</v>
@@ -3148,10 +3379,10 @@
     </row>
     <row r="183" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A183" s="1">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="B183" t="s">
-        <v>153</v>
+        <v>166</v>
       </c>
       <c r="C183" s="2" t="s">
         <v>2</v>
@@ -3159,10 +3390,10 @@
     </row>
     <row r="184" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A184" s="1">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="B184" t="s">
-        <v>154</v>
+        <v>163</v>
       </c>
       <c r="C184" s="2" t="s">
         <v>2</v>
@@ -3170,10 +3401,10 @@
     </row>
     <row r="185" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A185" s="1">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="B185" t="s">
-        <v>155</v>
+        <v>170</v>
       </c>
       <c r="C185" s="2" t="s">
         <v>2</v>
@@ -3181,10 +3412,10 @@
     </row>
     <row r="186" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A186" s="1">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="B186" t="s">
-        <v>156</v>
+        <v>169</v>
       </c>
       <c r="C186" s="2" t="s">
         <v>2</v>
@@ -3192,10 +3423,10 @@
     </row>
     <row r="187" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A187" s="1">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B187" t="s">
-        <v>157</v>
+        <v>165</v>
       </c>
       <c r="C187" s="2" t="s">
         <v>2</v>
@@ -3203,10 +3434,10 @@
     </row>
     <row r="188" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A188" s="1">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="B188" t="s">
-        <v>158</v>
+        <v>167</v>
       </c>
       <c r="C188" s="2" t="s">
         <v>2</v>
@@ -3214,10 +3445,10 @@
     </row>
     <row r="189" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A189" s="1">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="B189" t="s">
-        <v>14</v>
+        <v>168</v>
       </c>
       <c r="C189" s="2" t="s">
         <v>2</v>
@@ -3225,33 +3456,968 @@
     </row>
     <row r="190" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A190" s="1">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="B190" t="s">
-        <v>77</v>
+        <v>14</v>
+      </c>
+      <c r="C190" s="2" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="191" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A191" s="1">
+        <v>13</v>
+      </c>
+      <c r="B191" t="s">
+        <v>77</v>
+      </c>
+      <c r="C191" s="2"/>
+    </row>
+    <row r="192" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A192" s="1">
+        <v>14</v>
+      </c>
+      <c r="B192" t="s">
+        <v>78</v>
+      </c>
+      <c r="C192" s="2"/>
+    </row>
+    <row r="194" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A194" s="4" t="s">
+        <v>157</v>
+      </c>
+      <c r="B194" s="5" t="s">
+        <v>149</v>
+      </c>
+      <c r="C194" s="4"/>
+      <c r="D194" s="6"/>
+    </row>
+    <row r="195" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A195" s="1">
+        <v>1</v>
+      </c>
+      <c r="B195" t="s">
+        <v>150</v>
+      </c>
+      <c r="C195" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="196" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A196" s="1">
+        <v>2</v>
+      </c>
+      <c r="B196" t="s">
+        <v>151</v>
+      </c>
+      <c r="C196" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="197" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A197" s="1">
+        <v>3</v>
+      </c>
+      <c r="B197" t="s">
+        <v>152</v>
+      </c>
+      <c r="C197" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="198" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A198" s="1">
+        <v>4</v>
+      </c>
+      <c r="B198" t="s">
+        <v>153</v>
+      </c>
+      <c r="C198" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="199" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A199" s="1">
+        <v>5</v>
+      </c>
+      <c r="B199" t="s">
+        <v>154</v>
+      </c>
+      <c r="C199" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="200" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A200" s="1">
+        <v>6</v>
+      </c>
+      <c r="B200" t="s">
+        <v>155</v>
+      </c>
+      <c r="C200" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="201" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A201" s="1">
+        <v>7</v>
+      </c>
+      <c r="B201" t="s">
+        <v>156</v>
+      </c>
+      <c r="C201" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="202" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A202" s="1">
+        <v>8</v>
+      </c>
+      <c r="B202" t="s">
+        <v>14</v>
+      </c>
+      <c r="C202" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="203" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A203" s="1">
+        <v>9</v>
+      </c>
+      <c r="B203" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="204" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A204" s="1">
         <v>10</v>
       </c>
-      <c r="B191" t="s">
+      <c r="B204" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="193" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A193" s="4" t="s">
-        <v>161</v>
-      </c>
-      <c r="B193" s="5" t="s">
-        <v>162</v>
-      </c>
-      <c r="C193" s="4"/>
-      <c r="D193" s="6"/>
-    </row>
-    <row r="194" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A194" s="1">
+    <row r="206" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A206" s="4" t="s">
+        <v>159</v>
+      </c>
+      <c r="B206" s="5" t="s">
+        <v>160</v>
+      </c>
+      <c r="C206" s="4"/>
+      <c r="D206" s="6"/>
+    </row>
+    <row r="207" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A207" s="1">
         <v>1</v>
+      </c>
+      <c r="B207" t="s">
+        <v>171</v>
+      </c>
+      <c r="C207" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="208" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A208" s="1">
+        <v>2</v>
+      </c>
+      <c r="B208" t="s">
+        <v>172</v>
+      </c>
+      <c r="C208" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="209" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A209" s="1">
+        <v>3</v>
+      </c>
+      <c r="B209" t="s">
+        <v>173</v>
+      </c>
+      <c r="C209" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="210" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A210" s="1">
+        <v>4</v>
+      </c>
+      <c r="B210" t="s">
+        <v>176</v>
+      </c>
+      <c r="C210" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="211" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A211" s="1">
+        <v>5</v>
+      </c>
+      <c r="B211" t="s">
+        <v>177</v>
+      </c>
+      <c r="C211" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="212" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A212" s="1">
+        <v>6</v>
+      </c>
+      <c r="B212" t="s">
+        <v>14</v>
+      </c>
+      <c r="C212" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="213" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A213" s="1">
+        <v>7</v>
+      </c>
+      <c r="B213" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="214" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A214" s="1">
+        <v>8</v>
+      </c>
+      <c r="B214" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="215" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C215" s="2"/>
+    </row>
+    <row r="216" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A216" s="4" t="s">
+        <v>178</v>
+      </c>
+      <c r="B216" s="5" t="s">
+        <v>179</v>
+      </c>
+      <c r="C216" s="4"/>
+      <c r="D216" s="6"/>
+    </row>
+    <row r="217" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A217" s="1">
+        <v>1</v>
+      </c>
+      <c r="B217" t="s">
+        <v>125</v>
+      </c>
+      <c r="C217" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="218" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A218" s="1">
+        <v>2</v>
+      </c>
+      <c r="B218" t="s">
+        <v>180</v>
+      </c>
+      <c r="C218" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="219" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A219" s="1">
+        <v>3</v>
+      </c>
+      <c r="B219" t="s">
+        <v>181</v>
+      </c>
+      <c r="C219" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="220" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A220" s="1">
+        <v>4</v>
+      </c>
+      <c r="B220" t="s">
+        <v>182</v>
+      </c>
+      <c r="C220" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="221" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A221" s="1">
+        <v>5</v>
+      </c>
+      <c r="B221" t="s">
+        <v>183</v>
+      </c>
+      <c r="C221" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="222" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A222" s="1">
+        <v>6</v>
+      </c>
+      <c r="B222" t="s">
+        <v>184</v>
+      </c>
+      <c r="C222" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="223" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A223" s="1">
+        <v>7</v>
+      </c>
+      <c r="B223" t="s">
+        <v>14</v>
+      </c>
+      <c r="C223" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="224" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A224" s="1">
+        <v>8</v>
+      </c>
+      <c r="B224" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="225" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A225" s="1">
+        <v>9</v>
+      </c>
+      <c r="B225" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="227" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A227" s="4" t="s">
+        <v>185</v>
+      </c>
+      <c r="B227" s="5" t="s">
+        <v>187</v>
+      </c>
+      <c r="C227" s="4"/>
+      <c r="D227" s="6"/>
+    </row>
+    <row r="228" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A228" s="1">
+        <v>1</v>
+      </c>
+      <c r="B228" t="s">
+        <v>186</v>
+      </c>
+      <c r="C228" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="229" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A229" s="1">
+        <v>2</v>
+      </c>
+      <c r="B229" t="s">
+        <v>188</v>
+      </c>
+      <c r="C229" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="230" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A230" s="1">
+        <v>3</v>
+      </c>
+      <c r="B230" t="s">
+        <v>189</v>
+      </c>
+      <c r="C230" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="231" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A231" s="1">
+        <v>4</v>
+      </c>
+      <c r="B231" t="s">
+        <v>190</v>
+      </c>
+      <c r="C231" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="232" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A232" s="1">
+        <v>5</v>
+      </c>
+      <c r="B232" t="s">
+        <v>191</v>
+      </c>
+      <c r="C232" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="233" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A233" s="1">
+        <v>6</v>
+      </c>
+      <c r="B233" t="s">
+        <v>14</v>
+      </c>
+      <c r="C233" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="234" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A234" s="1">
+        <v>7</v>
+      </c>
+      <c r="B234" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="235" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A235" s="1">
+        <v>8</v>
+      </c>
+      <c r="B235" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="237" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A237" s="4" t="s">
+        <v>192</v>
+      </c>
+      <c r="B237" s="5" t="s">
+        <v>193</v>
+      </c>
+      <c r="C237" s="4"/>
+      <c r="D237" s="6"/>
+    </row>
+    <row r="238" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A238" s="1">
+        <v>1</v>
+      </c>
+      <c r="B238" t="s">
+        <v>125</v>
+      </c>
+      <c r="C238" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="239" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A239" s="1">
+        <v>2</v>
+      </c>
+      <c r="B239" t="s">
+        <v>194</v>
+      </c>
+      <c r="C239" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="240" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A240" s="1">
+        <v>3</v>
+      </c>
+      <c r="B240" t="s">
+        <v>195</v>
+      </c>
+      <c r="C240" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="241" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A241" s="1">
+        <v>4</v>
+      </c>
+      <c r="B241" t="s">
+        <v>199</v>
+      </c>
+      <c r="C241" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="242" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A242" s="1">
+        <v>5</v>
+      </c>
+      <c r="B242" t="s">
+        <v>196</v>
+      </c>
+      <c r="C242" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="243" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A243" s="1">
+        <v>6</v>
+      </c>
+      <c r="B243" t="s">
+        <v>197</v>
+      </c>
+      <c r="C243" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="244" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A244" s="1">
+        <v>7</v>
+      </c>
+      <c r="B244" t="s">
+        <v>198</v>
+      </c>
+      <c r="C244" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="245" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A245" s="1">
+        <v>8</v>
+      </c>
+      <c r="B245" t="s">
+        <v>200</v>
+      </c>
+      <c r="C245" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="246" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A246" s="1">
+        <v>9</v>
+      </c>
+      <c r="B246" t="s">
+        <v>201</v>
+      </c>
+      <c r="C246" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="247" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A247" s="1">
+        <v>10</v>
+      </c>
+      <c r="B247" t="s">
+        <v>202</v>
+      </c>
+      <c r="C247" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="248" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A248" s="1">
+        <v>11</v>
+      </c>
+      <c r="B248" t="s">
+        <v>203</v>
+      </c>
+      <c r="C248" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="249" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A249" s="1">
+        <v>12</v>
+      </c>
+      <c r="B249" t="s">
+        <v>204</v>
+      </c>
+      <c r="C249" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="250" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A250" s="1">
+        <v>13</v>
+      </c>
+      <c r="B250" t="s">
+        <v>14</v>
+      </c>
+      <c r="C250" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="251" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A251" s="1">
+        <v>14</v>
+      </c>
+      <c r="B251" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="252" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A252" s="1">
+        <v>15</v>
+      </c>
+      <c r="B252" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="254" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A254" s="4" t="s">
+        <v>205</v>
+      </c>
+      <c r="B254" s="5" t="s">
+        <v>206</v>
+      </c>
+      <c r="C254" s="4"/>
+      <c r="D254" s="6"/>
+    </row>
+    <row r="255" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A255" s="1">
+        <v>1</v>
+      </c>
+      <c r="B255" t="s">
+        <v>125</v>
+      </c>
+      <c r="C255" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="256" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A256" s="1">
+        <v>2</v>
+      </c>
+      <c r="B256" t="s">
+        <v>207</v>
+      </c>
+      <c r="C256" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="257" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A257" s="1">
+        <v>3</v>
+      </c>
+      <c r="B257" t="s">
+        <v>208</v>
+      </c>
+      <c r="C257" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="258" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A258" s="1">
+        <v>4</v>
+      </c>
+      <c r="B258" t="s">
+        <v>209</v>
+      </c>
+      <c r="C258" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="259" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A259" s="1">
+        <v>5</v>
+      </c>
+      <c r="B259" t="s">
+        <v>210</v>
+      </c>
+      <c r="C259" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="260" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A260" s="1">
+        <v>6</v>
+      </c>
+      <c r="B260" t="s">
+        <v>14</v>
+      </c>
+      <c r="C260" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="261" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A261" s="1">
+        <v>7</v>
+      </c>
+      <c r="B261" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="262" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A262" s="1">
+        <v>8</v>
+      </c>
+      <c r="B262" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="264" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A264" s="4" t="s">
+        <v>211</v>
+      </c>
+      <c r="B264" s="5" t="s">
+        <v>212</v>
+      </c>
+      <c r="C264" s="4"/>
+      <c r="D264" s="6"/>
+    </row>
+    <row r="265" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A265" s="1">
+        <v>1</v>
+      </c>
+      <c r="B265" t="s">
+        <v>213</v>
+      </c>
+      <c r="C265" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="266" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A266" s="1">
+        <v>2</v>
+      </c>
+      <c r="B266" t="s">
+        <v>214</v>
+      </c>
+      <c r="C266" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="267" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A267" s="1">
+        <v>3</v>
+      </c>
+      <c r="B267" t="s">
+        <v>215</v>
+      </c>
+      <c r="C267" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="268" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A268" s="1">
+        <v>4</v>
+      </c>
+      <c r="B268" t="s">
+        <v>14</v>
+      </c>
+      <c r="C268" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="269" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A269" s="1">
+        <v>5</v>
+      </c>
+      <c r="B269" t="s">
+        <v>77</v>
+      </c>
+      <c r="C269" s="2"/>
+    </row>
+    <row r="270" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A270" s="1">
+        <v>6</v>
+      </c>
+      <c r="B270" t="s">
+        <v>78</v>
+      </c>
+      <c r="C270" s="2"/>
+    </row>
+    <row r="272" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A272" s="4" t="s">
+        <v>216</v>
+      </c>
+      <c r="B272" s="5" t="s">
+        <v>217</v>
+      </c>
+      <c r="C272" s="4"/>
+      <c r="D272" s="6"/>
+    </row>
+    <row r="273" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A273" s="1">
+        <v>1</v>
+      </c>
+      <c r="B273" t="s">
+        <v>125</v>
+      </c>
+      <c r="C273" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="274" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A274" s="1">
+        <v>2</v>
+      </c>
+      <c r="B274" t="s">
+        <v>218</v>
+      </c>
+      <c r="C274" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="275" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A275" s="1">
+        <v>3</v>
+      </c>
+      <c r="B275" t="s">
+        <v>219</v>
+      </c>
+      <c r="C275" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="276" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A276" s="1">
+        <v>4</v>
+      </c>
+      <c r="B276" t="s">
+        <v>220</v>
+      </c>
+      <c r="C276" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="277" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A277" s="1">
+        <v>5</v>
+      </c>
+      <c r="B277" t="s">
+        <v>222</v>
+      </c>
+      <c r="C277" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="278" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A278" s="1">
+        <v>6</v>
+      </c>
+      <c r="B278" t="s">
+        <v>221</v>
+      </c>
+      <c r="C278" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="279" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A279" s="1">
+        <v>7</v>
+      </c>
+      <c r="B279" t="s">
+        <v>223</v>
+      </c>
+      <c r="C279" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="280" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A280" s="1">
+        <v>8</v>
+      </c>
+      <c r="B280" t="s">
+        <v>224</v>
+      </c>
+      <c r="C280" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="281" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A281" s="1">
+        <v>9</v>
+      </c>
+      <c r="B281" t="s">
+        <v>225</v>
+      </c>
+      <c r="C281" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="282" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A282" s="1">
+        <v>10</v>
+      </c>
+      <c r="B282" t="s">
+        <v>226</v>
+      </c>
+      <c r="C282" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="283" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A283" s="1">
+        <v>11</v>
+      </c>
+      <c r="B283" t="s">
+        <v>227</v>
+      </c>
+      <c r="C283" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="284" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A284" s="1">
+        <v>12</v>
+      </c>
+      <c r="B284" t="s">
+        <v>228</v>
+      </c>
+      <c r="C284" s="2"/>
+    </row>
+    <row r="285" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A285" s="1">
+        <v>13</v>
+      </c>
+      <c r="B285" t="s">
+        <v>229</v>
+      </c>
+      <c r="C285" s="2"/>
+    </row>
+    <row r="286" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A286" s="1">
+        <v>14</v>
+      </c>
+      <c r="B286" t="s">
+        <v>230</v>
+      </c>
+      <c r="C286" s="2"/>
+    </row>
+    <row r="287" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A287" s="1">
+        <v>15</v>
+      </c>
+      <c r="B287" t="s">
+        <v>231</v>
+      </c>
+      <c r="C287" s="2"/>
+    </row>
+    <row r="288" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A288" s="1">
+        <v>16</v>
+      </c>
+      <c r="B288" t="s">
+        <v>232</v>
+      </c>
+      <c r="C288" s="2"/>
+    </row>
+    <row r="289" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A289" s="1">
+        <v>17</v>
+      </c>
+      <c r="B289" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="290" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A290" s="1">
+        <v>18</v>
+      </c>
+      <c r="B290" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="291" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A291" s="1">
+        <v>19</v>
+      </c>
+      <c r="B291" t="s">
+        <v>78</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fix Elder & Elder File - Not complete
</commit_message>
<xml_diff>
--- a/Tasks.xlsx
+++ b/Tasks.xlsx
@@ -15,11 +15,12 @@
     <definedName name="LOCAL_MYSQL_DATE_FORMAT" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
   </definedNames>
   <calcPr calcId="144525"/>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="482" uniqueCount="233">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="495" uniqueCount="236">
   <si>
     <t>Login</t>
   </si>
@@ -1136,6 +1137,15 @@
   </si>
   <si>
     <t>اظهار حقل Details عند اختيار الاجار أواشياء اخرى</t>
+  </si>
+  <si>
+    <t>منع الاضافة في حال كان العضو له استبانة (ممكن تحويله على صفحة تعديل الاستبانة)</t>
+  </si>
+  <si>
+    <t>اضافة زر تعديل بيانات العائلة وربطه بالصفحة العائلة</t>
+  </si>
+  <si>
+    <t>عند فتح الصفحة لا تظهر ملفات العضو المدخلة من قبل</t>
   </si>
 </sst>
 </file>
@@ -1615,10 +1625,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D291"/>
+  <dimension ref="A1:D294"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+    <sheetView tabSelected="1" topLeftCell="A102" workbookViewId="0">
+      <selection activeCell="C116" sqref="C116"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2064,6 +2074,9 @@
       <c r="B45" t="s">
         <v>36</v>
       </c>
+      <c r="C45" s="2" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
@@ -2203,6 +2216,9 @@
       <c r="B60" t="s">
         <v>46</v>
       </c>
+      <c r="C60" s="2" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" s="1">
@@ -2244,6 +2260,9 @@
       <c r="B64" t="s">
         <v>36</v>
       </c>
+      <c r="C64" s="2" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" s="9" t="s">
@@ -2423,38 +2442,39 @@
       <c r="B85" t="s">
         <v>95</v>
       </c>
-      <c r="C85" s="2"/>
+      <c r="C85" s="2" t="s">
+        <v>2</v>
+      </c>
       <c r="D85" s="7" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A87" s="4" t="s">
+    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A86" s="1">
+        <v>5</v>
+      </c>
+      <c r="B86" t="s">
+        <v>234</v>
+      </c>
+      <c r="C86" s="2"/>
+      <c r="D86" s="7"/>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A88" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="B87" s="5" t="s">
+      <c r="B88" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="C87" s="4"/>
-      <c r="D87" s="6"/>
-    </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A88" s="1">
-        <v>1</v>
-      </c>
-      <c r="B88" t="s">
-        <v>98</v>
-      </c>
-      <c r="C88" s="2" t="s">
-        <v>2</v>
-      </c>
+      <c r="C88" s="4"/>
+      <c r="D88" s="6"/>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A89" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B89" t="s">
-        <v>67</v>
+        <v>98</v>
       </c>
       <c r="C89" s="2" t="s">
         <v>2</v>
@@ -2462,10 +2482,10 @@
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A90" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B90" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C90" s="2" t="s">
         <v>2</v>
@@ -2473,10 +2493,10 @@
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A91" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B91" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C91" s="2" t="s">
         <v>2</v>
@@ -2484,10 +2504,10 @@
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A92" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B92" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C92" s="2" t="s">
         <v>2</v>
@@ -2495,10 +2515,10 @@
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A93" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B93" t="s">
-        <v>99</v>
+        <v>70</v>
       </c>
       <c r="C93" s="2" t="s">
         <v>2</v>
@@ -2506,10 +2526,10 @@
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A94" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B94" t="s">
-        <v>71</v>
+        <v>99</v>
       </c>
       <c r="C94" s="2" t="s">
         <v>2</v>
@@ -2517,10 +2537,10 @@
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A95" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B95" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C95" s="2" t="s">
         <v>2</v>
@@ -2528,173 +2548,183 @@
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A96" s="1">
+        <v>8</v>
+      </c>
+      <c r="B96" t="s">
+        <v>72</v>
+      </c>
+      <c r="C96" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A97" s="1">
         <v>9</v>
       </c>
-      <c r="B96" t="s">
+      <c r="B97" t="s">
         <v>100</v>
       </c>
-      <c r="C96" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D96" s="7" t="s">
+      <c r="C97" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D97" s="7" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A97" s="1">
+    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A98" s="1">
         <v>10</v>
       </c>
-      <c r="B97" t="s">
+      <c r="B98" t="s">
         <v>77</v>
       </c>
-      <c r="C97" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A98" s="1">
+      <c r="C98" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A99" s="1">
         <v>11</v>
       </c>
-      <c r="B98" t="s">
+      <c r="B99" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A99" s="1">
+      <c r="C99" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A100" s="1">
         <v>12</v>
       </c>
-      <c r="B99" t="s">
+      <c r="B100" t="s">
         <v>73</v>
       </c>
-      <c r="C99" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A100" s="1">
+      <c r="C100" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A101" s="1">
         <v>13</v>
       </c>
-      <c r="B100" t="s">
+      <c r="B101" t="s">
         <v>74</v>
       </c>
-      <c r="C100" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A101" s="1">
+      <c r="C101" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A102" s="1">
         <v>14</v>
       </c>
-      <c r="B101" t="s">
+      <c r="B102" t="s">
         <v>75</v>
       </c>
-      <c r="C101" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A102" s="1">
+      <c r="C102" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A103" s="1">
         <v>15</v>
       </c>
-      <c r="B102" t="s">
+      <c r="B103" t="s">
         <v>76</v>
       </c>
-      <c r="C102" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B103" t="s">
+      <c r="C103" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B104" t="s">
         <v>105</v>
       </c>
-      <c r="C103" s="2"/>
-    </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B104" t="s">
+      <c r="C104" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B105" t="s">
         <v>106</v>
       </c>
-      <c r="C104" s="2"/>
-    </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A105" s="1">
+      <c r="C105" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A106" s="1">
         <v>16</v>
       </c>
-      <c r="B105" t="s">
+      <c r="B106" t="s">
         <v>77</v>
       </c>
-      <c r="C105" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A106" s="1">
+      <c r="C106" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A107" s="1">
         <v>17</v>
       </c>
-      <c r="B106" t="s">
+      <c r="B107" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A107" s="1">
+      <c r="C107" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A108" s="1">
         <v>18</v>
       </c>
-      <c r="B107" t="s">
+      <c r="B108" t="s">
         <v>79</v>
       </c>
-      <c r="C107" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A108" s="1">
+      <c r="C108" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A109" s="1">
         <v>19</v>
       </c>
-      <c r="B108" t="s">
+      <c r="B109" t="s">
         <v>80</v>
       </c>
-      <c r="C108" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A109" s="1">
+      <c r="C109" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A110" s="1">
         <v>20</v>
       </c>
-      <c r="B109" t="s">
+      <c r="B110" t="s">
         <v>81</v>
       </c>
-      <c r="C109" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A110" s="1">
+      <c r="C110" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A111" s="1">
         <v>21</v>
       </c>
-      <c r="B110" t="s">
+      <c r="B111" t="s">
         <v>82</v>
       </c>
-      <c r="C110" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A111" s="1">
+      <c r="C111" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A112" s="1">
         <v>22</v>
       </c>
-      <c r="B111" t="s">
+      <c r="B112" t="s">
         <v>83</v>
-      </c>
-      <c r="C111" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="112" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A112" s="1">
-        <v>23</v>
-      </c>
-      <c r="B112" t="s">
-        <v>84</v>
       </c>
       <c r="C112" s="2" t="s">
         <v>2</v>
@@ -2702,10 +2732,10 @@
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A113" s="1">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B113" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C113" s="2" t="s">
         <v>2</v>
@@ -2713,10 +2743,10 @@
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A114" s="1">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B114" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C114" s="2" t="s">
         <v>2</v>
@@ -2724,87 +2754,87 @@
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A115" s="1">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B115" t="s">
-        <v>87</v>
+        <v>86</v>
+      </c>
+      <c r="C115" s="2" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A116" s="1">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B116" t="s">
-        <v>88</v>
-      </c>
-      <c r="C116" s="2" t="s">
-        <v>2</v>
+        <v>87</v>
       </c>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A117" s="1">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B117" t="s">
-        <v>101</v>
-      </c>
-      <c r="C117" s="2"/>
+        <v>88</v>
+      </c>
+      <c r="C117" s="2" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A118" s="1">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B118" t="s">
-        <v>77</v>
+        <v>101</v>
       </c>
       <c r="C118" s="2"/>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A119" s="1">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B119" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C119" s="2"/>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A120" s="1">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B120" t="s">
-        <v>103</v>
-      </c>
-      <c r="C120" s="2" t="s">
-        <v>2</v>
-      </c>
+        <v>78</v>
+      </c>
+      <c r="C120" s="2"/>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A121" s="1">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B121" t="s">
-        <v>104</v>
-      </c>
-      <c r="C121" s="2"/>
+        <v>103</v>
+      </c>
+      <c r="C121" s="2" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A122" s="1">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B122" t="s">
-        <v>90</v>
-      </c>
-      <c r="D122" s="8" t="s">
-        <v>89</v>
-      </c>
+        <v>104</v>
+      </c>
+      <c r="C122" s="2"/>
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A123" s="1">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B123" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D123" s="8" t="s">
         <v>89</v>
@@ -2812,72 +2842,75 @@
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A124" s="1">
+        <v>34</v>
+      </c>
+      <c r="B124" t="s">
+        <v>91</v>
+      </c>
+      <c r="D124" s="8" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="125" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A125" s="1">
         <v>35</v>
       </c>
-      <c r="B124" t="s">
+      <c r="B125" t="s">
         <v>97</v>
       </c>
-      <c r="D124" s="7" t="s">
+      <c r="D125" s="7" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A126" s="9" t="s">
+      <c r="A126" s="1">
+        <v>36</v>
+      </c>
+      <c r="B126" t="s">
+        <v>235</v>
+      </c>
+      <c r="C126" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D126" s="7" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="128" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A128" s="9" t="s">
         <v>96</v>
       </c>
-      <c r="B126" s="9"/>
-      <c r="C126" s="9"/>
-      <c r="D126" s="9"/>
-    </row>
-    <row r="127" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A127" s="1">
-        <v>1</v>
-      </c>
-      <c r="B127" t="s">
-        <v>107</v>
-      </c>
-      <c r="C127" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="128" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A128" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="B128" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="C128" s="4"/>
-      <c r="D128" s="6"/>
+      <c r="B128" s="9"/>
+      <c r="C128" s="9"/>
+      <c r="D128" s="9"/>
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A129" s="1">
         <v>1</v>
       </c>
       <c r="B129" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C129" s="2" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A130" s="1">
-        <v>2</v>
-      </c>
-      <c r="B130" t="s">
-        <v>129</v>
-      </c>
-      <c r="C130" s="2" t="s">
-        <v>2</v>
-      </c>
+      <c r="A130" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B130" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="C130" s="4"/>
+      <c r="D130" s="6"/>
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A131" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B131" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="C131" s="2" t="s">
         <v>2</v>
@@ -2885,10 +2918,10 @@
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A132" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B132" t="s">
-        <v>115</v>
+        <v>129</v>
       </c>
       <c r="C132" s="2" t="s">
         <v>2</v>
@@ -2896,10 +2929,10 @@
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A133" s="1">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B133" t="s">
-        <v>75</v>
+        <v>114</v>
       </c>
       <c r="C133" s="2" t="s">
         <v>2</v>
@@ -2907,10 +2940,10 @@
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A134" s="1">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B134" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
       <c r="C134" s="2" t="s">
         <v>2</v>
@@ -2918,10 +2951,10 @@
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A135" s="1">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B135" t="s">
-        <v>111</v>
+        <v>75</v>
       </c>
       <c r="C135" s="2" t="s">
         <v>2</v>
@@ -2929,10 +2962,10 @@
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A136" s="1">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B136" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C136" s="2" t="s">
         <v>2</v>
@@ -2940,10 +2973,10 @@
     </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A137" s="1">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B137" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C137" s="2" t="s">
         <v>2</v>
@@ -2951,10 +2984,10 @@
     </row>
     <row r="138" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A138" s="1">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B138" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="C138" s="2" t="s">
         <v>2</v>
@@ -2962,10 +2995,10 @@
     </row>
     <row r="139" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A139" s="1">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B139" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="C139" s="2" t="s">
         <v>2</v>
@@ -2973,10 +3006,10 @@
     </row>
     <row r="140" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A140" s="1">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B140" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C140" s="2" t="s">
         <v>2</v>
@@ -2984,88 +3017,83 @@
     </row>
     <row r="141" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A141" s="1">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B141" t="s">
-        <v>130</v>
+        <v>117</v>
+      </c>
+      <c r="C141" s="2" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="142" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A142" s="1">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B142" t="s">
-        <v>131</v>
+        <v>118</v>
+      </c>
+      <c r="C142" s="2" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="143" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A143" s="1">
+        <v>13</v>
+      </c>
+      <c r="B143" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="144" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A144" s="1">
+        <v>14</v>
+      </c>
+      <c r="B144" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="145" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A145" s="1">
         <v>15</v>
       </c>
-      <c r="B143" t="s">
+      <c r="B145" t="s">
         <v>132</v>
       </c>
-      <c r="C143" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="144" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B144" t="s">
+      <c r="C145" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="146" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B146" t="s">
         <v>128</v>
       </c>
-      <c r="D144" s="7" t="s">
+      <c r="D146" s="7" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="146" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A146" s="4" t="s">
+    <row r="147" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B147" t="s">
+        <v>233</v>
+      </c>
+      <c r="D147" s="7"/>
+    </row>
+    <row r="149" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A149" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="B146" s="5" t="s">
+      <c r="B149" s="5" t="s">
         <v>119</v>
       </c>
-      <c r="C146" s="4"/>
-      <c r="D146" s="6"/>
-    </row>
-    <row r="147" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A147" s="1">
-        <v>1</v>
-      </c>
-      <c r="B147" t="s">
-        <v>120</v>
-      </c>
-      <c r="C147" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="148" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A148" s="1">
-        <v>2</v>
-      </c>
-      <c r="B148" t="s">
-        <v>121</v>
-      </c>
-      <c r="C148" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="149" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A149" s="1">
-        <v>3</v>
-      </c>
-      <c r="B149" t="s">
-        <v>122</v>
-      </c>
-      <c r="C149" s="2" t="s">
-        <v>2</v>
-      </c>
+      <c r="C149" s="4"/>
+      <c r="D149" s="6"/>
     </row>
     <row r="150" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A150" s="1">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B150" t="s">
-        <v>133</v>
+        <v>120</v>
       </c>
       <c r="C150" s="2" t="s">
         <v>2</v>
@@ -3073,62 +3101,62 @@
     </row>
     <row r="151" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A151" s="1">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B151" t="s">
-        <v>134</v>
-      </c>
-      <c r="C151" s="2"/>
+        <v>121</v>
+      </c>
+      <c r="C151" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="152" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A152" s="1">
+        <v>3</v>
+      </c>
+      <c r="B152" t="s">
+        <v>122</v>
+      </c>
+      <c r="C152" s="2" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="153" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A153" s="4" t="s">
-        <v>123</v>
-      </c>
-      <c r="B153" s="5" t="s">
-        <v>124</v>
-      </c>
-      <c r="C153" s="4"/>
-      <c r="D153" s="6"/>
+      <c r="A153" s="1">
+        <v>4</v>
+      </c>
+      <c r="B153" t="s">
+        <v>133</v>
+      </c>
+      <c r="C153" s="2" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="154" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A154" s="1">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="B154" t="s">
-        <v>125</v>
-      </c>
-      <c r="C154" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="155" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A155" s="1">
-        <v>2</v>
-      </c>
-      <c r="B155" t="s">
-        <v>14</v>
-      </c>
-      <c r="C155" s="2" t="s">
-        <v>2</v>
-      </c>
+        <v>134</v>
+      </c>
+      <c r="C154" s="2"/>
     </row>
     <row r="156" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A156" s="1">
-        <v>3</v>
-      </c>
-      <c r="B156" t="s">
-        <v>137</v>
-      </c>
-      <c r="C156" s="2" t="s">
-        <v>2</v>
-      </c>
+      <c r="A156" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="B156" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="C156" s="4"/>
+      <c r="D156" s="6"/>
     </row>
     <row r="157" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A157" s="1">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B157" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C157" s="2" t="s">
         <v>2</v>
@@ -3136,18 +3164,21 @@
     </row>
     <row r="158" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A158" s="1">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B158" t="s">
-        <v>127</v>
+        <v>14</v>
+      </c>
+      <c r="C158" s="2" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="159" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A159" s="1">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B159" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="C159" s="2" t="s">
         <v>2</v>
@@ -3155,10 +3186,10 @@
     </row>
     <row r="160" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A160" s="1">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B160" t="s">
-        <v>136</v>
+        <v>126</v>
       </c>
       <c r="C160" s="2" t="s">
         <v>2</v>
@@ -3166,83 +3197,80 @@
     </row>
     <row r="161" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A161" s="1">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B161" t="s">
-        <v>138</v>
-      </c>
-      <c r="C161" s="2" t="s">
-        <v>2</v>
+        <v>127</v>
       </c>
     </row>
     <row r="162" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A162" s="1">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B162" t="s">
-        <v>139</v>
+        <v>135</v>
+      </c>
+      <c r="C162" s="2" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="163" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A163" s="1">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B163" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="C163" s="2" t="s">
         <v>2</v>
       </c>
     </row>
+    <row r="164" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A164" s="1">
+        <v>8</v>
+      </c>
+      <c r="B164" t="s">
+        <v>138</v>
+      </c>
+      <c r="C164" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
     <row r="165" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A165" s="4" t="s">
-        <v>141</v>
-      </c>
-      <c r="B165" s="5" t="s">
-        <v>142</v>
-      </c>
-      <c r="C165" s="4"/>
-      <c r="D165" s="6"/>
+      <c r="A165" s="1">
+        <v>9</v>
+      </c>
+      <c r="B165" t="s">
+        <v>139</v>
+      </c>
     </row>
     <row r="166" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A166" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="B166" t="s">
-        <v>125</v>
+        <v>140</v>
       </c>
       <c r="C166" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="167" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A167" s="1">
-        <v>2</v>
-      </c>
-      <c r="B167" t="s">
-        <v>143</v>
-      </c>
-      <c r="C167" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
     <row r="168" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A168" s="1">
-        <v>3</v>
-      </c>
-      <c r="B168" t="s">
-        <v>174</v>
-      </c>
-      <c r="C168" s="2" t="s">
-        <v>2</v>
-      </c>
+      <c r="A168" s="4" t="s">
+        <v>141</v>
+      </c>
+      <c r="B168" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="C168" s="4"/>
+      <c r="D168" s="6"/>
     </row>
     <row r="169" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A169" s="1">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B169" t="s">
-        <v>144</v>
+        <v>125</v>
       </c>
       <c r="C169" s="2" t="s">
         <v>2</v>
@@ -3250,10 +3278,10 @@
     </row>
     <row r="170" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A170" s="1">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B170" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C170" s="2" t="s">
         <v>2</v>
@@ -3261,10 +3289,10 @@
     </row>
     <row r="171" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A171" s="1">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B171" t="s">
-        <v>146</v>
+        <v>174</v>
       </c>
       <c r="C171" s="2" t="s">
         <v>2</v>
@@ -3272,10 +3300,10 @@
     </row>
     <row r="172" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A172" s="1">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B172" t="s">
-        <v>175</v>
+        <v>144</v>
       </c>
       <c r="C172" s="2" t="s">
         <v>2</v>
@@ -3283,10 +3311,10 @@
     </row>
     <row r="173" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A173" s="1">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B173" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C173" s="2" t="s">
         <v>2</v>
@@ -3294,10 +3322,10 @@
     </row>
     <row r="174" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A174" s="1">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B174" t="s">
-        <v>14</v>
+        <v>146</v>
       </c>
       <c r="C174" s="2" t="s">
         <v>2</v>
@@ -3305,74 +3333,74 @@
     </row>
     <row r="175" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A175" s="1">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B175" t="s">
-        <v>77</v>
-      </c>
-      <c r="C175" s="2"/>
+        <v>175</v>
+      </c>
+      <c r="C175" s="2" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="176" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A176" s="1">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B176" t="s">
-        <v>78</v>
-      </c>
-      <c r="C176" s="2"/>
+        <v>147</v>
+      </c>
+      <c r="C176" s="2" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="177" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C177" s="2"/>
+      <c r="A177" s="1">
+        <v>9</v>
+      </c>
+      <c r="B177" t="s">
+        <v>14</v>
+      </c>
+      <c r="C177" s="2" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="178" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A178" s="4" t="s">
-        <v>148</v>
-      </c>
-      <c r="B178" s="5" t="s">
-        <v>158</v>
-      </c>
-      <c r="C178" s="4"/>
-      <c r="D178" s="6"/>
+      <c r="A178" s="1">
+        <v>10</v>
+      </c>
+      <c r="B178" t="s">
+        <v>77</v>
+      </c>
+      <c r="C178" s="2"/>
     </row>
     <row r="179" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A179" s="1">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="B179" t="s">
-        <v>125</v>
-      </c>
-      <c r="C179" s="2" t="s">
-        <v>2</v>
-      </c>
+        <v>78</v>
+      </c>
+      <c r="C179" s="2"/>
     </row>
     <row r="180" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A180" s="1">
-        <v>2</v>
-      </c>
-      <c r="B180" t="s">
-        <v>161</v>
-      </c>
-      <c r="C180" s="2" t="s">
-        <v>2</v>
-      </c>
+      <c r="C180" s="2"/>
     </row>
     <row r="181" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A181" s="1">
-        <v>3</v>
-      </c>
-      <c r="B181" t="s">
-        <v>162</v>
-      </c>
-      <c r="C181" s="2" t="s">
-        <v>2</v>
-      </c>
+      <c r="A181" s="4" t="s">
+        <v>148</v>
+      </c>
+      <c r="B181" s="5" t="s">
+        <v>158</v>
+      </c>
+      <c r="C181" s="4"/>
+      <c r="D181" s="6"/>
     </row>
     <row r="182" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A182" s="1">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B182" t="s">
-        <v>164</v>
+        <v>125</v>
       </c>
       <c r="C182" s="2" t="s">
         <v>2</v>
@@ -3380,10 +3408,10 @@
     </row>
     <row r="183" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A183" s="1">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B183" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="C183" s="2" t="s">
         <v>2</v>
@@ -3391,10 +3419,10 @@
     </row>
     <row r="184" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A184" s="1">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B184" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C184" s="2" t="s">
         <v>2</v>
@@ -3402,10 +3430,10 @@
     </row>
     <row r="185" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A185" s="1">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B185" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="C185" s="2" t="s">
         <v>2</v>
@@ -3413,10 +3441,10 @@
     </row>
     <row r="186" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A186" s="1">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B186" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="C186" s="2" t="s">
         <v>2</v>
@@ -3424,10 +3452,10 @@
     </row>
     <row r="187" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A187" s="1">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B187" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="C187" s="2" t="s">
         <v>2</v>
@@ -3435,10 +3463,10 @@
     </row>
     <row r="188" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A188" s="1">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B188" t="s">
-        <v>167</v>
+        <v>170</v>
       </c>
       <c r="C188" s="2" t="s">
         <v>2</v>
@@ -3446,10 +3474,10 @@
     </row>
     <row r="189" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A189" s="1">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B189" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="C189" s="2" t="s">
         <v>2</v>
@@ -3457,10 +3485,10 @@
     </row>
     <row r="190" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A190" s="1">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B190" t="s">
-        <v>14</v>
+        <v>165</v>
       </c>
       <c r="C190" s="2" t="s">
         <v>2</v>
@@ -3468,71 +3496,71 @@
     </row>
     <row r="191" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A191" s="1">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B191" t="s">
-        <v>77</v>
-      </c>
-      <c r="C191" s="2"/>
+        <v>167</v>
+      </c>
+      <c r="C191" s="2" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="192" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A192" s="1">
+        <v>11</v>
+      </c>
+      <c r="B192" t="s">
+        <v>168</v>
+      </c>
+      <c r="C192" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="193" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A193" s="1">
+        <v>12</v>
+      </c>
+      <c r="B193" t="s">
         <v>14</v>
       </c>
-      <c r="B192" t="s">
-        <v>78</v>
-      </c>
-      <c r="C192" s="2"/>
+      <c r="C193" s="2" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="194" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A194" s="4" t="s">
-        <v>157</v>
-      </c>
-      <c r="B194" s="5" t="s">
-        <v>149</v>
-      </c>
-      <c r="C194" s="4"/>
-      <c r="D194" s="6"/>
+      <c r="A194" s="1">
+        <v>13</v>
+      </c>
+      <c r="B194" t="s">
+        <v>77</v>
+      </c>
+      <c r="C194" s="2"/>
     </row>
     <row r="195" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A195" s="1">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="B195" t="s">
-        <v>150</v>
-      </c>
-      <c r="C195" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="196" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A196" s="1">
-        <v>2</v>
-      </c>
-      <c r="B196" t="s">
-        <v>151</v>
-      </c>
-      <c r="C196" s="2" t="s">
-        <v>2</v>
-      </c>
+        <v>78</v>
+      </c>
+      <c r="C195" s="2"/>
     </row>
     <row r="197" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A197" s="1">
-        <v>3</v>
-      </c>
-      <c r="B197" t="s">
-        <v>152</v>
-      </c>
-      <c r="C197" s="2" t="s">
-        <v>2</v>
-      </c>
+      <c r="A197" s="4" t="s">
+        <v>157</v>
+      </c>
+      <c r="B197" s="5" t="s">
+        <v>149</v>
+      </c>
+      <c r="C197" s="4"/>
+      <c r="D197" s="6"/>
     </row>
     <row r="198" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A198" s="1">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B198" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="C198" s="2" t="s">
         <v>2</v>
@@ -3540,10 +3568,10 @@
     </row>
     <row r="199" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A199" s="1">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B199" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="C199" s="2" t="s">
         <v>2</v>
@@ -3551,10 +3579,10 @@
     </row>
     <row r="200" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A200" s="1">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B200" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="C200" s="2" t="s">
         <v>2</v>
@@ -3562,10 +3590,10 @@
     </row>
     <row r="201" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A201" s="1">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B201" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="C201" s="2" t="s">
         <v>2</v>
@@ -3573,10 +3601,10 @@
     </row>
     <row r="202" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A202" s="1">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B202" t="s">
-        <v>14</v>
+        <v>154</v>
       </c>
       <c r="C202" s="2" t="s">
         <v>2</v>
@@ -3584,69 +3612,69 @@
     </row>
     <row r="203" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A203" s="1">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B203" t="s">
-        <v>77</v>
+        <v>155</v>
+      </c>
+      <c r="C203" s="2" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="204" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A204" s="1">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B204" t="s">
-        <v>78</v>
+        <v>156</v>
+      </c>
+      <c r="C204" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="205" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A205" s="1">
+        <v>8</v>
+      </c>
+      <c r="B205" t="s">
+        <v>14</v>
+      </c>
+      <c r="C205" s="2" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="206" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A206" s="4" t="s">
-        <v>159</v>
-      </c>
-      <c r="B206" s="5" t="s">
-        <v>160</v>
-      </c>
-      <c r="C206" s="4"/>
-      <c r="D206" s="6"/>
+      <c r="A206" s="1">
+        <v>9</v>
+      </c>
+      <c r="B206" t="s">
+        <v>77</v>
+      </c>
     </row>
     <row r="207" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A207" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="B207" t="s">
-        <v>171</v>
-      </c>
-      <c r="C207" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="208" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A208" s="1">
-        <v>2</v>
-      </c>
-      <c r="B208" t="s">
-        <v>172</v>
-      </c>
-      <c r="C208" s="2" t="s">
-        <v>2</v>
+        <v>78</v>
       </c>
     </row>
     <row r="209" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A209" s="1">
-        <v>3</v>
-      </c>
-      <c r="B209" t="s">
-        <v>173</v>
-      </c>
-      <c r="C209" s="2" t="s">
-        <v>2</v>
-      </c>
+      <c r="A209" s="4" t="s">
+        <v>159</v>
+      </c>
+      <c r="B209" s="5" t="s">
+        <v>160</v>
+      </c>
+      <c r="C209" s="4"/>
+      <c r="D209" s="6"/>
     </row>
     <row r="210" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A210" s="1">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B210" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="C210" s="2" t="s">
         <v>2</v>
@@ -3654,10 +3682,10 @@
     </row>
     <row r="211" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A211" s="1">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B211" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
       <c r="C211" s="2" t="s">
         <v>2</v>
@@ -3665,10 +3693,10 @@
     </row>
     <row r="212" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A212" s="1">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B212" t="s">
-        <v>14</v>
+        <v>173</v>
       </c>
       <c r="C212" s="2" t="s">
         <v>2</v>
@@ -3676,72 +3704,72 @@
     </row>
     <row r="213" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A213" s="1">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B213" t="s">
-        <v>77</v>
+        <v>176</v>
+      </c>
+      <c r="C213" s="2" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="214" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A214" s="1">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B214" t="s">
-        <v>78</v>
+        <v>177</v>
+      </c>
+      <c r="C214" s="2" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="215" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C215" s="2"/>
+      <c r="A215" s="1">
+        <v>6</v>
+      </c>
+      <c r="B215" t="s">
+        <v>14</v>
+      </c>
+      <c r="C215" s="2" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="216" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A216" s="4" t="s">
-        <v>178</v>
-      </c>
-      <c r="B216" s="5" t="s">
-        <v>179</v>
-      </c>
-      <c r="C216" s="4"/>
-      <c r="D216" s="6"/>
+      <c r="A216" s="1">
+        <v>7</v>
+      </c>
+      <c r="B216" t="s">
+        <v>77</v>
+      </c>
     </row>
     <row r="217" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A217" s="1">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="B217" t="s">
-        <v>125</v>
-      </c>
-      <c r="C217" s="2" t="s">
-        <v>2</v>
+        <v>78</v>
       </c>
     </row>
     <row r="218" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A218" s="1">
-        <v>2</v>
-      </c>
-      <c r="B218" t="s">
-        <v>180</v>
-      </c>
-      <c r="C218" s="2" t="s">
-        <v>2</v>
-      </c>
+      <c r="C218" s="2"/>
     </row>
     <row r="219" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A219" s="1">
-        <v>3</v>
-      </c>
-      <c r="B219" t="s">
-        <v>181</v>
-      </c>
-      <c r="C219" s="2" t="s">
-        <v>2</v>
-      </c>
+      <c r="A219" s="4" t="s">
+        <v>178</v>
+      </c>
+      <c r="B219" s="5" t="s">
+        <v>179</v>
+      </c>
+      <c r="C219" s="4"/>
+      <c r="D219" s="6"/>
     </row>
     <row r="220" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A220" s="1">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B220" t="s">
-        <v>182</v>
+        <v>125</v>
       </c>
       <c r="C220" s="2" t="s">
         <v>2</v>
@@ -3749,10 +3777,10 @@
     </row>
     <row r="221" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A221" s="1">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B221" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="C221" s="2" t="s">
         <v>2</v>
@@ -3760,10 +3788,10 @@
     </row>
     <row r="222" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A222" s="1">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B222" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="C222" s="2" t="s">
         <v>2</v>
@@ -3771,10 +3799,10 @@
     </row>
     <row r="223" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A223" s="1">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B223" t="s">
-        <v>14</v>
+        <v>182</v>
       </c>
       <c r="C223" s="2" t="s">
         <v>2</v>
@@ -3782,69 +3810,69 @@
     </row>
     <row r="224" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A224" s="1">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B224" t="s">
-        <v>77</v>
+        <v>183</v>
+      </c>
+      <c r="C224" s="2" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="225" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A225" s="1">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B225" t="s">
-        <v>78</v>
+        <v>184</v>
+      </c>
+      <c r="C225" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="226" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A226" s="1">
+        <v>7</v>
+      </c>
+      <c r="B226" t="s">
+        <v>14</v>
+      </c>
+      <c r="C226" s="2" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="227" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A227" s="4" t="s">
-        <v>185</v>
-      </c>
-      <c r="B227" s="5" t="s">
-        <v>187</v>
-      </c>
-      <c r="C227" s="4"/>
-      <c r="D227" s="6"/>
+      <c r="A227" s="1">
+        <v>8</v>
+      </c>
+      <c r="B227" t="s">
+        <v>77</v>
+      </c>
     </row>
     <row r="228" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A228" s="1">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="B228" t="s">
-        <v>186</v>
-      </c>
-      <c r="C228" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="229" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A229" s="1">
-        <v>2</v>
-      </c>
-      <c r="B229" t="s">
-        <v>188</v>
-      </c>
-      <c r="C229" s="2" t="s">
-        <v>2</v>
+        <v>78</v>
       </c>
     </row>
     <row r="230" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A230" s="1">
-        <v>3</v>
-      </c>
-      <c r="B230" t="s">
-        <v>189</v>
-      </c>
-      <c r="C230" s="2" t="s">
-        <v>2</v>
-      </c>
+      <c r="A230" s="4" t="s">
+        <v>185</v>
+      </c>
+      <c r="B230" s="5" t="s">
+        <v>187</v>
+      </c>
+      <c r="C230" s="4"/>
+      <c r="D230" s="6"/>
     </row>
     <row r="231" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A231" s="1">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B231" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="C231" s="2" t="s">
         <v>2</v>
@@ -3852,10 +3880,10 @@
     </row>
     <row r="232" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A232" s="1">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B232" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="C232" s="2" t="s">
         <v>2</v>
@@ -3863,10 +3891,10 @@
     </row>
     <row r="233" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A233" s="1">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B233" t="s">
-        <v>14</v>
+        <v>189</v>
       </c>
       <c r="C233" s="2" t="s">
         <v>2</v>
@@ -3874,238 +3902,238 @@
     </row>
     <row r="234" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A234" s="1">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B234" t="s">
-        <v>77</v>
+        <v>190</v>
+      </c>
+      <c r="C234" s="2" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="235" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A235" s="1">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B235" t="s">
-        <v>78</v>
+        <v>191</v>
+      </c>
+      <c r="C235" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="236" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A236" s="1">
+        <v>6</v>
+      </c>
+      <c r="B236" t="s">
+        <v>14</v>
+      </c>
+      <c r="C236" s="2" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="237" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A237" s="4" t="s">
-        <v>192</v>
-      </c>
-      <c r="B237" s="5" t="s">
-        <v>193</v>
-      </c>
-      <c r="C237" s="4"/>
-      <c r="D237" s="6"/>
+      <c r="A237" s="1">
+        <v>7</v>
+      </c>
+      <c r="B237" t="s">
+        <v>77</v>
+      </c>
     </row>
     <row r="238" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A238" s="1">
+        <v>8</v>
+      </c>
+      <c r="B238" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="240" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A240" s="4" t="s">
+        <v>192</v>
+      </c>
+      <c r="B240" s="5" t="s">
+        <v>193</v>
+      </c>
+      <c r="C240" s="4"/>
+      <c r="D240" s="6"/>
+    </row>
+    <row r="241" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A241" s="1">
         <v>1</v>
       </c>
-      <c r="B238" t="s">
+      <c r="B241" t="s">
         <v>125</v>
       </c>
-      <c r="C238" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="239" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A239" s="1">
-        <v>2</v>
-      </c>
-      <c r="B239" t="s">
+      <c r="C241" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="242" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A242" s="1">
+        <v>2</v>
+      </c>
+      <c r="B242" t="s">
         <v>194</v>
       </c>
-      <c r="C239" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="240" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A240" s="1">
+      <c r="C242" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="243" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A243" s="1">
         <v>3</v>
       </c>
-      <c r="B240" t="s">
+      <c r="B243" t="s">
         <v>195</v>
       </c>
-      <c r="C240" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="241" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A241" s="1">
+      <c r="C243" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="244" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A244" s="1">
         <v>4</v>
       </c>
-      <c r="B241" t="s">
+      <c r="B244" t="s">
         <v>199</v>
       </c>
-      <c r="C241" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="242" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A242" s="1">
+      <c r="C244" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="245" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A245" s="1">
         <v>5</v>
       </c>
-      <c r="B242" t="s">
+      <c r="B245" t="s">
         <v>196</v>
       </c>
-      <c r="C242" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="243" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A243" s="1">
+      <c r="C245" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="246" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A246" s="1">
         <v>6</v>
       </c>
-      <c r="B243" t="s">
+      <c r="B246" t="s">
         <v>197</v>
       </c>
-      <c r="C243" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="244" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A244" s="1">
+      <c r="C246" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="247" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A247" s="1">
         <v>7</v>
       </c>
-      <c r="B244" t="s">
+      <c r="B247" t="s">
         <v>198</v>
       </c>
-      <c r="C244" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="245" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A245" s="1">
+      <c r="C247" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="248" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A248" s="1">
         <v>8</v>
       </c>
-      <c r="B245" t="s">
+      <c r="B248" t="s">
         <v>200</v>
       </c>
-      <c r="C245" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="246" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A246" s="1">
+      <c r="C248" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="249" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A249" s="1">
         <v>9</v>
       </c>
-      <c r="B246" t="s">
+      <c r="B249" t="s">
         <v>201</v>
       </c>
-      <c r="C246" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="247" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A247" s="1">
+      <c r="C249" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="250" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A250" s="1">
         <v>10</v>
       </c>
-      <c r="B247" t="s">
+      <c r="B250" t="s">
         <v>202</v>
       </c>
-      <c r="C247" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="248" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A248" s="1">
+      <c r="C250" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="251" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A251" s="1">
         <v>11</v>
       </c>
-      <c r="B248" t="s">
+      <c r="B251" t="s">
         <v>203</v>
       </c>
-      <c r="C248" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="249" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A249" s="1">
+      <c r="C251" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="252" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A252" s="1">
         <v>12</v>
       </c>
-      <c r="B249" t="s">
+      <c r="B252" t="s">
         <v>204</v>
       </c>
-      <c r="C249" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="250" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A250" s="1">
+      <c r="C252" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="253" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A253" s="1">
         <v>13</v>
       </c>
-      <c r="B250" t="s">
+      <c r="B253" t="s">
         <v>14</v>
       </c>
-      <c r="C250" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="251" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A251" s="1">
+      <c r="C253" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="254" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A254" s="1">
         <v>14</v>
       </c>
-      <c r="B251" t="s">
+      <c r="B254" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="252" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A252" s="1">
+    <row r="255" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A255" s="1">
         <v>15</v>
       </c>
-      <c r="B252" t="s">
+      <c r="B255" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="254" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A254" s="4" t="s">
+    <row r="257" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A257" s="4" t="s">
         <v>205</v>
       </c>
-      <c r="B254" s="5" t="s">
+      <c r="B257" s="5" t="s">
         <v>206</v>
       </c>
-      <c r="C254" s="4"/>
-      <c r="D254" s="6"/>
-    </row>
-    <row r="255" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A255" s="1">
-        <v>1</v>
-      </c>
-      <c r="B255" t="s">
-        <v>125</v>
-      </c>
-      <c r="C255" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="256" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A256" s="1">
-        <v>2</v>
-      </c>
-      <c r="B256" t="s">
-        <v>207</v>
-      </c>
-      <c r="C256" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="257" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A257" s="1">
-        <v>3</v>
-      </c>
-      <c r="B257" t="s">
-        <v>208</v>
-      </c>
-      <c r="C257" s="2" t="s">
-        <v>2</v>
-      </c>
+      <c r="C257" s="4"/>
+      <c r="D257" s="6"/>
     </row>
     <row r="258" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A258" s="1">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B258" t="s">
-        <v>209</v>
+        <v>125</v>
       </c>
       <c r="C258" s="2" t="s">
         <v>2</v>
@@ -4113,10 +4141,10 @@
     </row>
     <row r="259" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A259" s="1">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B259" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="C259" s="2" t="s">
         <v>2</v>
@@ -4124,10 +4152,10 @@
     </row>
     <row r="260" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A260" s="1">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B260" t="s">
-        <v>14</v>
+        <v>208</v>
       </c>
       <c r="C260" s="2" t="s">
         <v>2</v>
@@ -4135,69 +4163,69 @@
     </row>
     <row r="261" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A261" s="1">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B261" t="s">
-        <v>77</v>
+        <v>209</v>
+      </c>
+      <c r="C261" s="2" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="262" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A262" s="1">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B262" t="s">
-        <v>78</v>
+        <v>210</v>
+      </c>
+      <c r="C262" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="263" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A263" s="1">
+        <v>6</v>
+      </c>
+      <c r="B263" t="s">
+        <v>14</v>
+      </c>
+      <c r="C263" s="2" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="264" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A264" s="4" t="s">
-        <v>211</v>
-      </c>
-      <c r="B264" s="5" t="s">
-        <v>212</v>
-      </c>
-      <c r="C264" s="4"/>
-      <c r="D264" s="6"/>
+      <c r="A264" s="1">
+        <v>7</v>
+      </c>
+      <c r="B264" t="s">
+        <v>77</v>
+      </c>
     </row>
     <row r="265" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A265" s="1">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="B265" t="s">
-        <v>213</v>
-      </c>
-      <c r="C265" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="266" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A266" s="1">
-        <v>2</v>
-      </c>
-      <c r="B266" t="s">
-        <v>214</v>
-      </c>
-      <c r="C266" s="2" t="s">
-        <v>2</v>
+        <v>78</v>
       </c>
     </row>
     <row r="267" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A267" s="1">
-        <v>3</v>
-      </c>
-      <c r="B267" t="s">
-        <v>215</v>
-      </c>
-      <c r="C267" s="2" t="s">
-        <v>2</v>
-      </c>
+      <c r="A267" s="4" t="s">
+        <v>211</v>
+      </c>
+      <c r="B267" s="5" t="s">
+        <v>212</v>
+      </c>
+      <c r="C267" s="4"/>
+      <c r="D267" s="6"/>
     </row>
     <row r="268" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A268" s="1">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B268" t="s">
-        <v>14</v>
+        <v>213</v>
       </c>
       <c r="C268" s="2" t="s">
         <v>2</v>
@@ -4205,225 +4233,258 @@
     </row>
     <row r="269" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A269" s="1">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B269" t="s">
-        <v>77</v>
-      </c>
-      <c r="C269" s="2"/>
+        <v>214</v>
+      </c>
+      <c r="C269" s="2" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="270" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A270" s="1">
+        <v>3</v>
+      </c>
+      <c r="B270" t="s">
+        <v>215</v>
+      </c>
+      <c r="C270" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="271" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A271" s="1">
+        <v>4</v>
+      </c>
+      <c r="B271" t="s">
+        <v>14</v>
+      </c>
+      <c r="C271" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="272" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A272" s="1">
+        <v>5</v>
+      </c>
+      <c r="B272" t="s">
+        <v>77</v>
+      </c>
+      <c r="C272" s="2"/>
+    </row>
+    <row r="273" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A273" s="1">
         <v>6</v>
       </c>
-      <c r="B270" t="s">
+      <c r="B273" t="s">
         <v>78</v>
       </c>
-      <c r="C270" s="2"/>
-    </row>
-    <row r="272" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A272" s="4" t="s">
+      <c r="C273" s="2"/>
+    </row>
+    <row r="275" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A275" s="4" t="s">
         <v>216</v>
       </c>
-      <c r="B272" s="5" t="s">
+      <c r="B275" s="5" t="s">
         <v>217</v>
       </c>
-      <c r="C272" s="4"/>
-      <c r="D272" s="6"/>
-    </row>
-    <row r="273" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A273" s="1">
+      <c r="C275" s="4"/>
+      <c r="D275" s="6"/>
+    </row>
+    <row r="276" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A276" s="1">
         <v>1</v>
       </c>
-      <c r="B273" t="s">
+      <c r="B276" t="s">
         <v>125</v>
       </c>
-      <c r="C273" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="274" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A274" s="1">
-        <v>2</v>
-      </c>
-      <c r="B274" t="s">
+      <c r="C276" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="277" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A277" s="1">
+        <v>2</v>
+      </c>
+      <c r="B277" t="s">
         <v>218</v>
       </c>
-      <c r="C274" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="275" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A275" s="1">
+      <c r="C277" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="278" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A278" s="1">
         <v>3</v>
       </c>
-      <c r="B275" t="s">
+      <c r="B278" t="s">
         <v>219</v>
       </c>
-      <c r="C275" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="276" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A276" s="1">
+      <c r="C278" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="279" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A279" s="1">
         <v>4</v>
       </c>
-      <c r="B276" t="s">
+      <c r="B279" t="s">
         <v>220</v>
       </c>
-      <c r="C276" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="277" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A277" s="1">
+      <c r="C279" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="280" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A280" s="1">
         <v>5</v>
       </c>
-      <c r="B277" t="s">
+      <c r="B280" t="s">
         <v>222</v>
       </c>
-      <c r="C277" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="278" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A278" s="1">
+      <c r="C280" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="281" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A281" s="1">
         <v>6</v>
       </c>
-      <c r="B278" t="s">
+      <c r="B281" t="s">
         <v>221</v>
       </c>
-      <c r="C278" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="279" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A279" s="1">
+      <c r="C281" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="282" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A282" s="1">
         <v>7</v>
       </c>
-      <c r="B279" t="s">
+      <c r="B282" t="s">
         <v>223</v>
       </c>
-      <c r="C279" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="280" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A280" s="1">
+      <c r="C282" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="283" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A283" s="1">
         <v>8</v>
       </c>
-      <c r="B280" t="s">
+      <c r="B283" t="s">
         <v>224</v>
       </c>
-      <c r="C280" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="281" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A281" s="1">
+      <c r="C283" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="284" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A284" s="1">
         <v>9</v>
       </c>
-      <c r="B281" t="s">
+      <c r="B284" t="s">
         <v>225</v>
       </c>
-      <c r="C281" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="282" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A282" s="1">
+      <c r="C284" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="285" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A285" s="1">
         <v>10</v>
       </c>
-      <c r="B282" t="s">
+      <c r="B285" t="s">
         <v>226</v>
       </c>
-      <c r="C282" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="283" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A283" s="1">
+      <c r="C285" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="286" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A286" s="1">
         <v>11</v>
       </c>
-      <c r="B283" t="s">
+      <c r="B286" t="s">
         <v>227</v>
       </c>
-      <c r="C283" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="284" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A284" s="1">
+      <c r="C286" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="287" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A287" s="1">
         <v>12</v>
       </c>
-      <c r="B284" t="s">
+      <c r="B287" t="s">
         <v>228</v>
       </c>
-      <c r="C284" s="2"/>
-    </row>
-    <row r="285" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A285" s="1">
+      <c r="C287" s="2"/>
+    </row>
+    <row r="288" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A288" s="1">
         <v>13</v>
       </c>
-      <c r="B285" t="s">
+      <c r="B288" t="s">
         <v>229</v>
       </c>
-      <c r="C285" s="2"/>
-    </row>
-    <row r="286" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A286" s="1">
+      <c r="C288" s="2"/>
+    </row>
+    <row r="289" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A289" s="1">
         <v>14</v>
       </c>
-      <c r="B286" t="s">
+      <c r="B289" t="s">
         <v>230</v>
       </c>
-      <c r="C286" s="2"/>
-    </row>
-    <row r="287" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A287" s="1">
+      <c r="C289" s="2"/>
+    </row>
+    <row r="290" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A290" s="1">
         <v>15</v>
       </c>
-      <c r="B287" t="s">
+      <c r="B290" t="s">
         <v>231</v>
       </c>
-      <c r="C287" s="2"/>
-    </row>
-    <row r="288" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A288" s="1">
+      <c r="C290" s="2"/>
+    </row>
+    <row r="291" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A291" s="1">
         <v>16</v>
       </c>
-      <c r="B288" t="s">
+      <c r="B291" t="s">
         <v>232</v>
       </c>
-      <c r="C288" s="2"/>
-    </row>
-    <row r="289" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A289" s="1">
+      <c r="C291" s="2"/>
+    </row>
+    <row r="292" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A292" s="1">
         <v>17</v>
       </c>
-      <c r="B289" t="s">
+      <c r="B292" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="290" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A290" s="1">
+    <row r="293" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A293" s="1">
         <v>18</v>
       </c>
-      <c r="B290" t="s">
+      <c r="B293" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="291" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A291" s="1">
+    <row r="294" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A294" s="1">
         <v>19</v>
       </c>
-      <c r="B291" t="s">
+      <c r="B294" t="s">
         <v>78</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="8">
-    <mergeCell ref="A126:D126"/>
+    <mergeCell ref="A128:D128"/>
     <mergeCell ref="A71:D71"/>
     <mergeCell ref="A1:D1"/>
     <mergeCell ref="A7:D7"/>

</xml_diff>

<commit_message>
Fix Follow up & Aid Recommendation
</commit_message>
<xml_diff>
--- a/Tasks.xlsx
+++ b/Tasks.xlsx
@@ -15,12 +15,11 @@
     <definedName name="LOCAL_MYSQL_DATE_FORMAT" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
   </definedNames>
   <calcPr calcId="144525"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="495" uniqueCount="236">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="519" uniqueCount="247">
   <si>
     <t>Login</t>
   </si>
@@ -1146,6 +1145,39 @@
   </si>
   <si>
     <t>عند فتح الصفحة لا تظهر ملفات العضو المدخلة من قبل</t>
+  </si>
+  <si>
+    <t>Family Member</t>
+  </si>
+  <si>
+    <t>Design the page</t>
+  </si>
+  <si>
+    <t>Get Elder Family Members</t>
+  </si>
+  <si>
+    <t>Get Constants</t>
+  </si>
+  <si>
+    <t>Insert Family Member</t>
+  </si>
+  <si>
+    <t>Fix DB (Remove Survey_Id)</t>
+  </si>
+  <si>
+    <t>Update Family Member</t>
+  </si>
+  <si>
+    <t>Delete Family Member</t>
+  </si>
+  <si>
+    <t>If Member in Elder Family…hdn action -&gt; Update</t>
+  </si>
+  <si>
+    <t>If Member is not in Elder Family hdn action -&gt;Insert</t>
+  </si>
+  <si>
+    <t>If found fill the feelds</t>
   </si>
 </sst>
 </file>
@@ -1625,10 +1657,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D294"/>
+  <dimension ref="A1:D309"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A102" workbookViewId="0">
-      <selection activeCell="C116" sqref="C116"/>
+    <sheetView tabSelected="1" topLeftCell="A130" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A140" sqref="A140"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2876,41 +2908,48 @@
         <v>55</v>
       </c>
     </row>
+    <row r="127" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C127" s="2"/>
+      <c r="D127" s="7"/>
+    </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A128" s="9" t="s">
-        <v>96</v>
-      </c>
-      <c r="B128" s="9"/>
-      <c r="C128" s="9"/>
-      <c r="D128" s="9"/>
+      <c r="A128" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="B128" s="5" t="s">
+        <v>236</v>
+      </c>
+      <c r="C128" s="4"/>
+      <c r="D128" s="6"/>
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A129" s="1">
         <v>1</v>
       </c>
       <c r="B129" t="s">
-        <v>107</v>
+        <v>237</v>
       </c>
       <c r="C129" s="2" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A130" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="B130" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="C130" s="4"/>
-      <c r="D130" s="6"/>
+      <c r="A130" s="1">
+        <v>2</v>
+      </c>
+      <c r="B130" t="s">
+        <v>239</v>
+      </c>
+      <c r="C130" s="2" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A131" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B131" t="s">
-        <v>109</v>
+        <v>238</v>
       </c>
       <c r="C131" s="2" t="s">
         <v>2</v>
@@ -2918,10 +2957,10 @@
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A132" s="1">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B132" t="s">
-        <v>129</v>
+        <v>246</v>
       </c>
       <c r="C132" s="2" t="s">
         <v>2</v>
@@ -2929,10 +2968,10 @@
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A133" s="1">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B133" t="s">
-        <v>114</v>
+        <v>244</v>
       </c>
       <c r="C133" s="2" t="s">
         <v>2</v>
@@ -2940,10 +2979,10 @@
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A134" s="1">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B134" t="s">
-        <v>115</v>
+        <v>245</v>
       </c>
       <c r="C134" s="2" t="s">
         <v>2</v>
@@ -2951,10 +2990,10 @@
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A135" s="1">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B135" t="s">
-        <v>75</v>
+        <v>240</v>
       </c>
       <c r="C135" s="2" t="s">
         <v>2</v>
@@ -2962,10 +3001,10 @@
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A136" s="1">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B136" t="s">
-        <v>110</v>
+        <v>242</v>
       </c>
       <c r="C136" s="2" t="s">
         <v>2</v>
@@ -2973,10 +3012,10 @@
     </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A137" s="1">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B137" t="s">
-        <v>111</v>
+        <v>243</v>
       </c>
       <c r="C137" s="2" t="s">
         <v>2</v>
@@ -2984,116 +3023,113 @@
     </row>
     <row r="138" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A138" s="1">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B138" t="s">
-        <v>112</v>
+        <v>14</v>
       </c>
       <c r="C138" s="2" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="139" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A139" s="1">
-        <v>9</v>
-      </c>
-      <c r="B139" t="s">
-        <v>113</v>
-      </c>
-      <c r="C139" s="2" t="s">
-        <v>2</v>
-      </c>
+      <c r="A139"/>
+      <c r="C139" s="2"/>
     </row>
     <row r="140" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A140" s="1">
-        <v>10</v>
-      </c>
-      <c r="B140" t="s">
-        <v>116</v>
-      </c>
-      <c r="C140" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="141" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A141" s="1">
-        <v>11</v>
-      </c>
-      <c r="B141" t="s">
-        <v>117</v>
-      </c>
-      <c r="C141" s="2" t="s">
-        <v>2</v>
-      </c>
+      <c r="A140"/>
+      <c r="C140" s="2"/>
     </row>
     <row r="142" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A142" s="1">
-        <v>12</v>
-      </c>
-      <c r="B142" t="s">
-        <v>118</v>
-      </c>
-      <c r="C142" s="2" t="s">
-        <v>2</v>
-      </c>
+      <c r="A142" s="9" t="s">
+        <v>96</v>
+      </c>
+      <c r="B142" s="9"/>
+      <c r="C142" s="9"/>
+      <c r="D142" s="9"/>
     </row>
     <row r="143" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A143" s="1">
-        <v>13</v>
+        <v>1</v>
       </c>
       <c r="B143" t="s">
-        <v>130</v>
+        <v>107</v>
+      </c>
+      <c r="C143" s="2" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="144" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A144" s="1">
-        <v>14</v>
-      </c>
-      <c r="B144" t="s">
-        <v>131</v>
-      </c>
+      <c r="A144" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B144" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="C144" s="4"/>
+      <c r="D144" s="6"/>
     </row>
     <row r="145" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A145" s="1">
-        <v>15</v>
+        <v>1</v>
       </c>
       <c r="B145" t="s">
-        <v>132</v>
+        <v>109</v>
       </c>
       <c r="C145" s="2" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="146" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A146" s="1">
+        <v>2</v>
+      </c>
       <c r="B146" t="s">
-        <v>128</v>
-      </c>
-      <c r="D146" s="7" t="s">
-        <v>55</v>
+        <v>129</v>
+      </c>
+      <c r="C146" s="2" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="147" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A147" s="1">
+        <v>3</v>
+      </c>
       <c r="B147" t="s">
-        <v>233</v>
-      </c>
-      <c r="D147" s="7"/>
+        <v>114</v>
+      </c>
+      <c r="C147" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="148" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A148" s="1">
+        <v>4</v>
+      </c>
+      <c r="B148" t="s">
+        <v>115</v>
+      </c>
+      <c r="C148" s="2" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="149" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A149" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="B149" s="5" t="s">
-        <v>119</v>
-      </c>
-      <c r="C149" s="4"/>
-      <c r="D149" s="6"/>
+      <c r="A149" s="1">
+        <v>5</v>
+      </c>
+      <c r="B149" t="s">
+        <v>75</v>
+      </c>
+      <c r="C149" s="2" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="150" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A150" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B150" t="s">
-        <v>120</v>
+        <v>110</v>
       </c>
       <c r="C150" s="2" t="s">
         <v>2</v>
@@ -3101,10 +3137,10 @@
     </row>
     <row r="151" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A151" s="1">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="B151" t="s">
-        <v>121</v>
+        <v>111</v>
       </c>
       <c r="C151" s="2" t="s">
         <v>2</v>
@@ -3112,10 +3148,10 @@
     </row>
     <row r="152" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A152" s="1">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="B152" t="s">
-        <v>122</v>
+        <v>112</v>
       </c>
       <c r="C152" s="2" t="s">
         <v>2</v>
@@ -3123,10 +3159,10 @@
     </row>
     <row r="153" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A153" s="1">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="B153" t="s">
-        <v>133</v>
+        <v>113</v>
       </c>
       <c r="C153" s="2" t="s">
         <v>2</v>
@@ -3134,103 +3170,94 @@
     </row>
     <row r="154" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A154" s="1">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="B154" t="s">
-        <v>134</v>
-      </c>
-      <c r="C154" s="2"/>
+        <v>116</v>
+      </c>
+      <c r="C154" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="155" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A155" s="1">
+        <v>11</v>
+      </c>
+      <c r="B155" t="s">
+        <v>117</v>
+      </c>
+      <c r="C155" s="2" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="156" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A156" s="4" t="s">
-        <v>123</v>
-      </c>
-      <c r="B156" s="5" t="s">
-        <v>124</v>
-      </c>
-      <c r="C156" s="4"/>
-      <c r="D156" s="6"/>
+      <c r="A156" s="1">
+        <v>12</v>
+      </c>
+      <c r="B156" t="s">
+        <v>118</v>
+      </c>
+      <c r="C156" s="2" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="157" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A157" s="1">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="B157" t="s">
-        <v>125</v>
-      </c>
-      <c r="C157" s="2" t="s">
-        <v>2</v>
+        <v>130</v>
       </c>
     </row>
     <row r="158" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A158" s="1">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="B158" t="s">
-        <v>14</v>
-      </c>
-      <c r="C158" s="2" t="s">
-        <v>2</v>
+        <v>131</v>
       </c>
     </row>
     <row r="159" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A159" s="1">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="B159" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="C159" s="2" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="160" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A160" s="1">
-        <v>4</v>
-      </c>
       <c r="B160" t="s">
-        <v>126</v>
-      </c>
-      <c r="C160" s="2" t="s">
-        <v>2</v>
+        <v>128</v>
+      </c>
+      <c r="D160" s="7" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="161" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A161" s="1">
-        <v>5</v>
-      </c>
       <c r="B161" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="162" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A162" s="1">
-        <v>6</v>
-      </c>
-      <c r="B162" t="s">
-        <v>135</v>
-      </c>
-      <c r="C162" s="2" t="s">
-        <v>2</v>
-      </c>
+        <v>233</v>
+      </c>
+      <c r="D161" s="7"/>
     </row>
     <row r="163" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A163" s="1">
-        <v>7</v>
-      </c>
-      <c r="B163" t="s">
-        <v>136</v>
-      </c>
-      <c r="C163" s="2" t="s">
-        <v>2</v>
-      </c>
+      <c r="A163" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B163" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="C163" s="4"/>
+      <c r="D163" s="6"/>
     </row>
     <row r="164" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A164" s="1">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="B164" t="s">
-        <v>138</v>
+        <v>120</v>
       </c>
       <c r="C164" s="2" t="s">
         <v>2</v>
@@ -3238,61 +3265,62 @@
     </row>
     <row r="165" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A165" s="1">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="B165" t="s">
-        <v>139</v>
+        <v>121</v>
+      </c>
+      <c r="C165" s="2" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="166" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A166" s="1">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="B166" t="s">
-        <v>140</v>
+        <v>122</v>
       </c>
       <c r="C166" s="2" t="s">
         <v>2</v>
       </c>
     </row>
+    <row r="167" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A167" s="1">
+        <v>4</v>
+      </c>
+      <c r="B167" t="s">
+        <v>133</v>
+      </c>
+      <c r="C167" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
     <row r="168" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A168" s="4" t="s">
-        <v>141</v>
-      </c>
-      <c r="B168" s="5" t="s">
-        <v>142</v>
-      </c>
-      <c r="C168" s="4"/>
-      <c r="D168" s="6"/>
-    </row>
-    <row r="169" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A169" s="1">
-        <v>1</v>
-      </c>
-      <c r="B169" t="s">
-        <v>125</v>
-      </c>
-      <c r="C169" s="2" t="s">
-        <v>2</v>
-      </c>
+      <c r="A168" s="1">
+        <v>5</v>
+      </c>
+      <c r="B168" t="s">
+        <v>134</v>
+      </c>
+      <c r="C168" s="2"/>
     </row>
     <row r="170" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A170" s="1">
-        <v>2</v>
-      </c>
-      <c r="B170" t="s">
-        <v>143</v>
-      </c>
-      <c r="C170" s="2" t="s">
-        <v>2</v>
-      </c>
+      <c r="A170" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="B170" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="C170" s="4"/>
+      <c r="D170" s="6"/>
     </row>
     <row r="171" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A171" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B171" t="s">
-        <v>174</v>
+        <v>125</v>
       </c>
       <c r="C171" s="2" t="s">
         <v>2</v>
@@ -3300,10 +3328,10 @@
     </row>
     <row r="172" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A172" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B172" t="s">
-        <v>144</v>
+        <v>14</v>
       </c>
       <c r="C172" s="2" t="s">
         <v>2</v>
@@ -3311,10 +3339,10 @@
     </row>
     <row r="173" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A173" s="1">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B173" t="s">
-        <v>145</v>
+        <v>137</v>
       </c>
       <c r="C173" s="2" t="s">
         <v>2</v>
@@ -3322,10 +3350,10 @@
     </row>
     <row r="174" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A174" s="1">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B174" t="s">
-        <v>146</v>
+        <v>126</v>
       </c>
       <c r="C174" s="2" t="s">
         <v>2</v>
@@ -3333,21 +3361,18 @@
     </row>
     <row r="175" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A175" s="1">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B175" t="s">
-        <v>175</v>
-      </c>
-      <c r="C175" s="2" t="s">
-        <v>2</v>
+        <v>127</v>
       </c>
     </row>
     <row r="176" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A176" s="1">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B176" t="s">
-        <v>147</v>
+        <v>135</v>
       </c>
       <c r="C176" s="2" t="s">
         <v>2</v>
@@ -3355,10 +3380,10 @@
     </row>
     <row r="177" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A177" s="1">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B177" t="s">
-        <v>14</v>
+        <v>136</v>
       </c>
       <c r="C177" s="2" t="s">
         <v>2</v>
@@ -3366,63 +3391,62 @@
     </row>
     <row r="178" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A178" s="1">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B178" t="s">
-        <v>77</v>
-      </c>
-      <c r="C178" s="2"/>
+        <v>138</v>
+      </c>
+      <c r="C178" s="2" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="179" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A179" s="1">
+        <v>9</v>
+      </c>
+      <c r="B179" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="180" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A180" s="1">
+        <v>10</v>
+      </c>
+      <c r="B180" t="s">
+        <v>140</v>
+      </c>
+      <c r="C180" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="181" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A181" s="1">
         <v>11</v>
       </c>
-      <c r="B179" t="s">
-        <v>78</v>
-      </c>
-      <c r="C179" s="2"/>
-    </row>
-    <row r="180" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C180" s="2"/>
-    </row>
-    <row r="181" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A181" s="4" t="s">
-        <v>148</v>
-      </c>
-      <c r="B181" s="5" t="s">
-        <v>158</v>
-      </c>
-      <c r="C181" s="4"/>
-      <c r="D181" s="6"/>
-    </row>
-    <row r="182" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A182" s="1">
-        <v>1</v>
-      </c>
-      <c r="B182" t="s">
-        <v>125</v>
-      </c>
-      <c r="C182" s="2" t="s">
-        <v>2</v>
+      <c r="B181" t="s">
+        <v>241</v>
+      </c>
+      <c r="C181" s="2"/>
+      <c r="D181" s="7" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="183" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A183" s="1">
-        <v>2</v>
-      </c>
-      <c r="B183" t="s">
-        <v>161</v>
-      </c>
-      <c r="C183" s="2" t="s">
-        <v>2</v>
-      </c>
+      <c r="A183" s="4" t="s">
+        <v>141</v>
+      </c>
+      <c r="B183" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="C183" s="4"/>
+      <c r="D183" s="6"/>
     </row>
     <row r="184" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A184" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B184" t="s">
-        <v>162</v>
+        <v>125</v>
       </c>
       <c r="C184" s="2" t="s">
         <v>2</v>
@@ -3430,10 +3454,10 @@
     </row>
     <row r="185" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A185" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B185" t="s">
-        <v>164</v>
+        <v>143</v>
       </c>
       <c r="C185" s="2" t="s">
         <v>2</v>
@@ -3441,10 +3465,10 @@
     </row>
     <row r="186" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A186" s="1">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B186" t="s">
-        <v>166</v>
+        <v>174</v>
       </c>
       <c r="C186" s="2" t="s">
         <v>2</v>
@@ -3452,10 +3476,10 @@
     </row>
     <row r="187" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A187" s="1">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B187" t="s">
-        <v>163</v>
+        <v>144</v>
       </c>
       <c r="C187" s="2" t="s">
         <v>2</v>
@@ -3463,10 +3487,10 @@
     </row>
     <row r="188" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A188" s="1">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B188" t="s">
-        <v>170</v>
+        <v>145</v>
       </c>
       <c r="C188" s="2" t="s">
         <v>2</v>
@@ -3474,10 +3498,10 @@
     </row>
     <row r="189" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A189" s="1">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B189" t="s">
-        <v>169</v>
+        <v>146</v>
       </c>
       <c r="C189" s="2" t="s">
         <v>2</v>
@@ -3485,10 +3509,10 @@
     </row>
     <row r="190" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A190" s="1">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B190" t="s">
-        <v>165</v>
+        <v>175</v>
       </c>
       <c r="C190" s="2" t="s">
         <v>2</v>
@@ -3496,10 +3520,10 @@
     </row>
     <row r="191" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A191" s="1">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B191" t="s">
-        <v>167</v>
+        <v>147</v>
       </c>
       <c r="C191" s="2" t="s">
         <v>2</v>
@@ -3507,10 +3531,10 @@
     </row>
     <row r="192" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A192" s="1">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B192" t="s">
-        <v>168</v>
+        <v>14</v>
       </c>
       <c r="C192" s="2" t="s">
         <v>2</v>
@@ -3518,49 +3542,52 @@
     </row>
     <row r="193" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A193" s="1">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B193" t="s">
-        <v>14</v>
-      </c>
-      <c r="C193" s="2" t="s">
-        <v>2</v>
-      </c>
+        <v>77</v>
+      </c>
+      <c r="C193" s="2"/>
     </row>
     <row r="194" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A194" s="1">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B194" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C194" s="2"/>
     </row>
     <row r="195" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A195" s="1">
-        <v>14</v>
-      </c>
-      <c r="B195" t="s">
-        <v>78</v>
-      </c>
       <c r="C195" s="2"/>
     </row>
+    <row r="196" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A196" s="4" t="s">
+        <v>148</v>
+      </c>
+      <c r="B196" s="5" t="s">
+        <v>158</v>
+      </c>
+      <c r="C196" s="4"/>
+      <c r="D196" s="6"/>
+    </row>
     <row r="197" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A197" s="4" t="s">
-        <v>157</v>
-      </c>
-      <c r="B197" s="5" t="s">
-        <v>149</v>
-      </c>
-      <c r="C197" s="4"/>
-      <c r="D197" s="6"/>
+      <c r="A197" s="1">
+        <v>1</v>
+      </c>
+      <c r="B197" t="s">
+        <v>125</v>
+      </c>
+      <c r="C197" s="2" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="198" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A198" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B198" t="s">
-        <v>150</v>
+        <v>161</v>
       </c>
       <c r="C198" s="2" t="s">
         <v>2</v>
@@ -3568,10 +3595,10 @@
     </row>
     <row r="199" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A199" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B199" t="s">
-        <v>151</v>
+        <v>162</v>
       </c>
       <c r="C199" s="2" t="s">
         <v>2</v>
@@ -3579,10 +3606,10 @@
     </row>
     <row r="200" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A200" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B200" t="s">
-        <v>152</v>
+        <v>164</v>
       </c>
       <c r="C200" s="2" t="s">
         <v>2</v>
@@ -3590,10 +3617,10 @@
     </row>
     <row r="201" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A201" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B201" t="s">
-        <v>153</v>
+        <v>166</v>
       </c>
       <c r="C201" s="2" t="s">
         <v>2</v>
@@ -3601,10 +3628,10 @@
     </row>
     <row r="202" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A202" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B202" t="s">
-        <v>154</v>
+        <v>163</v>
       </c>
       <c r="C202" s="2" t="s">
         <v>2</v>
@@ -3612,10 +3639,10 @@
     </row>
     <row r="203" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A203" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B203" t="s">
-        <v>155</v>
+        <v>170</v>
       </c>
       <c r="C203" s="2" t="s">
         <v>2</v>
@@ -3623,10 +3650,10 @@
     </row>
     <row r="204" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A204" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B204" t="s">
-        <v>156</v>
+        <v>169</v>
       </c>
       <c r="C204" s="2" t="s">
         <v>2</v>
@@ -3634,10 +3661,10 @@
     </row>
     <row r="205" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A205" s="1">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B205" t="s">
-        <v>14</v>
+        <v>165</v>
       </c>
       <c r="C205" s="2" t="s">
         <v>2</v>
@@ -3645,69 +3672,71 @@
     </row>
     <row r="206" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A206" s="1">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B206" t="s">
-        <v>77</v>
+        <v>167</v>
+      </c>
+      <c r="C206" s="2" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="207" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A207" s="1">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B207" t="s">
-        <v>78</v>
+        <v>168</v>
+      </c>
+      <c r="C207" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="208" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A208" s="1">
+        <v>12</v>
+      </c>
+      <c r="B208" t="s">
+        <v>14</v>
+      </c>
+      <c r="C208" s="2" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="209" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A209" s="4" t="s">
-        <v>159</v>
-      </c>
-      <c r="B209" s="5" t="s">
-        <v>160</v>
-      </c>
-      <c r="C209" s="4"/>
-      <c r="D209" s="6"/>
+      <c r="A209" s="1">
+        <v>13</v>
+      </c>
+      <c r="B209" t="s">
+        <v>77</v>
+      </c>
+      <c r="C209" s="2"/>
     </row>
     <row r="210" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A210" s="1">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="B210" t="s">
-        <v>171</v>
-      </c>
-      <c r="C210" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="211" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A211" s="1">
-        <v>2</v>
-      </c>
-      <c r="B211" t="s">
-        <v>172</v>
-      </c>
-      <c r="C211" s="2" t="s">
-        <v>2</v>
-      </c>
+        <v>78</v>
+      </c>
+      <c r="C210" s="2"/>
     </row>
     <row r="212" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A212" s="1">
-        <v>3</v>
-      </c>
-      <c r="B212" t="s">
-        <v>173</v>
-      </c>
-      <c r="C212" s="2" t="s">
-        <v>2</v>
-      </c>
+      <c r="A212" s="4" t="s">
+        <v>157</v>
+      </c>
+      <c r="B212" s="5" t="s">
+        <v>149</v>
+      </c>
+      <c r="C212" s="4"/>
+      <c r="D212" s="6"/>
     </row>
     <row r="213" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A213" s="1">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B213" t="s">
-        <v>176</v>
+        <v>150</v>
       </c>
       <c r="C213" s="2" t="s">
         <v>2</v>
@@ -3715,10 +3744,10 @@
     </row>
     <row r="214" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A214" s="1">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B214" t="s">
-        <v>177</v>
+        <v>151</v>
       </c>
       <c r="C214" s="2" t="s">
         <v>2</v>
@@ -3726,10 +3755,10 @@
     </row>
     <row r="215" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A215" s="1">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B215" t="s">
-        <v>14</v>
+        <v>152</v>
       </c>
       <c r="C215" s="2" t="s">
         <v>2</v>
@@ -3737,39 +3766,54 @@
     </row>
     <row r="216" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A216" s="1">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B216" t="s">
-        <v>77</v>
+        <v>153</v>
+      </c>
+      <c r="C216" s="2" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="217" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A217" s="1">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B217" t="s">
-        <v>78</v>
+        <v>154</v>
+      </c>
+      <c r="C217" s="2" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="218" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C218" s="2"/>
+      <c r="A218" s="1">
+        <v>6</v>
+      </c>
+      <c r="B218" t="s">
+        <v>155</v>
+      </c>
+      <c r="C218" s="2" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="219" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A219" s="4" t="s">
-        <v>178</v>
-      </c>
-      <c r="B219" s="5" t="s">
-        <v>179</v>
-      </c>
-      <c r="C219" s="4"/>
-      <c r="D219" s="6"/>
+      <c r="A219" s="1">
+        <v>7</v>
+      </c>
+      <c r="B219" t="s">
+        <v>156</v>
+      </c>
+      <c r="C219" s="2" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="220" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A220" s="1">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="B220" t="s">
-        <v>125</v>
+        <v>14</v>
       </c>
       <c r="C220" s="2" t="s">
         <v>2</v>
@@ -3777,54 +3821,36 @@
     </row>
     <row r="221" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A221" s="1">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="B221" t="s">
-        <v>180</v>
-      </c>
-      <c r="C221" s="2" t="s">
-        <v>2</v>
+        <v>77</v>
       </c>
     </row>
     <row r="222" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A222" s="1">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="B222" t="s">
-        <v>181</v>
-      </c>
-      <c r="C222" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="223" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A223" s="1">
-        <v>4</v>
-      </c>
-      <c r="B223" t="s">
-        <v>182</v>
-      </c>
-      <c r="C223" s="2" t="s">
-        <v>2</v>
+        <v>78</v>
       </c>
     </row>
     <row r="224" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A224" s="1">
-        <v>5</v>
-      </c>
-      <c r="B224" t="s">
-        <v>183</v>
-      </c>
-      <c r="C224" s="2" t="s">
-        <v>2</v>
-      </c>
+      <c r="A224" s="4" t="s">
+        <v>159</v>
+      </c>
+      <c r="B224" s="5" t="s">
+        <v>160</v>
+      </c>
+      <c r="C224" s="4"/>
+      <c r="D224" s="6"/>
     </row>
     <row r="225" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A225" s="1">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="B225" t="s">
-        <v>184</v>
+        <v>171</v>
       </c>
       <c r="C225" s="2" t="s">
         <v>2</v>
@@ -3832,10 +3858,10 @@
     </row>
     <row r="226" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A226" s="1">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B226" t="s">
-        <v>14</v>
+        <v>172</v>
       </c>
       <c r="C226" s="2" t="s">
         <v>2</v>
@@ -3843,80 +3869,83 @@
     </row>
     <row r="227" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A227" s="1">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="B227" t="s">
-        <v>77</v>
+        <v>173</v>
+      </c>
+      <c r="C227" s="2" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="228" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A228" s="1">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="B228" t="s">
-        <v>78</v>
+        <v>176</v>
+      </c>
+      <c r="C228" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="229" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A229" s="1">
+        <v>5</v>
+      </c>
+      <c r="B229" t="s">
+        <v>177</v>
+      </c>
+      <c r="C229" s="2" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="230" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A230" s="4" t="s">
-        <v>185</v>
-      </c>
-      <c r="B230" s="5" t="s">
-        <v>187</v>
-      </c>
-      <c r="C230" s="4"/>
-      <c r="D230" s="6"/>
+      <c r="A230" s="1">
+        <v>6</v>
+      </c>
+      <c r="B230" t="s">
+        <v>14</v>
+      </c>
+      <c r="C230" s="2" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="231" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A231" s="1">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="B231" t="s">
-        <v>186</v>
-      </c>
-      <c r="C231" s="2" t="s">
-        <v>2</v>
+        <v>77</v>
       </c>
     </row>
     <row r="232" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A232" s="1">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="B232" t="s">
-        <v>188</v>
-      </c>
-      <c r="C232" s="2" t="s">
-        <v>2</v>
+        <v>78</v>
       </c>
     </row>
     <row r="233" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A233" s="1">
-        <v>3</v>
-      </c>
-      <c r="B233" t="s">
-        <v>189</v>
-      </c>
-      <c r="C233" s="2" t="s">
-        <v>2</v>
-      </c>
+      <c r="C233" s="2"/>
     </row>
     <row r="234" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A234" s="1">
-        <v>4</v>
-      </c>
-      <c r="B234" t="s">
-        <v>190</v>
-      </c>
-      <c r="C234" s="2" t="s">
-        <v>2</v>
-      </c>
+      <c r="A234" s="4" t="s">
+        <v>178</v>
+      </c>
+      <c r="B234" s="5" t="s">
+        <v>179</v>
+      </c>
+      <c r="C234" s="4"/>
+      <c r="D234" s="6"/>
     </row>
     <row r="235" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A235" s="1">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="B235" t="s">
-        <v>191</v>
+        <v>125</v>
       </c>
       <c r="C235" s="2" t="s">
         <v>2</v>
@@ -3924,10 +3953,10 @@
     </row>
     <row r="236" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A236" s="1">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="B236" t="s">
-        <v>14</v>
+        <v>180</v>
       </c>
       <c r="C236" s="2" t="s">
         <v>2</v>
@@ -3935,205 +3964,205 @@
     </row>
     <row r="237" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A237" s="1">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="B237" t="s">
-        <v>77</v>
+        <v>181</v>
+      </c>
+      <c r="C237" s="2" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="238" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A238" s="1">
+        <v>4</v>
+      </c>
+      <c r="B238" t="s">
+        <v>182</v>
+      </c>
+      <c r="C238" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="239" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A239" s="1">
+        <v>5</v>
+      </c>
+      <c r="B239" t="s">
+        <v>183</v>
+      </c>
+      <c r="C239" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="240" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A240" s="1">
+        <v>6</v>
+      </c>
+      <c r="B240" t="s">
+        <v>184</v>
+      </c>
+      <c r="C240" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="241" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A241" s="1">
+        <v>7</v>
+      </c>
+      <c r="B241" t="s">
+        <v>14</v>
+      </c>
+      <c r="C241" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="242" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A242" s="1">
         <v>8</v>
       </c>
-      <c r="B238" t="s">
+      <c r="B242" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="243" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A243" s="1">
+        <v>9</v>
+      </c>
+      <c r="B243" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="240" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A240" s="4" t="s">
+    <row r="245" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A245" s="4" t="s">
+        <v>185</v>
+      </c>
+      <c r="B245" s="5" t="s">
+        <v>187</v>
+      </c>
+      <c r="C245" s="4"/>
+      <c r="D245" s="6"/>
+    </row>
+    <row r="246" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A246" s="1">
+        <v>1</v>
+      </c>
+      <c r="B246" t="s">
+        <v>186</v>
+      </c>
+      <c r="C246" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="247" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A247" s="1">
+        <v>2</v>
+      </c>
+      <c r="B247" t="s">
+        <v>188</v>
+      </c>
+      <c r="C247" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="248" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A248" s="1">
+        <v>3</v>
+      </c>
+      <c r="B248" t="s">
+        <v>189</v>
+      </c>
+      <c r="C248" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="249" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A249" s="1">
+        <v>4</v>
+      </c>
+      <c r="B249" t="s">
+        <v>190</v>
+      </c>
+      <c r="C249" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="250" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A250" s="1">
+        <v>5</v>
+      </c>
+      <c r="B250" t="s">
+        <v>191</v>
+      </c>
+      <c r="C250" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="251" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A251" s="1">
+        <v>6</v>
+      </c>
+      <c r="B251" t="s">
+        <v>14</v>
+      </c>
+      <c r="C251" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="252" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A252" s="1">
+        <v>7</v>
+      </c>
+      <c r="B252" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="253" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A253" s="1">
+        <v>8</v>
+      </c>
+      <c r="B253" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="255" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A255" s="4" t="s">
         <v>192</v>
       </c>
-      <c r="B240" s="5" t="s">
+      <c r="B255" s="5" t="s">
         <v>193</v>
       </c>
-      <c r="C240" s="4"/>
-      <c r="D240" s="6"/>
-    </row>
-    <row r="241" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A241" s="1">
+      <c r="C255" s="4"/>
+      <c r="D255" s="6"/>
+    </row>
+    <row r="256" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A256" s="1">
         <v>1</v>
       </c>
-      <c r="B241" t="s">
+      <c r="B256" t="s">
         <v>125</v>
       </c>
-      <c r="C241" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="242" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A242" s="1">
-        <v>2</v>
-      </c>
-      <c r="B242" t="s">
+      <c r="C256" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="257" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A257" s="1">
+        <v>2</v>
+      </c>
+      <c r="B257" t="s">
         <v>194</v>
       </c>
-      <c r="C242" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="243" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A243" s="1">
-        <v>3</v>
-      </c>
-      <c r="B243" t="s">
-        <v>195</v>
-      </c>
-      <c r="C243" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="244" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A244" s="1">
-        <v>4</v>
-      </c>
-      <c r="B244" t="s">
-        <v>199</v>
-      </c>
-      <c r="C244" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="245" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A245" s="1">
-        <v>5</v>
-      </c>
-      <c r="B245" t="s">
-        <v>196</v>
-      </c>
-      <c r="C245" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="246" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A246" s="1">
-        <v>6</v>
-      </c>
-      <c r="B246" t="s">
-        <v>197</v>
-      </c>
-      <c r="C246" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="247" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A247" s="1">
-        <v>7</v>
-      </c>
-      <c r="B247" t="s">
-        <v>198</v>
-      </c>
-      <c r="C247" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="248" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A248" s="1">
-        <v>8</v>
-      </c>
-      <c r="B248" t="s">
-        <v>200</v>
-      </c>
-      <c r="C248" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="249" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A249" s="1">
-        <v>9</v>
-      </c>
-      <c r="B249" t="s">
-        <v>201</v>
-      </c>
-      <c r="C249" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="250" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A250" s="1">
-        <v>10</v>
-      </c>
-      <c r="B250" t="s">
-        <v>202</v>
-      </c>
-      <c r="C250" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="251" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A251" s="1">
-        <v>11</v>
-      </c>
-      <c r="B251" t="s">
-        <v>203</v>
-      </c>
-      <c r="C251" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="252" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A252" s="1">
-        <v>12</v>
-      </c>
-      <c r="B252" t="s">
-        <v>204</v>
-      </c>
-      <c r="C252" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="253" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A253" s="1">
-        <v>13</v>
-      </c>
-      <c r="B253" t="s">
-        <v>14</v>
-      </c>
-      <c r="C253" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="254" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A254" s="1">
-        <v>14</v>
-      </c>
-      <c r="B254" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="255" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A255" s="1">
-        <v>15</v>
-      </c>
-      <c r="B255" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="257" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A257" s="4" t="s">
-        <v>205</v>
-      </c>
-      <c r="B257" s="5" t="s">
-        <v>206</v>
-      </c>
-      <c r="C257" s="4"/>
-      <c r="D257" s="6"/>
+      <c r="C257" s="2" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="258" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A258" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B258" t="s">
-        <v>125</v>
+        <v>195</v>
       </c>
       <c r="C258" s="2" t="s">
         <v>2</v>
@@ -4141,10 +4170,10 @@
     </row>
     <row r="259" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A259" s="1">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B259" t="s">
-        <v>207</v>
+        <v>199</v>
       </c>
       <c r="C259" s="2" t="s">
         <v>2</v>
@@ -4152,10 +4181,10 @@
     </row>
     <row r="260" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A260" s="1">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B260" t="s">
-        <v>208</v>
+        <v>196</v>
       </c>
       <c r="C260" s="2" t="s">
         <v>2</v>
@@ -4163,10 +4192,10 @@
     </row>
     <row r="261" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A261" s="1">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B261" t="s">
-        <v>209</v>
+        <v>197</v>
       </c>
       <c r="C261" s="2" t="s">
         <v>2</v>
@@ -4174,10 +4203,10 @@
     </row>
     <row r="262" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A262" s="1">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B262" t="s">
-        <v>210</v>
+        <v>198</v>
       </c>
       <c r="C262" s="2" t="s">
         <v>2</v>
@@ -4185,10 +4214,10 @@
     </row>
     <row r="263" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A263" s="1">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B263" t="s">
-        <v>14</v>
+        <v>200</v>
       </c>
       <c r="C263" s="2" t="s">
         <v>2</v>
@@ -4196,36 +4225,54 @@
     </row>
     <row r="264" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A264" s="1">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B264" t="s">
-        <v>77</v>
+        <v>201</v>
+      </c>
+      <c r="C264" s="2" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="265" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A265" s="1">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B265" t="s">
-        <v>78</v>
+        <v>202</v>
+      </c>
+      <c r="C265" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="266" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A266" s="1">
+        <v>11</v>
+      </c>
+      <c r="B266" t="s">
+        <v>203</v>
+      </c>
+      <c r="C266" s="2" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="267" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A267" s="4" t="s">
-        <v>211</v>
-      </c>
-      <c r="B267" s="5" t="s">
-        <v>212</v>
-      </c>
-      <c r="C267" s="4"/>
-      <c r="D267" s="6"/>
+      <c r="A267" s="1">
+        <v>12</v>
+      </c>
+      <c r="B267" t="s">
+        <v>204</v>
+      </c>
+      <c r="C267" s="2" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="268" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A268" s="1">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="B268" t="s">
-        <v>213</v>
+        <v>14</v>
       </c>
       <c r="C268" s="2" t="s">
         <v>2</v>
@@ -4233,71 +4280,69 @@
     </row>
     <row r="269" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A269" s="1">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="B269" t="s">
-        <v>214</v>
-      </c>
-      <c r="C269" s="2" t="s">
-        <v>2</v>
+        <v>77</v>
       </c>
     </row>
     <row r="270" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A270" s="1">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="B270" t="s">
-        <v>215</v>
-      </c>
-      <c r="C270" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="271" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A271" s="1">
-        <v>4</v>
-      </c>
-      <c r="B271" t="s">
-        <v>14</v>
-      </c>
-      <c r="C271" s="2" t="s">
-        <v>2</v>
+        <v>78</v>
       </c>
     </row>
     <row r="272" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A272" s="1">
-        <v>5</v>
-      </c>
-      <c r="B272" t="s">
-        <v>77</v>
-      </c>
-      <c r="C272" s="2"/>
+      <c r="A272" s="4" t="s">
+        <v>205</v>
+      </c>
+      <c r="B272" s="5" t="s">
+        <v>206</v>
+      </c>
+      <c r="C272" s="4"/>
+      <c r="D272" s="6"/>
     </row>
     <row r="273" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A273" s="1">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="B273" t="s">
-        <v>78</v>
-      </c>
-      <c r="C273" s="2"/>
+        <v>125</v>
+      </c>
+      <c r="C273" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="274" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A274" s="1">
+        <v>2</v>
+      </c>
+      <c r="B274" t="s">
+        <v>207</v>
+      </c>
+      <c r="C274" s="2" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="275" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A275" s="4" t="s">
-        <v>216</v>
-      </c>
-      <c r="B275" s="5" t="s">
-        <v>217</v>
-      </c>
-      <c r="C275" s="4"/>
-      <c r="D275" s="6"/>
+      <c r="A275" s="1">
+        <v>3</v>
+      </c>
+      <c r="B275" t="s">
+        <v>208</v>
+      </c>
+      <c r="C275" s="2" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="276" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A276" s="1">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="B276" t="s">
-        <v>125</v>
+        <v>209</v>
       </c>
       <c r="C276" s="2" t="s">
         <v>2</v>
@@ -4305,10 +4350,10 @@
     </row>
     <row r="277" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A277" s="1">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="B277" t="s">
-        <v>218</v>
+        <v>210</v>
       </c>
       <c r="C277" s="2" t="s">
         <v>2</v>
@@ -4316,10 +4361,10 @@
     </row>
     <row r="278" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A278" s="1">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="B278" t="s">
-        <v>219</v>
+        <v>14</v>
       </c>
       <c r="C278" s="2" t="s">
         <v>2</v>
@@ -4327,54 +4372,36 @@
     </row>
     <row r="279" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A279" s="1">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="B279" t="s">
-        <v>220</v>
-      </c>
-      <c r="C279" s="2" t="s">
-        <v>2</v>
+        <v>77</v>
       </c>
     </row>
     <row r="280" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A280" s="1">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="B280" t="s">
-        <v>222</v>
-      </c>
-      <c r="C280" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="281" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A281" s="1">
-        <v>6</v>
-      </c>
-      <c r="B281" t="s">
-        <v>221</v>
-      </c>
-      <c r="C281" s="2" t="s">
-        <v>2</v>
+        <v>78</v>
       </c>
     </row>
     <row r="282" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A282" s="1">
-        <v>7</v>
-      </c>
-      <c r="B282" t="s">
-        <v>223</v>
-      </c>
-      <c r="C282" s="2" t="s">
-        <v>2</v>
-      </c>
+      <c r="A282" s="4" t="s">
+        <v>211</v>
+      </c>
+      <c r="B282" s="5" t="s">
+        <v>212</v>
+      </c>
+      <c r="C282" s="4"/>
+      <c r="D282" s="6"/>
     </row>
     <row r="283" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A283" s="1">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="B283" t="s">
-        <v>224</v>
+        <v>213</v>
       </c>
       <c r="C283" s="2" t="s">
         <v>2</v>
@@ -4382,10 +4409,10 @@
     </row>
     <row r="284" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A284" s="1">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="B284" t="s">
-        <v>225</v>
+        <v>214</v>
       </c>
       <c r="C284" s="2" t="s">
         <v>2</v>
@@ -4393,10 +4420,10 @@
     </row>
     <row r="285" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A285" s="1">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="B285" t="s">
-        <v>226</v>
+        <v>215</v>
       </c>
       <c r="C285" s="2" t="s">
         <v>2</v>
@@ -4404,10 +4431,10 @@
     </row>
     <row r="286" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A286" s="1">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="B286" t="s">
-        <v>227</v>
+        <v>14</v>
       </c>
       <c r="C286" s="2" t="s">
         <v>2</v>
@@ -4415,76 +4442,225 @@
     </row>
     <row r="287" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A287" s="1">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="B287" t="s">
-        <v>228</v>
+        <v>77</v>
       </c>
       <c r="C287" s="2"/>
     </row>
     <row r="288" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A288" s="1">
+        <v>6</v>
+      </c>
+      <c r="B288" t="s">
+        <v>78</v>
+      </c>
+      <c r="C288" s="2"/>
+    </row>
+    <row r="290" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A290" s="4" t="s">
+        <v>216</v>
+      </c>
+      <c r="B290" s="5" t="s">
+        <v>217</v>
+      </c>
+      <c r="C290" s="4"/>
+      <c r="D290" s="6"/>
+    </row>
+    <row r="291" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A291" s="1">
+        <v>1</v>
+      </c>
+      <c r="B291" t="s">
+        <v>125</v>
+      </c>
+      <c r="C291" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="292" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A292" s="1">
+        <v>2</v>
+      </c>
+      <c r="B292" t="s">
+        <v>218</v>
+      </c>
+      <c r="C292" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="293" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A293" s="1">
+        <v>3</v>
+      </c>
+      <c r="B293" t="s">
+        <v>219</v>
+      </c>
+      <c r="C293" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="294" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A294" s="1">
+        <v>4</v>
+      </c>
+      <c r="B294" t="s">
+        <v>220</v>
+      </c>
+      <c r="C294" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="295" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A295" s="1">
+        <v>5</v>
+      </c>
+      <c r="B295" t="s">
+        <v>222</v>
+      </c>
+      <c r="C295" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="296" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A296" s="1">
+        <v>6</v>
+      </c>
+      <c r="B296" t="s">
+        <v>221</v>
+      </c>
+      <c r="C296" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="297" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A297" s="1">
+        <v>7</v>
+      </c>
+      <c r="B297" t="s">
+        <v>223</v>
+      </c>
+      <c r="C297" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="298" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A298" s="1">
+        <v>8</v>
+      </c>
+      <c r="B298" t="s">
+        <v>224</v>
+      </c>
+      <c r="C298" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="299" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A299" s="1">
+        <v>9</v>
+      </c>
+      <c r="B299" t="s">
+        <v>225</v>
+      </c>
+      <c r="C299" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="300" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A300" s="1">
+        <v>10</v>
+      </c>
+      <c r="B300" t="s">
+        <v>226</v>
+      </c>
+      <c r="C300" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="301" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A301" s="1">
+        <v>11</v>
+      </c>
+      <c r="B301" t="s">
+        <v>227</v>
+      </c>
+      <c r="C301" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="302" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A302" s="1">
+        <v>12</v>
+      </c>
+      <c r="B302" t="s">
+        <v>228</v>
+      </c>
+      <c r="C302" s="2"/>
+    </row>
+    <row r="303" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A303" s="1">
         <v>13</v>
       </c>
-      <c r="B288" t="s">
+      <c r="B303" t="s">
         <v>229</v>
       </c>
-      <c r="C288" s="2"/>
-    </row>
-    <row r="289" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A289" s="1">
+      <c r="C303" s="2"/>
+    </row>
+    <row r="304" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A304" s="1">
         <v>14</v>
       </c>
-      <c r="B289" t="s">
+      <c r="B304" t="s">
         <v>230</v>
       </c>
-      <c r="C289" s="2"/>
-    </row>
-    <row r="290" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A290" s="1">
+      <c r="C304" s="2"/>
+    </row>
+    <row r="305" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A305" s="1">
         <v>15</v>
       </c>
-      <c r="B290" t="s">
+      <c r="B305" t="s">
         <v>231</v>
       </c>
-      <c r="C290" s="2"/>
-    </row>
-    <row r="291" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A291" s="1">
+      <c r="C305" s="2"/>
+    </row>
+    <row r="306" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A306" s="1">
         <v>16</v>
       </c>
-      <c r="B291" t="s">
+      <c r="B306" t="s">
         <v>232</v>
       </c>
-      <c r="C291" s="2"/>
-    </row>
-    <row r="292" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A292" s="1">
+      <c r="C306" s="2"/>
+    </row>
+    <row r="307" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A307" s="1">
         <v>17</v>
       </c>
-      <c r="B292" t="s">
+      <c r="B307" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="293" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A293" s="1">
+    <row r="308" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A308" s="1">
         <v>18</v>
       </c>
-      <c r="B293" t="s">
+      <c r="B308" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="294" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A294" s="1">
+    <row r="309" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A309" s="1">
         <v>19</v>
       </c>
-      <c r="B294" t="s">
+      <c r="B309" t="s">
         <v>78</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="8">
-    <mergeCell ref="A128:D128"/>
+    <mergeCell ref="A142:D142"/>
     <mergeCell ref="A71:D71"/>
     <mergeCell ref="A1:D1"/>
     <mergeCell ref="A7:D7"/>

</xml_diff>

<commit_message>
echo emp name in nav bar
</commit_message>
<xml_diff>
--- a/Tasks.xlsx
+++ b/Tasks.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="558" uniqueCount="266">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="560" uniqueCount="267">
   <si>
     <t>Login</t>
   </si>
@@ -1235,6 +1235,9 @@
   </si>
   <si>
     <t>Insert_By</t>
+  </si>
+  <si>
+    <t>اظهار اسم الموظف في راس الصفحة</t>
   </si>
 </sst>
 </file>
@@ -1717,10 +1720,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D328"/>
+  <dimension ref="A1:D329"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1766,7 +1769,10 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>4</v>
+        <v>266</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -1774,34 +1780,31 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
         <v>5</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="10" t="s">
+      <c r="B6" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="13"/>
-      <c r="C7" s="13"/>
-      <c r="D7" s="13"/>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="1">
-        <v>1</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>2</v>
-      </c>
+      <c r="B8" s="13"/>
+      <c r="C8" s="13"/>
+      <c r="D8" s="13"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>2</v>
@@ -1809,10 +1812,10 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>2</v>
@@ -1820,10 +1823,10 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>2</v>
@@ -1831,10 +1834,10 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>2</v>
@@ -1842,10 +1845,10 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>2</v>
@@ -1853,55 +1856,55 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
-        <v>7</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>12</v>
+        <v>6</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
+        <v>7</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="1">
         <v>8</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="B16" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="10" t="s">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="B17" s="14"/>
-      <c r="C17" s="14"/>
-      <c r="D17" s="14"/>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="4" t="s">
+      <c r="B18" s="14"/>
+      <c r="C18" s="14"/>
+      <c r="D18" s="14"/>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="B18" s="5" t="s">
+      <c r="B19" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C18" s="4"/>
-      <c r="D18" s="6"/>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="1">
-        <v>1</v>
-      </c>
-      <c r="B19" t="s">
-        <v>18</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>2</v>
-      </c>
+      <c r="C19" s="4"/>
+      <c r="D19" s="6"/>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B20" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="C20" s="2" t="s">
         <v>2</v>
@@ -1909,10 +1912,10 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B21" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>2</v>
@@ -1920,10 +1923,10 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B22" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C22" s="2" t="s">
         <v>2</v>
@@ -1931,10 +1934,10 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B23" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C23" s="2" t="s">
         <v>2</v>
@@ -1942,10 +1945,10 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B24" t="s">
-        <v>44</v>
+        <v>20</v>
       </c>
       <c r="C24" s="2" t="s">
         <v>2</v>
@@ -1953,10 +1956,10 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B25" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C25" s="2" t="s">
         <v>2</v>
@@ -1964,10 +1967,10 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B26" t="s">
-        <v>22</v>
+        <v>45</v>
       </c>
       <c r="C26" s="2" t="s">
         <v>2</v>
@@ -1975,45 +1978,45 @@
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
+        <v>8</v>
+      </c>
+      <c r="B27" t="s">
+        <v>22</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="1">
         <v>9</v>
       </c>
-      <c r="B27" t="s">
+      <c r="B28" t="s">
         <v>57</v>
       </c>
-      <c r="C27" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D27" s="7" t="s">
+      <c r="C28" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D28" s="7" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="4" t="s">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="B29" s="5" t="s">
+      <c r="B30" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="C29" s="4"/>
-      <c r="D29" s="6"/>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="1">
-        <v>1</v>
-      </c>
-      <c r="B30" t="s">
-        <v>25</v>
-      </c>
-      <c r="C30" s="2" t="s">
-        <v>2</v>
-      </c>
+      <c r="C30" s="4"/>
+      <c r="D30" s="6"/>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B31" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="C31" s="2" t="s">
         <v>2</v>
@@ -2021,10 +2024,10 @@
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B32" t="s">
-        <v>14</v>
+        <v>31</v>
       </c>
       <c r="C32" s="2" t="s">
         <v>2</v>
@@ -2032,10 +2035,10 @@
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B33" t="s">
-        <v>27</v>
+        <v>14</v>
       </c>
       <c r="C33" s="2" t="s">
         <v>2</v>
@@ -2043,10 +2046,10 @@
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B34" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C34" s="2" t="s">
         <v>2</v>
@@ -2054,10 +2057,10 @@
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B35" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C35" s="2" t="s">
         <v>2</v>
@@ -2065,10 +2068,10 @@
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B36" t="s">
-        <v>53</v>
+        <v>29</v>
       </c>
       <c r="C36" s="2" t="s">
         <v>2</v>
@@ -2076,10 +2079,10 @@
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B37" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C37" s="2" t="s">
         <v>2</v>
@@ -2087,10 +2090,10 @@
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B38" t="s">
-        <v>30</v>
+        <v>54</v>
       </c>
       <c r="C38" s="2" t="s">
         <v>2</v>
@@ -2098,10 +2101,10 @@
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B39" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="C39" s="2" t="s">
         <v>2</v>
@@ -2109,10 +2112,10 @@
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B40" t="s">
-        <v>52</v>
+        <v>35</v>
       </c>
       <c r="C40" s="2" t="s">
         <v>2</v>
@@ -2123,7 +2126,7 @@
         <v>11</v>
       </c>
       <c r="B41" t="s">
-        <v>32</v>
+        <v>52</v>
       </c>
       <c r="C41" s="2" t="s">
         <v>2</v>
@@ -2131,10 +2134,10 @@
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B42" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C42" s="2" t="s">
         <v>2</v>
@@ -2142,10 +2145,10 @@
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B43" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C43" s="2" t="s">
         <v>2</v>
@@ -2153,10 +2156,10 @@
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B44" t="s">
-        <v>43</v>
+        <v>34</v>
       </c>
       <c r="C44" s="2" t="s">
         <v>2</v>
@@ -2164,10 +2167,10 @@
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B45" t="s">
-        <v>36</v>
+        <v>43</v>
       </c>
       <c r="C45" s="2" t="s">
         <v>2</v>
@@ -2175,53 +2178,53 @@
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
+        <v>15</v>
+      </c>
+      <c r="B46" t="s">
+        <v>36</v>
+      </c>
+      <c r="C46" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A47" s="1">
         <v>16</v>
       </c>
-      <c r="B46" t="s">
+      <c r="B47" t="s">
         <v>56</v>
       </c>
-      <c r="C46" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D46" s="7" t="s">
+      <c r="C47" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D47" s="7" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A48" s="10" t="s">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A49" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="B48" s="10"/>
-      <c r="C48" s="10"/>
-      <c r="D48" s="10"/>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A49" s="4" t="s">
+      <c r="B49" s="10"/>
+      <c r="C49" s="10"/>
+      <c r="D49" s="10"/>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A50" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="B49" s="5" t="s">
+      <c r="B50" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="C49" s="4"/>
-      <c r="D49" s="6"/>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A50" s="1">
-        <v>1</v>
-      </c>
-      <c r="B50" t="s">
-        <v>39</v>
-      </c>
-      <c r="C50" s="2" t="s">
-        <v>2</v>
-      </c>
+      <c r="C50" s="4"/>
+      <c r="D50" s="6"/>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B51" t="s">
-        <v>26</v>
+        <v>39</v>
       </c>
       <c r="C51" s="2" t="s">
         <v>2</v>
@@ -2229,10 +2232,10 @@
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B52" t="s">
-        <v>40</v>
+        <v>26</v>
       </c>
       <c r="C52" s="2" t="s">
         <v>2</v>
@@ -2240,54 +2243,54 @@
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B53" t="s">
-        <v>21</v>
-      </c>
-      <c r="C53" s="2"/>
+        <v>40</v>
+      </c>
+      <c r="C53" s="2" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" s="1">
+        <v>4</v>
+      </c>
+      <c r="B54" t="s">
+        <v>21</v>
+      </c>
+      <c r="C54" s="2"/>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A55" s="1">
         <v>5</v>
       </c>
-      <c r="B54" t="s">
+      <c r="B55" t="s">
         <v>57</v>
       </c>
-      <c r="C54" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D54" s="7" t="s">
+      <c r="C55" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D55" s="7" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A56" s="4" t="s">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A57" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="B56" s="5" t="s">
+      <c r="B57" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="C56" s="4"/>
-      <c r="D56" s="6"/>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A57" s="1">
-        <v>1</v>
-      </c>
-      <c r="B57" t="s">
-        <v>42</v>
-      </c>
-      <c r="C57" s="2" t="s">
-        <v>2</v>
-      </c>
+      <c r="C57" s="4"/>
+      <c r="D57" s="6"/>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B58" t="s">
-        <v>31</v>
+        <v>42</v>
       </c>
       <c r="C58" s="2" t="s">
         <v>2</v>
@@ -2295,10 +2298,10 @@
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B59" t="s">
-        <v>14</v>
+        <v>31</v>
       </c>
       <c r="C59" s="2" t="s">
         <v>2</v>
@@ -2306,10 +2309,10 @@
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B60" t="s">
-        <v>46</v>
+        <v>14</v>
       </c>
       <c r="C60" s="2" t="s">
         <v>2</v>
@@ -2317,10 +2320,10 @@
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B61" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C61" s="2" t="s">
         <v>2</v>
@@ -2328,10 +2331,10 @@
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B62" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C62" s="2" t="s">
         <v>2</v>
@@ -2339,10 +2342,10 @@
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B63" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="C63" s="2" t="s">
         <v>2</v>
@@ -2350,72 +2353,72 @@
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" s="1">
+        <v>7</v>
+      </c>
+      <c r="B64" t="s">
+        <v>43</v>
+      </c>
+      <c r="C64" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A65" s="1">
         <v>8</v>
       </c>
-      <c r="B64" t="s">
+      <c r="B65" t="s">
         <v>36</v>
       </c>
-      <c r="C64" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A66" s="10" t="s">
+      <c r="C65" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A67" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="B66" s="10"/>
-      <c r="C66" s="10"/>
-      <c r="D66" s="10"/>
-    </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A67" s="1">
-        <v>1</v>
-      </c>
-      <c r="B67" t="s">
-        <v>50</v>
-      </c>
+      <c r="B67" s="10"/>
+      <c r="C67" s="10"/>
+      <c r="D67" s="10"/>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B68" t="s">
-        <v>14</v>
+        <v>50</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" s="1">
+        <v>2</v>
+      </c>
+      <c r="B69" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A70" s="1">
         <v>3</v>
       </c>
-      <c r="B69" t="s">
+      <c r="B70" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A71" s="10" t="s">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A72" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="B71" s="10"/>
-      <c r="C71" s="10"/>
-      <c r="D71" s="10"/>
-    </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A72" s="1">
-        <v>1</v>
-      </c>
-      <c r="B72" t="s">
-        <v>59</v>
-      </c>
-      <c r="C72" s="2" t="s">
-        <v>2</v>
-      </c>
+      <c r="B72" s="10"/>
+      <c r="C72" s="10"/>
+      <c r="D72" s="10"/>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B73" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C73" s="2" t="s">
         <v>2</v>
@@ -2423,10 +2426,10 @@
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B74" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C74" s="2" t="s">
         <v>2</v>
@@ -2434,10 +2437,10 @@
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B75" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C75" s="2" t="s">
         <v>2</v>
@@ -2445,10 +2448,10 @@
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B76" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C76" s="2" t="s">
         <v>2</v>
@@ -2456,10 +2459,10 @@
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B77" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C77" s="2" t="s">
         <v>2</v>
@@ -2467,53 +2470,53 @@
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" s="1">
+        <v>6</v>
+      </c>
+      <c r="B78" t="s">
+        <v>65</v>
+      </c>
+      <c r="C78" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A79" s="1">
         <v>7</v>
       </c>
-      <c r="B78" t="s">
+      <c r="B79" t="s">
         <v>64</v>
       </c>
-      <c r="C78" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C79" s="2"/>
+      <c r="C79" s="2" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A80" s="10" t="s">
+      <c r="C80" s="2"/>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A81" s="10" t="s">
         <v>92</v>
       </c>
-      <c r="B80" s="10"/>
-      <c r="C80" s="10"/>
-      <c r="D80" s="10"/>
-    </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A81" s="4" t="s">
+      <c r="B81" s="10"/>
+      <c r="C81" s="10"/>
+      <c r="D81" s="10"/>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A82" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="B81" s="5" t="s">
+      <c r="B82" s="5" t="s">
         <v>102</v>
       </c>
-      <c r="C81" s="4"/>
-      <c r="D81" s="6"/>
-    </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A82" s="1">
-        <v>1</v>
-      </c>
-      <c r="B82" t="s">
-        <v>94</v>
-      </c>
-      <c r="C82" s="2" t="s">
-        <v>2</v>
-      </c>
+      <c r="C82" s="4"/>
+      <c r="D82" s="6"/>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B83" t="s">
-        <v>26</v>
+        <v>94</v>
       </c>
       <c r="C83" s="2" t="s">
         <v>2</v>
@@ -2521,10 +2524,10 @@
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A84" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B84" t="s">
-        <v>93</v>
+        <v>26</v>
       </c>
       <c r="C84" s="2" t="s">
         <v>2</v>
@@ -2532,55 +2535,55 @@
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B85" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C85" s="2" t="s">
         <v>2</v>
-      </c>
-      <c r="D85" s="7" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A86" s="1">
+        <v>4</v>
+      </c>
+      <c r="B86" t="s">
+        <v>95</v>
+      </c>
+      <c r="C86" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D86" s="7" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A87" s="1">
         <v>5</v>
       </c>
-      <c r="B86" t="s">
+      <c r="B87" t="s">
         <v>234</v>
       </c>
-      <c r="C86" s="2"/>
-      <c r="D86" s="7"/>
-    </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A88" s="4" t="s">
+      <c r="C87" s="2"/>
+      <c r="D87" s="7"/>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A89" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="B88" s="5" t="s">
+      <c r="B89" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="C88" s="4"/>
-      <c r="D88" s="6"/>
-    </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A89" s="1">
-        <v>1</v>
-      </c>
-      <c r="B89" t="s">
-        <v>98</v>
-      </c>
-      <c r="C89" s="2" t="s">
-        <v>2</v>
-      </c>
+      <c r="C89" s="4"/>
+      <c r="D89" s="6"/>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A90" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B90" t="s">
-        <v>67</v>
+        <v>98</v>
       </c>
       <c r="C90" s="2" t="s">
         <v>2</v>
@@ -2588,10 +2591,10 @@
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A91" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B91" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C91" s="2" t="s">
         <v>2</v>
@@ -2599,10 +2602,10 @@
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A92" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B92" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C92" s="2" t="s">
         <v>2</v>
@@ -2610,10 +2613,10 @@
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A93" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B93" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C93" s="2" t="s">
         <v>2</v>
@@ -2621,10 +2624,10 @@
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A94" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B94" t="s">
-        <v>99</v>
+        <v>70</v>
       </c>
       <c r="C94" s="2" t="s">
         <v>2</v>
@@ -2632,10 +2635,10 @@
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A95" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B95" t="s">
-        <v>71</v>
+        <v>99</v>
       </c>
       <c r="C95" s="2" t="s">
         <v>2</v>
@@ -2643,10 +2646,10 @@
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A96" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B96" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C96" s="2" t="s">
         <v>2</v>
@@ -2654,35 +2657,35 @@
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A97" s="1">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B97" t="s">
-        <v>100</v>
+        <v>72</v>
       </c>
       <c r="C97" s="2" t="s">
         <v>2</v>
-      </c>
-      <c r="D97" s="7" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A98" s="1">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B98" t="s">
-        <v>77</v>
+        <v>100</v>
       </c>
       <c r="C98" s="2" t="s">
         <v>2</v>
+      </c>
+      <c r="D98" s="7" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A99" s="1">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B99" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C99" s="2" t="s">
         <v>2</v>
@@ -2690,10 +2693,10 @@
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A100" s="1">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B100" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="C100" s="2" t="s">
         <v>2</v>
@@ -2701,10 +2704,10 @@
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A101" s="1">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B101" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C101" s="2" t="s">
         <v>2</v>
@@ -2712,10 +2715,10 @@
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A102" s="1">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B102" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C102" s="2" t="s">
         <v>2</v>
@@ -2723,18 +2726,21 @@
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A103" s="1">
+        <v>14</v>
+      </c>
+      <c r="B103" t="s">
+        <v>75</v>
+      </c>
+      <c r="C103" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A104" s="1">
         <v>15</v>
       </c>
-      <c r="B103" t="s">
+      <c r="B104" t="s">
         <v>76</v>
-      </c>
-      <c r="C103" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B104" t="s">
-        <v>105</v>
       </c>
       <c r="C104" s="2" t="s">
         <v>2</v>
@@ -2742,18 +2748,15 @@
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B105" t="s">
+        <v>105</v>
+      </c>
+      <c r="C105" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B106" t="s">
         <v>106</v>
-      </c>
-      <c r="C105" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A106" s="1">
-        <v>16</v>
-      </c>
-      <c r="B106" t="s">
-        <v>77</v>
       </c>
       <c r="C106" s="2" t="s">
         <v>2</v>
@@ -2761,10 +2764,10 @@
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A107" s="1">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B107" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C107" s="2" t="s">
         <v>2</v>
@@ -2772,10 +2775,10 @@
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A108" s="1">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B108" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C108" s="2" t="s">
         <v>2</v>
@@ -2783,10 +2786,10 @@
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A109" s="1">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B109" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C109" s="2" t="s">
         <v>2</v>
@@ -2794,10 +2797,10 @@
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A110" s="1">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B110" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C110" s="2" t="s">
         <v>2</v>
@@ -2805,10 +2808,10 @@
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A111" s="1">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B111" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C111" s="2" t="s">
         <v>2</v>
@@ -2816,10 +2819,10 @@
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A112" s="1">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B112" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C112" s="2" t="s">
         <v>2</v>
@@ -2827,10 +2830,10 @@
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A113" s="1">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B113" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C113" s="2" t="s">
         <v>2</v>
@@ -2838,10 +2841,10 @@
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A114" s="1">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B114" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C114" s="2" t="s">
         <v>2</v>
@@ -2849,10 +2852,10 @@
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A115" s="1">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B115" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C115" s="2" t="s">
         <v>2</v>
@@ -2860,87 +2863,87 @@
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A116" s="1">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B116" t="s">
-        <v>87</v>
+        <v>86</v>
+      </c>
+      <c r="C116" s="2" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A117" s="1">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B117" t="s">
-        <v>88</v>
-      </c>
-      <c r="C117" s="2" t="s">
-        <v>2</v>
+        <v>87</v>
       </c>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A118" s="1">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B118" t="s">
-        <v>101</v>
-      </c>
-      <c r="C118" s="2"/>
+        <v>88</v>
+      </c>
+      <c r="C118" s="2" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A119" s="1">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B119" t="s">
-        <v>77</v>
+        <v>101</v>
       </c>
       <c r="C119" s="2"/>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A120" s="1">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B120" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C120" s="2"/>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A121" s="1">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B121" t="s">
-        <v>103</v>
-      </c>
-      <c r="C121" s="2" t="s">
-        <v>2</v>
-      </c>
+        <v>78</v>
+      </c>
+      <c r="C121" s="2"/>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A122" s="1">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B122" t="s">
-        <v>104</v>
-      </c>
-      <c r="C122" s="2"/>
+        <v>103</v>
+      </c>
+      <c r="C122" s="2" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A123" s="1">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B123" t="s">
-        <v>90</v>
-      </c>
-      <c r="D123" s="8" t="s">
-        <v>89</v>
-      </c>
+        <v>104</v>
+      </c>
+      <c r="C123" s="2"/>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A124" s="1">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B124" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D124" s="8" t="s">
         <v>89</v>
@@ -2948,60 +2951,60 @@
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A125" s="1">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B125" t="s">
-        <v>97</v>
-      </c>
-      <c r="D125" s="7" t="s">
-        <v>55</v>
+        <v>91</v>
+      </c>
+      <c r="D125" s="8" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A126" s="1">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B126" t="s">
-        <v>235</v>
-      </c>
-      <c r="C126" s="2" t="s">
-        <v>2</v>
+        <v>97</v>
       </c>
       <c r="D126" s="7" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C127" s="2"/>
-      <c r="D127" s="7"/>
+      <c r="A127" s="1">
+        <v>36</v>
+      </c>
+      <c r="B127" t="s">
+        <v>235</v>
+      </c>
+      <c r="C127" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D127" s="7" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A128" s="4" t="s">
+      <c r="C128" s="2"/>
+      <c r="D128" s="7"/>
+    </row>
+    <row r="129" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A129" s="4" t="s">
         <v>123</v>
       </c>
-      <c r="B128" s="5" t="s">
+      <c r="B129" s="5" t="s">
         <v>236</v>
       </c>
-      <c r="C128" s="4"/>
-      <c r="D128" s="6"/>
-    </row>
-    <row r="129" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A129" s="1">
-        <v>1</v>
-      </c>
-      <c r="B129" t="s">
-        <v>237</v>
-      </c>
-      <c r="C129" s="2" t="s">
-        <v>2</v>
-      </c>
+      <c r="C129" s="4"/>
+      <c r="D129" s="6"/>
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A130" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B130" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="C130" s="2" t="s">
         <v>2</v>
@@ -3009,10 +3012,10 @@
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A131" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B131" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="C131" s="2" t="s">
         <v>2</v>
@@ -3020,10 +3023,10 @@
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A132" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B132" t="s">
-        <v>246</v>
+        <v>238</v>
       </c>
       <c r="C132" s="2" t="s">
         <v>2</v>
@@ -3031,10 +3034,10 @@
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A133" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B133" t="s">
-        <v>244</v>
+        <v>246</v>
       </c>
       <c r="C133" s="2" t="s">
         <v>2</v>
@@ -3042,10 +3045,10 @@
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A134" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B134" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="C134" s="2" t="s">
         <v>2</v>
@@ -3053,10 +3056,10 @@
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A135" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B135" t="s">
-        <v>240</v>
+        <v>245</v>
       </c>
       <c r="C135" s="2" t="s">
         <v>2</v>
@@ -3064,10 +3067,10 @@
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A136" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B136" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="C136" s="2" t="s">
         <v>2</v>
@@ -3075,10 +3078,10 @@
     </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A137" s="1">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B137" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="C137" s="2" t="s">
         <v>2</v>
@@ -3086,44 +3089,44 @@
     </row>
     <row r="138" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A138" s="1">
+        <v>9</v>
+      </c>
+      <c r="B138" t="s">
+        <v>243</v>
+      </c>
+      <c r="C138" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="139" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A139" s="1">
         <v>10</v>
       </c>
-      <c r="B138" t="s">
+      <c r="B139" t="s">
         <v>14</v>
       </c>
-      <c r="C138" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="139" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A139"/>
-      <c r="C139" s="2"/>
+      <c r="C139" s="2" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="140" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A140" s="10" t="s">
+      <c r="A140"/>
+      <c r="C140" s="2"/>
+    </row>
+    <row r="141" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A141" s="10" t="s">
         <v>247</v>
       </c>
-      <c r="B140" s="10"/>
-      <c r="C140" s="10"/>
-      <c r="D140" s="10"/>
-    </row>
-    <row r="141" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A141" s="1">
-        <v>1</v>
-      </c>
-      <c r="B141" t="s">
-        <v>67</v>
-      </c>
-      <c r="C141" s="2" t="s">
-        <v>2</v>
-      </c>
+      <c r="B141" s="10"/>
+      <c r="C141" s="10"/>
+      <c r="D141" s="10"/>
     </row>
     <row r="142" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A142" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B142" t="s">
-        <v>248</v>
+        <v>67</v>
       </c>
       <c r="C142" s="2" t="s">
         <v>2</v>
@@ -3131,44 +3134,44 @@
     </row>
     <row r="143" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A143" s="1">
+        <v>2</v>
+      </c>
+      <c r="B143" t="s">
+        <v>248</v>
+      </c>
+      <c r="C143" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="144" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A144" s="1">
         <v>3</v>
       </c>
-      <c r="B143" t="s">
+      <c r="B144" t="s">
         <v>249</v>
       </c>
-      <c r="C143"/>
-    </row>
-    <row r="144" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A144"/>
       <c r="C144"/>
     </row>
     <row r="145" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A145" s="4" t="s">
+      <c r="A145"/>
+      <c r="C145"/>
+    </row>
+    <row r="146" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A146" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="B145" s="5" t="s">
+      <c r="B146" s="5" t="s">
         <v>250</v>
       </c>
-      <c r="C145" s="4"/>
-      <c r="D145" s="6"/>
-    </row>
-    <row r="146" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A146" s="1">
-        <v>1</v>
-      </c>
-      <c r="B146" t="s">
-        <v>67</v>
-      </c>
-      <c r="C146" s="2" t="s">
-        <v>2</v>
-      </c>
+      <c r="C146" s="4"/>
+      <c r="D146" s="6"/>
     </row>
     <row r="147" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A147" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B147" t="s">
-        <v>251</v>
+        <v>67</v>
       </c>
       <c r="C147" s="2" t="s">
         <v>2</v>
@@ -3176,10 +3179,10 @@
     </row>
     <row r="148" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A148" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B148" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C148" s="2" t="s">
         <v>2</v>
@@ -3187,10 +3190,10 @@
     </row>
     <row r="149" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A149" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B149" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="C149" s="2" t="s">
         <v>2</v>
@@ -3198,10 +3201,10 @@
     </row>
     <row r="150" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A150" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B150" t="s">
-        <v>253</v>
+        <v>255</v>
       </c>
       <c r="C150" s="2" t="s">
         <v>2</v>
@@ -3209,10 +3212,10 @@
     </row>
     <row r="151" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A151" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B151" t="s">
-        <v>14</v>
+        <v>253</v>
       </c>
       <c r="C151" s="2" t="s">
         <v>2</v>
@@ -3220,17 +3223,25 @@
     </row>
     <row r="152" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A152" s="1">
+        <v>6</v>
+      </c>
+      <c r="B152" t="s">
+        <v>14</v>
+      </c>
+      <c r="C152" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="153" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A153" s="1">
         <v>7</v>
       </c>
-      <c r="B152" t="s">
+      <c r="B153" t="s">
         <v>254</v>
       </c>
-      <c r="C152" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="153" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C153"/>
+      <c r="C153" s="2" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="154" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C154"/>
@@ -3250,52 +3261,44 @@
     <row r="159" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C159"/>
     </row>
-    <row r="161" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A161" s="10" t="s">
+    <row r="160" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C160"/>
+    </row>
+    <row r="162" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A162" s="10" t="s">
         <v>96</v>
       </c>
-      <c r="B161" s="10"/>
-      <c r="C161" s="10"/>
-      <c r="D161" s="10"/>
-    </row>
-    <row r="162" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A162" s="1">
+      <c r="B162" s="10"/>
+      <c r="C162" s="10"/>
+      <c r="D162" s="10"/>
+    </row>
+    <row r="163" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A163" s="1">
         <v>1</v>
       </c>
-      <c r="B162" t="s">
+      <c r="B163" t="s">
         <v>107</v>
       </c>
-      <c r="C162" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="163" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A163" s="4" t="s">
+      <c r="C163" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="164" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A164" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="B163" s="5" t="s">
+      <c r="B164" s="5" t="s">
         <v>108</v>
       </c>
-      <c r="C163" s="4"/>
-      <c r="D163" s="6"/>
-    </row>
-    <row r="164" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A164" s="1">
-        <v>1</v>
-      </c>
-      <c r="B164" t="s">
-        <v>109</v>
-      </c>
-      <c r="C164" s="2" t="s">
-        <v>2</v>
-      </c>
+      <c r="C164" s="4"/>
+      <c r="D164" s="6"/>
     </row>
     <row r="165" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A165" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B165" t="s">
-        <v>129</v>
+        <v>109</v>
       </c>
       <c r="C165" s="2" t="s">
         <v>2</v>
@@ -3303,10 +3306,10 @@
     </row>
     <row r="166" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A166" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B166" t="s">
-        <v>114</v>
+        <v>129</v>
       </c>
       <c r="C166" s="2" t="s">
         <v>2</v>
@@ -3314,10 +3317,10 @@
     </row>
     <row r="167" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A167" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B167" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C167" s="2" t="s">
         <v>2</v>
@@ -3325,10 +3328,10 @@
     </row>
     <row r="168" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A168" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B168" t="s">
-        <v>75</v>
+        <v>115</v>
       </c>
       <c r="C168" s="2" t="s">
         <v>2</v>
@@ -3336,10 +3339,10 @@
     </row>
     <row r="169" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A169" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B169" t="s">
-        <v>110</v>
+        <v>75</v>
       </c>
       <c r="C169" s="2" t="s">
         <v>2</v>
@@ -3347,10 +3350,10 @@
     </row>
     <row r="170" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A170" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B170" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C170" s="2" t="s">
         <v>2</v>
@@ -3358,10 +3361,10 @@
     </row>
     <row r="171" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A171" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B171" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C171" s="2" t="s">
         <v>2</v>
@@ -3369,10 +3372,10 @@
     </row>
     <row r="172" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A172" s="1">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B172" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C172" s="2" t="s">
         <v>2</v>
@@ -3380,10 +3383,10 @@
     </row>
     <row r="173" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A173" s="1">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B173" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="C173" s="2" t="s">
         <v>2</v>
@@ -3391,10 +3394,10 @@
     </row>
     <row r="174" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A174" s="1">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B174" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C174" s="2" t="s">
         <v>2</v>
@@ -3402,10 +3405,10 @@
     </row>
     <row r="175" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A175" s="1">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B175" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C175" s="2" t="s">
         <v>2</v>
@@ -3413,72 +3416,72 @@
     </row>
     <row r="176" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A176" s="1">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B176" t="s">
-        <v>130</v>
+        <v>118</v>
+      </c>
+      <c r="C176" s="2" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="177" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A177" s="1">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B177" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="178" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A178" s="1">
+        <v>14</v>
+      </c>
+      <c r="B178" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="179" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A179" s="1">
         <v>15</v>
       </c>
-      <c r="B178" t="s">
+      <c r="B179" t="s">
         <v>132</v>
       </c>
-      <c r="C178" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="179" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B179" t="s">
-        <v>128</v>
-      </c>
-      <c r="D179" s="7" t="s">
-        <v>55</v>
+      <c r="C179" s="2" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="180" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B180" t="s">
+        <v>128</v>
+      </c>
+      <c r="D180" s="7" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="181" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B181" t="s">
         <v>233</v>
       </c>
-      <c r="D180" s="7"/>
-    </row>
-    <row r="182" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A182" s="4" t="s">
+      <c r="D181" s="7"/>
+    </row>
+    <row r="183" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A183" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="B182" s="5" t="s">
+      <c r="B183" s="5" t="s">
         <v>119</v>
       </c>
-      <c r="C182" s="4"/>
-      <c r="D182" s="6"/>
-    </row>
-    <row r="183" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A183" s="1">
-        <v>1</v>
-      </c>
-      <c r="B183" t="s">
-        <v>120</v>
-      </c>
-      <c r="C183" s="2" t="s">
-        <v>2</v>
-      </c>
+      <c r="C183" s="4"/>
+      <c r="D183" s="6"/>
     </row>
     <row r="184" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A184" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B184" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C184" s="2" t="s">
         <v>2</v>
@@ -3486,10 +3489,10 @@
     </row>
     <row r="185" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A185" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B185" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C185" s="2" t="s">
         <v>2</v>
@@ -3497,10 +3500,10 @@
     </row>
     <row r="186" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A186" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B186" t="s">
-        <v>133</v>
+        <v>122</v>
       </c>
       <c r="C186" s="2" t="s">
         <v>2</v>
@@ -3508,40 +3511,40 @@
     </row>
     <row r="187" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A187" s="1">
+        <v>4</v>
+      </c>
+      <c r="B187" t="s">
+        <v>133</v>
+      </c>
+      <c r="C187" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="188" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A188" s="1">
         <v>5</v>
       </c>
-      <c r="B187" t="s">
+      <c r="B188" t="s">
         <v>134</v>
       </c>
-      <c r="C187" s="2"/>
-    </row>
-    <row r="189" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A189" s="4" t="s">
+      <c r="C188" s="2"/>
+    </row>
+    <row r="190" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A190" s="4" t="s">
         <v>123</v>
       </c>
-      <c r="B189" s="5" t="s">
+      <c r="B190" s="5" t="s">
         <v>124</v>
       </c>
-      <c r="C189" s="4"/>
-      <c r="D189" s="6"/>
-    </row>
-    <row r="190" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A190" s="1">
-        <v>1</v>
-      </c>
-      <c r="B190" t="s">
-        <v>125</v>
-      </c>
-      <c r="C190" s="2" t="s">
-        <v>2</v>
-      </c>
+      <c r="C190" s="4"/>
+      <c r="D190" s="6"/>
     </row>
     <row r="191" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A191" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B191" t="s">
-        <v>14</v>
+        <v>125</v>
       </c>
       <c r="C191" s="2" t="s">
         <v>2</v>
@@ -3549,10 +3552,10 @@
     </row>
     <row r="192" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A192" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B192" t="s">
-        <v>137</v>
+        <v>14</v>
       </c>
       <c r="C192" s="2" t="s">
         <v>2</v>
@@ -3560,10 +3563,10 @@
     </row>
     <row r="193" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A193" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B193" t="s">
-        <v>126</v>
+        <v>137</v>
       </c>
       <c r="C193" s="2" t="s">
         <v>2</v>
@@ -3571,29 +3574,29 @@
     </row>
     <row r="194" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A194" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B194" t="s">
-        <v>127</v>
+        <v>126</v>
+      </c>
+      <c r="C194" s="2" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="195" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A195" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B195" t="s">
-        <v>135</v>
-      </c>
-      <c r="C195" s="2" t="s">
-        <v>2</v>
+        <v>127</v>
       </c>
     </row>
     <row r="196" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A196" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B196" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C196" s="2" t="s">
         <v>2</v>
@@ -3601,10 +3604,10 @@
     </row>
     <row r="197" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A197" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B197" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="C197" s="2" t="s">
         <v>2</v>
@@ -3612,62 +3615,62 @@
     </row>
     <row r="198" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A198" s="1">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B198" t="s">
-        <v>139</v>
+        <v>138</v>
+      </c>
+      <c r="C198" s="2" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="199" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A199" s="1">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B199" t="s">
-        <v>140</v>
-      </c>
-      <c r="C199" s="2" t="s">
-        <v>2</v>
+        <v>139</v>
       </c>
     </row>
     <row r="200" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A200" s="1">
+        <v>10</v>
+      </c>
+      <c r="B200" t="s">
+        <v>140</v>
+      </c>
+      <c r="C200" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="201" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A201" s="1">
         <v>11</v>
       </c>
-      <c r="B200" t="s">
+      <c r="B201" t="s">
         <v>241</v>
       </c>
-      <c r="C200" s="2"/>
-      <c r="D200" s="7" t="s">
+      <c r="C201" s="2"/>
+      <c r="D201" s="7" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="202" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A202" s="4" t="s">
+    <row r="203" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A203" s="4" t="s">
         <v>141</v>
       </c>
-      <c r="B202" s="5" t="s">
+      <c r="B203" s="5" t="s">
         <v>142</v>
       </c>
-      <c r="C202" s="4"/>
-      <c r="D202" s="6"/>
-    </row>
-    <row r="203" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A203" s="1">
-        <v>1</v>
-      </c>
-      <c r="B203" t="s">
-        <v>125</v>
-      </c>
-      <c r="C203" s="2" t="s">
-        <v>2</v>
-      </c>
+      <c r="C203" s="4"/>
+      <c r="D203" s="6"/>
     </row>
     <row r="204" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A204" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B204" t="s">
-        <v>143</v>
+        <v>125</v>
       </c>
       <c r="C204" s="2" t="s">
         <v>2</v>
@@ -3675,10 +3678,10 @@
     </row>
     <row r="205" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A205" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B205" t="s">
-        <v>174</v>
+        <v>143</v>
       </c>
       <c r="C205" s="2" t="s">
         <v>2</v>
@@ -3686,10 +3689,10 @@
     </row>
     <row r="206" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A206" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B206" t="s">
-        <v>144</v>
+        <v>174</v>
       </c>
       <c r="C206" s="2" t="s">
         <v>2</v>
@@ -3697,10 +3700,10 @@
     </row>
     <row r="207" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A207" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B207" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C207" s="2" t="s">
         <v>2</v>
@@ -3708,10 +3711,10 @@
     </row>
     <row r="208" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A208" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B208" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C208" s="2" t="s">
         <v>2</v>
@@ -3719,10 +3722,10 @@
     </row>
     <row r="209" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A209" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B209" t="s">
-        <v>175</v>
+        <v>146</v>
       </c>
       <c r="C209" s="2" t="s">
         <v>2</v>
@@ -3730,10 +3733,10 @@
     </row>
     <row r="210" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A210" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B210" t="s">
-        <v>147</v>
+        <v>175</v>
       </c>
       <c r="C210" s="2" t="s">
         <v>2</v>
@@ -3741,10 +3744,10 @@
     </row>
     <row r="211" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A211" s="1">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B211" t="s">
-        <v>14</v>
+        <v>147</v>
       </c>
       <c r="C211" s="2" t="s">
         <v>2</v>
@@ -3752,52 +3755,52 @@
     </row>
     <row r="212" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A212" s="1">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B212" t="s">
-        <v>77</v>
-      </c>
-      <c r="C212" s="2"/>
+        <v>14</v>
+      </c>
+      <c r="C212" s="2" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="213" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A213" s="1">
+        <v>10</v>
+      </c>
+      <c r="B213" t="s">
+        <v>77</v>
+      </c>
+      <c r="C213" s="2"/>
+    </row>
+    <row r="214" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A214" s="1">
         <v>11</v>
       </c>
-      <c r="B213" t="s">
+      <c r="B214" t="s">
         <v>78</v>
       </c>
-      <c r="C213" s="2"/>
-    </row>
-    <row r="214" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C214" s="2"/>
     </row>
     <row r="215" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A215" s="4" t="s">
+      <c r="C215" s="2"/>
+    </row>
+    <row r="216" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A216" s="4" t="s">
         <v>148</v>
       </c>
-      <c r="B215" s="5" t="s">
+      <c r="B216" s="5" t="s">
         <v>158</v>
       </c>
-      <c r="C215" s="4"/>
-      <c r="D215" s="6"/>
-    </row>
-    <row r="216" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A216" s="1">
-        <v>1</v>
-      </c>
-      <c r="B216" t="s">
-        <v>125</v>
-      </c>
-      <c r="C216" s="2" t="s">
-        <v>2</v>
-      </c>
+      <c r="C216" s="4"/>
+      <c r="D216" s="6"/>
     </row>
     <row r="217" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A217" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B217" t="s">
-        <v>161</v>
+        <v>125</v>
       </c>
       <c r="C217" s="2" t="s">
         <v>2</v>
@@ -3805,10 +3808,10 @@
     </row>
     <row r="218" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A218" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B218" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C218" s="2" t="s">
         <v>2</v>
@@ -3816,10 +3819,10 @@
     </row>
     <row r="219" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A219" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B219" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="C219" s="2" t="s">
         <v>2</v>
@@ -3827,10 +3830,10 @@
     </row>
     <row r="220" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A220" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B220" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="C220" s="2" t="s">
         <v>2</v>
@@ -3838,10 +3841,10 @@
     </row>
     <row r="221" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A221" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B221" t="s">
-        <v>163</v>
+        <v>166</v>
       </c>
       <c r="C221" s="2" t="s">
         <v>2</v>
@@ -3849,10 +3852,10 @@
     </row>
     <row r="222" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A222" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B222" t="s">
-        <v>170</v>
+        <v>163</v>
       </c>
       <c r="C222" s="2" t="s">
         <v>2</v>
@@ -3860,10 +3863,10 @@
     </row>
     <row r="223" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A223" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B223" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="C223" s="2" t="s">
         <v>2</v>
@@ -3871,10 +3874,10 @@
     </row>
     <row r="224" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A224" s="1">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B224" t="s">
-        <v>165</v>
+        <v>169</v>
       </c>
       <c r="C224" s="2" t="s">
         <v>2</v>
@@ -3882,10 +3885,10 @@
     </row>
     <row r="225" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A225" s="1">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B225" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="C225" s="2" t="s">
         <v>2</v>
@@ -3893,10 +3896,10 @@
     </row>
     <row r="226" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A226" s="1">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B226" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C226" s="2" t="s">
         <v>2</v>
@@ -3904,10 +3907,10 @@
     </row>
     <row r="227" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A227" s="1">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B227" t="s">
-        <v>14</v>
+        <v>168</v>
       </c>
       <c r="C227" s="2" t="s">
         <v>2</v>
@@ -3915,49 +3918,49 @@
     </row>
     <row r="228" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A228" s="1">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B228" t="s">
-        <v>77</v>
-      </c>
-      <c r="C228" s="2"/>
+        <v>14</v>
+      </c>
+      <c r="C228" s="2" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="229" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A229" s="1">
+        <v>13</v>
+      </c>
+      <c r="B229" t="s">
+        <v>77</v>
+      </c>
+      <c r="C229" s="2"/>
+    </row>
+    <row r="230" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A230" s="1">
         <v>14</v>
       </c>
-      <c r="B229" t="s">
+      <c r="B230" t="s">
         <v>78</v>
       </c>
-      <c r="C229" s="2"/>
-    </row>
-    <row r="231" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A231" s="4" t="s">
+      <c r="C230" s="2"/>
+    </row>
+    <row r="232" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A232" s="4" t="s">
         <v>157</v>
       </c>
-      <c r="B231" s="5" t="s">
+      <c r="B232" s="5" t="s">
         <v>149</v>
       </c>
-      <c r="C231" s="4"/>
-      <c r="D231" s="6"/>
-    </row>
-    <row r="232" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A232" s="1">
-        <v>1</v>
-      </c>
-      <c r="B232" t="s">
-        <v>150</v>
-      </c>
-      <c r="C232" s="2" t="s">
-        <v>2</v>
-      </c>
+      <c r="C232" s="4"/>
+      <c r="D232" s="6"/>
     </row>
     <row r="233" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A233" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B233" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C233" s="2" t="s">
         <v>2</v>
@@ -3965,10 +3968,10 @@
     </row>
     <row r="234" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A234" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B234" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C234" s="2" t="s">
         <v>2</v>
@@ -3976,10 +3979,10 @@
     </row>
     <row r="235" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A235" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B235" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C235" s="2" t="s">
         <v>2</v>
@@ -3987,10 +3990,10 @@
     </row>
     <row r="236" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A236" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B236" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C236" s="2" t="s">
         <v>2</v>
@@ -3998,10 +4001,10 @@
     </row>
     <row r="237" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A237" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B237" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C237" s="2" t="s">
         <v>2</v>
@@ -4009,10 +4012,10 @@
     </row>
     <row r="238" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A238" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B238" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C238" s="2" t="s">
         <v>2</v>
@@ -4020,10 +4023,10 @@
     </row>
     <row r="239" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A239" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B239" t="s">
-        <v>14</v>
+        <v>156</v>
       </c>
       <c r="C239" s="2" t="s">
         <v>2</v>
@@ -4031,47 +4034,47 @@
     </row>
     <row r="240" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A240" s="1">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B240" t="s">
-        <v>77</v>
+        <v>14</v>
+      </c>
+      <c r="C240" s="2" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="241" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A241" s="1">
+        <v>9</v>
+      </c>
+      <c r="B241" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="242" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A242" s="1">
         <v>10</v>
       </c>
-      <c r="B241" t="s">
+      <c r="B242" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="243" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A243" s="4" t="s">
+    <row r="244" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A244" s="4" t="s">
         <v>159</v>
       </c>
-      <c r="B243" s="5" t="s">
+      <c r="B244" s="5" t="s">
         <v>160</v>
       </c>
-      <c r="C243" s="4"/>
-      <c r="D243" s="6"/>
-    </row>
-    <row r="244" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A244" s="1">
-        <v>1</v>
-      </c>
-      <c r="B244" t="s">
-        <v>171</v>
-      </c>
-      <c r="C244" s="2" t="s">
-        <v>2</v>
-      </c>
+      <c r="C244" s="4"/>
+      <c r="D244" s="6"/>
     </row>
     <row r="245" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A245" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B245" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C245" s="2" t="s">
         <v>2</v>
@@ -4079,10 +4082,10 @@
     </row>
     <row r="246" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A246" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B246" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C246" s="2" t="s">
         <v>2</v>
@@ -4090,10 +4093,10 @@
     </row>
     <row r="247" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A247" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B247" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="C247" s="2" t="s">
         <v>2</v>
@@ -4101,10 +4104,10 @@
     </row>
     <row r="248" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A248" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B248" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C248" s="2" t="s">
         <v>2</v>
@@ -4112,10 +4115,10 @@
     </row>
     <row r="249" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A249" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B249" t="s">
-        <v>14</v>
+        <v>177</v>
       </c>
       <c r="C249" s="2" t="s">
         <v>2</v>
@@ -4123,50 +4126,50 @@
     </row>
     <row r="250" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A250" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B250" t="s">
-        <v>77</v>
+        <v>14</v>
+      </c>
+      <c r="C250" s="2" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="251" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A251" s="1">
+        <v>7</v>
+      </c>
+      <c r="B251" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="252" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A252" s="1">
         <v>8</v>
       </c>
-      <c r="B251" t="s">
+      <c r="B252" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="252" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C252" s="2"/>
-    </row>
     <row r="253" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A253" s="4" t="s">
+      <c r="C253" s="2"/>
+    </row>
+    <row r="254" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A254" s="4" t="s">
         <v>178</v>
       </c>
-      <c r="B253" s="5" t="s">
+      <c r="B254" s="5" t="s">
         <v>179</v>
       </c>
-      <c r="C253" s="4"/>
-      <c r="D253" s="6"/>
-    </row>
-    <row r="254" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A254" s="1">
-        <v>1</v>
-      </c>
-      <c r="B254" t="s">
-        <v>125</v>
-      </c>
-      <c r="C254" s="2" t="s">
-        <v>2</v>
-      </c>
+      <c r="C254" s="4"/>
+      <c r="D254" s="6"/>
     </row>
     <row r="255" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A255" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B255" t="s">
-        <v>180</v>
+        <v>125</v>
       </c>
       <c r="C255" s="2" t="s">
         <v>2</v>
@@ -4174,10 +4177,10 @@
     </row>
     <row r="256" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A256" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B256" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C256" s="2" t="s">
         <v>2</v>
@@ -4185,10 +4188,10 @@
     </row>
     <row r="257" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A257" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B257" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C257" s="2" t="s">
         <v>2</v>
@@ -4196,10 +4199,10 @@
     </row>
     <row r="258" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A258" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B258" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C258" s="2" t="s">
         <v>2</v>
@@ -4207,10 +4210,10 @@
     </row>
     <row r="259" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A259" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B259" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C259" s="2" t="s">
         <v>2</v>
@@ -4218,10 +4221,10 @@
     </row>
     <row r="260" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A260" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B260" t="s">
-        <v>14</v>
+        <v>184</v>
       </c>
       <c r="C260" s="2" t="s">
         <v>2</v>
@@ -4229,47 +4232,47 @@
     </row>
     <row r="261" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A261" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B261" t="s">
-        <v>77</v>
+        <v>14</v>
+      </c>
+      <c r="C261" s="2" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="262" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A262" s="1">
+        <v>8</v>
+      </c>
+      <c r="B262" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="263" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A263" s="1">
         <v>9</v>
       </c>
-      <c r="B262" t="s">
+      <c r="B263" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="264" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A264" s="4" t="s">
+    <row r="265" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A265" s="4" t="s">
         <v>185</v>
       </c>
-      <c r="B264" s="5" t="s">
+      <c r="B265" s="5" t="s">
         <v>187</v>
       </c>
-      <c r="C264" s="4"/>
-      <c r="D264" s="6"/>
-    </row>
-    <row r="265" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A265" s="1">
-        <v>1</v>
-      </c>
-      <c r="B265" t="s">
-        <v>186</v>
-      </c>
-      <c r="C265" s="2" t="s">
-        <v>2</v>
-      </c>
+      <c r="C265" s="4"/>
+      <c r="D265" s="6"/>
     </row>
     <row r="266" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A266" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B266" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="C266" s="2" t="s">
         <v>2</v>
@@ -4277,10 +4280,10 @@
     </row>
     <row r="267" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A267" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B267" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C267" s="2" t="s">
         <v>2</v>
@@ -4288,10 +4291,10 @@
     </row>
     <row r="268" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A268" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B268" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C268" s="2" t="s">
         <v>2</v>
@@ -4299,10 +4302,10 @@
     </row>
     <row r="269" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A269" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B269" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C269" s="2" t="s">
         <v>2</v>
@@ -4310,10 +4313,10 @@
     </row>
     <row r="270" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A270" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B270" t="s">
-        <v>14</v>
+        <v>191</v>
       </c>
       <c r="C270" s="2" t="s">
         <v>2</v>
@@ -4321,47 +4324,47 @@
     </row>
     <row r="271" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A271" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B271" t="s">
-        <v>77</v>
+        <v>14</v>
+      </c>
+      <c r="C271" s="2" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="272" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A272" s="1">
+        <v>7</v>
+      </c>
+      <c r="B272" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="273" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A273" s="1">
         <v>8</v>
       </c>
-      <c r="B272" t="s">
+      <c r="B273" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="274" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A274" s="4" t="s">
+    <row r="275" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A275" s="4" t="s">
         <v>192</v>
       </c>
-      <c r="B274" s="5" t="s">
+      <c r="B275" s="5" t="s">
         <v>193</v>
       </c>
-      <c r="C274" s="4"/>
-      <c r="D274" s="6"/>
-    </row>
-    <row r="275" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A275" s="1">
-        <v>1</v>
-      </c>
-      <c r="B275" t="s">
-        <v>125</v>
-      </c>
-      <c r="C275" s="2" t="s">
-        <v>2</v>
-      </c>
+      <c r="C275" s="4"/>
+      <c r="D275" s="6"/>
     </row>
     <row r="276" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A276" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B276" t="s">
-        <v>194</v>
+        <v>125</v>
       </c>
       <c r="C276" s="2" t="s">
         <v>2</v>
@@ -4369,10 +4372,10 @@
     </row>
     <row r="277" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A277" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B277" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C277" s="2" t="s">
         <v>2</v>
@@ -4380,10 +4383,10 @@
     </row>
     <row r="278" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A278" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B278" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="C278" s="2" t="s">
         <v>2</v>
@@ -4391,10 +4394,10 @@
     </row>
     <row r="279" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A279" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B279" t="s">
-        <v>196</v>
+        <v>199</v>
       </c>
       <c r="C279" s="2" t="s">
         <v>2</v>
@@ -4402,10 +4405,10 @@
     </row>
     <row r="280" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A280" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B280" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C280" s="2" t="s">
         <v>2</v>
@@ -4413,10 +4416,10 @@
     </row>
     <row r="281" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A281" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B281" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C281" s="2" t="s">
         <v>2</v>
@@ -4424,10 +4427,10 @@
     </row>
     <row r="282" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A282" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B282" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="C282" s="2" t="s">
         <v>2</v>
@@ -4435,10 +4438,10 @@
     </row>
     <row r="283" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A283" s="1">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B283" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C283" s="2" t="s">
         <v>2</v>
@@ -4446,10 +4449,10 @@
     </row>
     <row r="284" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A284" s="1">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B284" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C284" s="2" t="s">
         <v>2</v>
@@ -4457,10 +4460,10 @@
     </row>
     <row r="285" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A285" s="1">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B285" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C285" s="2" t="s">
         <v>2</v>
@@ -4468,10 +4471,10 @@
     </row>
     <row r="286" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A286" s="1">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B286" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C286" s="2" t="s">
         <v>2</v>
@@ -4479,10 +4482,10 @@
     </row>
     <row r="287" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A287" s="1">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B287" t="s">
-        <v>14</v>
+        <v>204</v>
       </c>
       <c r="C287" s="2" t="s">
         <v>2</v>
@@ -4490,47 +4493,47 @@
     </row>
     <row r="288" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A288" s="1">
+        <v>13</v>
+      </c>
+      <c r="B288" t="s">
         <v>14</v>
       </c>
-      <c r="B288" t="s">
-        <v>77</v>
+      <c r="C288" s="2" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="289" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A289" s="1">
+        <v>14</v>
+      </c>
+      <c r="B289" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="290" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A290" s="1">
         <v>15</v>
       </c>
-      <c r="B289" t="s">
+      <c r="B290" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="291" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A291" s="4" t="s">
+    <row r="292" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A292" s="4" t="s">
         <v>205</v>
       </c>
-      <c r="B291" s="5" t="s">
+      <c r="B292" s="5" t="s">
         <v>206</v>
       </c>
-      <c r="C291" s="4"/>
-      <c r="D291" s="6"/>
-    </row>
-    <row r="292" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A292" s="1">
-        <v>1</v>
-      </c>
-      <c r="B292" t="s">
-        <v>125</v>
-      </c>
-      <c r="C292" s="2" t="s">
-        <v>2</v>
-      </c>
+      <c r="C292" s="4"/>
+      <c r="D292" s="6"/>
     </row>
     <row r="293" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A293" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B293" t="s">
-        <v>207</v>
+        <v>125</v>
       </c>
       <c r="C293" s="2" t="s">
         <v>2</v>
@@ -4538,10 +4541,10 @@
     </row>
     <row r="294" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A294" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B294" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C294" s="2" t="s">
         <v>2</v>
@@ -4549,10 +4552,10 @@
     </row>
     <row r="295" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A295" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B295" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C295" s="2" t="s">
         <v>2</v>
@@ -4560,10 +4563,10 @@
     </row>
     <row r="296" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A296" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B296" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C296" s="2" t="s">
         <v>2</v>
@@ -4571,10 +4574,10 @@
     </row>
     <row r="297" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A297" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B297" t="s">
-        <v>14</v>
+        <v>210</v>
       </c>
       <c r="C297" s="2" t="s">
         <v>2</v>
@@ -4582,47 +4585,47 @@
     </row>
     <row r="298" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A298" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B298" t="s">
-        <v>77</v>
+        <v>14</v>
+      </c>
+      <c r="C298" s="2" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="299" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A299" s="1">
+        <v>7</v>
+      </c>
+      <c r="B299" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="300" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A300" s="1">
         <v>8</v>
       </c>
-      <c r="B299" t="s">
+      <c r="B300" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="301" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A301" s="4" t="s">
+    <row r="302" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A302" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="B301" s="5" t="s">
+      <c r="B302" s="5" t="s">
         <v>212</v>
       </c>
-      <c r="C301" s="4"/>
-      <c r="D301" s="6"/>
-    </row>
-    <row r="302" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A302" s="1">
-        <v>1</v>
-      </c>
-      <c r="B302" t="s">
-        <v>213</v>
-      </c>
-      <c r="C302" s="2" t="s">
-        <v>2</v>
-      </c>
+      <c r="C302" s="4"/>
+      <c r="D302" s="6"/>
     </row>
     <row r="303" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A303" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B303" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C303" s="2" t="s">
         <v>2</v>
@@ -4630,10 +4633,10 @@
     </row>
     <row r="304" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A304" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B304" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C304" s="2" t="s">
         <v>2</v>
@@ -4641,10 +4644,10 @@
     </row>
     <row r="305" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A305" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B305" t="s">
-        <v>14</v>
+        <v>215</v>
       </c>
       <c r="C305" s="2" t="s">
         <v>2</v>
@@ -4652,49 +4655,49 @@
     </row>
     <row r="306" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A306" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B306" t="s">
-        <v>77</v>
-      </c>
-      <c r="C306" s="2"/>
+        <v>14</v>
+      </c>
+      <c r="C306" s="2" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="307" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A307" s="1">
+        <v>5</v>
+      </c>
+      <c r="B307" t="s">
+        <v>77</v>
+      </c>
+      <c r="C307" s="2"/>
+    </row>
+    <row r="308" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A308" s="1">
         <v>6</v>
       </c>
-      <c r="B307" t="s">
+      <c r="B308" t="s">
         <v>78</v>
       </c>
-      <c r="C307" s="2"/>
-    </row>
-    <row r="309" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A309" s="4" t="s">
+      <c r="C308" s="2"/>
+    </row>
+    <row r="310" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A310" s="4" t="s">
         <v>216</v>
       </c>
-      <c r="B309" s="5" t="s">
+      <c r="B310" s="5" t="s">
         <v>217</v>
       </c>
-      <c r="C309" s="4"/>
-      <c r="D309" s="6"/>
-    </row>
-    <row r="310" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A310" s="1">
-        <v>1</v>
-      </c>
-      <c r="B310" t="s">
-        <v>125</v>
-      </c>
-      <c r="C310" s="2" t="s">
-        <v>2</v>
-      </c>
+      <c r="C310" s="4"/>
+      <c r="D310" s="6"/>
     </row>
     <row r="311" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A311" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B311" t="s">
-        <v>218</v>
+        <v>125</v>
       </c>
       <c r="C311" s="2" t="s">
         <v>2</v>
@@ -4702,10 +4705,10 @@
     </row>
     <row r="312" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A312" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B312" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="C312" s="2" t="s">
         <v>2</v>
@@ -4713,10 +4716,10 @@
     </row>
     <row r="313" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A313" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B313" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C313" s="2" t="s">
         <v>2</v>
@@ -4724,10 +4727,10 @@
     </row>
     <row r="314" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A314" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B314" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="C314" s="2" t="s">
         <v>2</v>
@@ -4735,10 +4738,10 @@
     </row>
     <row r="315" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A315" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B315" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="C315" s="2" t="s">
         <v>2</v>
@@ -4746,10 +4749,10 @@
     </row>
     <row r="316" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A316" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B316" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="C316" s="2" t="s">
         <v>2</v>
@@ -4757,10 +4760,10 @@
     </row>
     <row r="317" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A317" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B317" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="C317" s="2" t="s">
         <v>2</v>
@@ -4768,10 +4771,10 @@
     </row>
     <row r="318" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A318" s="1">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B318" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C318" s="2" t="s">
         <v>2</v>
@@ -4779,10 +4782,10 @@
     </row>
     <row r="319" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A319" s="1">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B319" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C319" s="2" t="s">
         <v>2</v>
@@ -4790,10 +4793,10 @@
     </row>
     <row r="320" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A320" s="1">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B320" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C320" s="2" t="s">
         <v>2</v>
@@ -4801,10 +4804,10 @@
     </row>
     <row r="321" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A321" s="1">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B321" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="C321" s="2" t="s">
         <v>2</v>
@@ -4812,10 +4815,10 @@
     </row>
     <row r="322" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A322" s="1">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B322" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="C322" s="2" t="s">
         <v>2</v>
@@ -4823,10 +4826,10 @@
     </row>
     <row r="323" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A323" s="1">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B323" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="C323" s="2" t="s">
         <v>2</v>
@@ -4834,10 +4837,10 @@
     </row>
     <row r="324" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A324" s="1">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B324" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="C324" s="2" t="s">
         <v>2</v>
@@ -4845,10 +4848,10 @@
     </row>
     <row r="325" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A325" s="1">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B325" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C325" s="2" t="s">
         <v>2</v>
@@ -4856,10 +4859,10 @@
     </row>
     <row r="326" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A326" s="1">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B326" t="s">
-        <v>14</v>
+        <v>232</v>
       </c>
       <c r="C326" s="2" t="s">
         <v>2</v>
@@ -4867,31 +4870,42 @@
     </row>
     <row r="327" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A327" s="1">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B327" t="s">
-        <v>77</v>
+        <v>14</v>
+      </c>
+      <c r="C327" s="2" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="328" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A328" s="1">
+        <v>18</v>
+      </c>
+      <c r="B328" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="329" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A329" s="1">
         <v>19</v>
       </c>
-      <c r="B328" t="s">
+      <c r="B329" t="s">
         <v>78</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="9">
-    <mergeCell ref="A161:D161"/>
-    <mergeCell ref="A71:D71"/>
+    <mergeCell ref="A162:D162"/>
+    <mergeCell ref="A72:D72"/>
     <mergeCell ref="A1:D1"/>
-    <mergeCell ref="A7:D7"/>
-    <mergeCell ref="A17:D17"/>
-    <mergeCell ref="A48:D48"/>
-    <mergeCell ref="A66:D66"/>
-    <mergeCell ref="A80:D80"/>
-    <mergeCell ref="A140:D140"/>
+    <mergeCell ref="A8:D8"/>
+    <mergeCell ref="A18:D18"/>
+    <mergeCell ref="A49:D49"/>
+    <mergeCell ref="A67:D67"/>
+    <mergeCell ref="A81:D81"/>
+    <mergeCell ref="A141:D141"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Income Report (Not Complete)
</commit_message>
<xml_diff>
--- a/Tasks.xlsx
+++ b/Tasks.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="560" uniqueCount="267">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="562" uniqueCount="268">
   <si>
     <t>Login</t>
   </si>
@@ -1238,6 +1238,9 @@
   </si>
   <si>
     <t>اظهار اسم الموظف في راس الصفحة</t>
+  </si>
+  <si>
+    <t>Insert Survey_Id</t>
   </si>
 </sst>
 </file>
@@ -1720,10 +1723,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D329"/>
+  <dimension ref="A1:D330"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" topLeftCell="A124" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C140" sqref="C140"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3110,34 +3113,35 @@
       </c>
     </row>
     <row r="140" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A140"/>
+      <c r="A140" s="1">
+        <v>11</v>
+      </c>
+      <c r="B140" t="s">
+        <v>267</v>
+      </c>
       <c r="C140" s="2"/>
+      <c r="D140" s="7" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="141" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A141" s="10" t="s">
+      <c r="A141"/>
+      <c r="C141" s="2"/>
+    </row>
+    <row r="142" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A142" s="10" t="s">
         <v>247</v>
       </c>
-      <c r="B141" s="10"/>
-      <c r="C141" s="10"/>
-      <c r="D141" s="10"/>
-    </row>
-    <row r="142" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A142" s="1">
-        <v>1</v>
-      </c>
-      <c r="B142" t="s">
-        <v>67</v>
-      </c>
-      <c r="C142" s="2" t="s">
-        <v>2</v>
-      </c>
+      <c r="B142" s="10"/>
+      <c r="C142" s="10"/>
+      <c r="D142" s="10"/>
     </row>
     <row r="143" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A143" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B143" t="s">
-        <v>248</v>
+        <v>67</v>
       </c>
       <c r="C143" s="2" t="s">
         <v>2</v>
@@ -3145,44 +3149,44 @@
     </row>
     <row r="144" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A144" s="1">
+        <v>2</v>
+      </c>
+      <c r="B144" t="s">
+        <v>248</v>
+      </c>
+      <c r="C144" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="145" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A145" s="1">
         <v>3</v>
       </c>
-      <c r="B144" t="s">
+      <c r="B145" t="s">
         <v>249</v>
       </c>
-      <c r="C144"/>
-    </row>
-    <row r="145" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A145"/>
       <c r="C145"/>
     </row>
     <row r="146" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A146" s="4" t="s">
+      <c r="A146"/>
+      <c r="C146"/>
+    </row>
+    <row r="147" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A147" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="B146" s="5" t="s">
+      <c r="B147" s="5" t="s">
         <v>250</v>
       </c>
-      <c r="C146" s="4"/>
-      <c r="D146" s="6"/>
-    </row>
-    <row r="147" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A147" s="1">
-        <v>1</v>
-      </c>
-      <c r="B147" t="s">
-        <v>67</v>
-      </c>
-      <c r="C147" s="2" t="s">
-        <v>2</v>
-      </c>
+      <c r="C147" s="4"/>
+      <c r="D147" s="6"/>
     </row>
     <row r="148" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A148" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B148" t="s">
-        <v>251</v>
+        <v>67</v>
       </c>
       <c r="C148" s="2" t="s">
         <v>2</v>
@@ -3190,10 +3194,10 @@
     </row>
     <row r="149" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A149" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B149" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C149" s="2" t="s">
         <v>2</v>
@@ -3201,10 +3205,10 @@
     </row>
     <row r="150" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A150" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B150" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="C150" s="2" t="s">
         <v>2</v>
@@ -3212,10 +3216,10 @@
     </row>
     <row r="151" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A151" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B151" t="s">
-        <v>253</v>
+        <v>255</v>
       </c>
       <c r="C151" s="2" t="s">
         <v>2</v>
@@ -3223,10 +3227,10 @@
     </row>
     <row r="152" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A152" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B152" t="s">
-        <v>14</v>
+        <v>253</v>
       </c>
       <c r="C152" s="2" t="s">
         <v>2</v>
@@ -3234,17 +3238,25 @@
     </row>
     <row r="153" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A153" s="1">
+        <v>6</v>
+      </c>
+      <c r="B153" t="s">
+        <v>14</v>
+      </c>
+      <c r="C153" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="154" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A154" s="1">
         <v>7</v>
       </c>
-      <c r="B153" t="s">
+      <c r="B154" t="s">
         <v>254</v>
       </c>
-      <c r="C153" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="154" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C154"/>
+      <c r="C154" s="2" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="155" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C155"/>
@@ -3264,52 +3276,44 @@
     <row r="160" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C160"/>
     </row>
-    <row r="162" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A162" s="10" t="s">
+    <row r="161" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C161"/>
+    </row>
+    <row r="163" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A163" s="10" t="s">
         <v>96</v>
       </c>
-      <c r="B162" s="10"/>
-      <c r="C162" s="10"/>
-      <c r="D162" s="10"/>
-    </row>
-    <row r="163" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A163" s="1">
+      <c r="B163" s="10"/>
+      <c r="C163" s="10"/>
+      <c r="D163" s="10"/>
+    </row>
+    <row r="164" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A164" s="1">
         <v>1</v>
       </c>
-      <c r="B163" t="s">
+      <c r="B164" t="s">
         <v>107</v>
       </c>
-      <c r="C163" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="164" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A164" s="4" t="s">
+      <c r="C164" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="165" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A165" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="B164" s="5" t="s">
+      <c r="B165" s="5" t="s">
         <v>108</v>
       </c>
-      <c r="C164" s="4"/>
-      <c r="D164" s="6"/>
-    </row>
-    <row r="165" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A165" s="1">
-        <v>1</v>
-      </c>
-      <c r="B165" t="s">
-        <v>109</v>
-      </c>
-      <c r="C165" s="2" t="s">
-        <v>2</v>
-      </c>
+      <c r="C165" s="4"/>
+      <c r="D165" s="6"/>
     </row>
     <row r="166" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A166" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B166" t="s">
-        <v>129</v>
+        <v>109</v>
       </c>
       <c r="C166" s="2" t="s">
         <v>2</v>
@@ -3317,10 +3321,10 @@
     </row>
     <row r="167" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A167" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B167" t="s">
-        <v>114</v>
+        <v>129</v>
       </c>
       <c r="C167" s="2" t="s">
         <v>2</v>
@@ -3328,10 +3332,10 @@
     </row>
     <row r="168" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A168" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B168" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C168" s="2" t="s">
         <v>2</v>
@@ -3339,10 +3343,10 @@
     </row>
     <row r="169" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A169" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B169" t="s">
-        <v>75</v>
+        <v>115</v>
       </c>
       <c r="C169" s="2" t="s">
         <v>2</v>
@@ -3350,10 +3354,10 @@
     </row>
     <row r="170" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A170" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B170" t="s">
-        <v>110</v>
+        <v>75</v>
       </c>
       <c r="C170" s="2" t="s">
         <v>2</v>
@@ -3361,10 +3365,10 @@
     </row>
     <row r="171" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A171" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B171" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C171" s="2" t="s">
         <v>2</v>
@@ -3372,10 +3376,10 @@
     </row>
     <row r="172" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A172" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B172" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C172" s="2" t="s">
         <v>2</v>
@@ -3383,10 +3387,10 @@
     </row>
     <row r="173" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A173" s="1">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B173" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C173" s="2" t="s">
         <v>2</v>
@@ -3394,10 +3398,10 @@
     </row>
     <row r="174" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A174" s="1">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B174" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="C174" s="2" t="s">
         <v>2</v>
@@ -3405,10 +3409,10 @@
     </row>
     <row r="175" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A175" s="1">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B175" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C175" s="2" t="s">
         <v>2</v>
@@ -3416,10 +3420,10 @@
     </row>
     <row r="176" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A176" s="1">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B176" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C176" s="2" t="s">
         <v>2</v>
@@ -3427,72 +3431,72 @@
     </row>
     <row r="177" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A177" s="1">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B177" t="s">
-        <v>130</v>
+        <v>118</v>
+      </c>
+      <c r="C177" s="2" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="178" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A178" s="1">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B178" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="179" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A179" s="1">
+        <v>14</v>
+      </c>
+      <c r="B179" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="180" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A180" s="1">
         <v>15</v>
       </c>
-      <c r="B179" t="s">
+      <c r="B180" t="s">
         <v>132</v>
       </c>
-      <c r="C179" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="180" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B180" t="s">
-        <v>128</v>
-      </c>
-      <c r="D180" s="7" t="s">
-        <v>55</v>
+      <c r="C180" s="2" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="181" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B181" t="s">
+        <v>128</v>
+      </c>
+      <c r="D181" s="7" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="182" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B182" t="s">
         <v>233</v>
       </c>
-      <c r="D181" s="7"/>
-    </row>
-    <row r="183" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A183" s="4" t="s">
+      <c r="D182" s="7"/>
+    </row>
+    <row r="184" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A184" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="B183" s="5" t="s">
+      <c r="B184" s="5" t="s">
         <v>119</v>
       </c>
-      <c r="C183" s="4"/>
-      <c r="D183" s="6"/>
-    </row>
-    <row r="184" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A184" s="1">
-        <v>1</v>
-      </c>
-      <c r="B184" t="s">
-        <v>120</v>
-      </c>
-      <c r="C184" s="2" t="s">
-        <v>2</v>
-      </c>
+      <c r="C184" s="4"/>
+      <c r="D184" s="6"/>
     </row>
     <row r="185" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A185" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B185" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C185" s="2" t="s">
         <v>2</v>
@@ -3500,10 +3504,10 @@
     </row>
     <row r="186" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A186" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B186" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C186" s="2" t="s">
         <v>2</v>
@@ -3511,10 +3515,10 @@
     </row>
     <row r="187" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A187" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B187" t="s">
-        <v>133</v>
+        <v>122</v>
       </c>
       <c r="C187" s="2" t="s">
         <v>2</v>
@@ -3522,40 +3526,40 @@
     </row>
     <row r="188" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A188" s="1">
+        <v>4</v>
+      </c>
+      <c r="B188" t="s">
+        <v>133</v>
+      </c>
+      <c r="C188" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="189" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A189" s="1">
         <v>5</v>
       </c>
-      <c r="B188" t="s">
+      <c r="B189" t="s">
         <v>134</v>
       </c>
-      <c r="C188" s="2"/>
-    </row>
-    <row r="190" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A190" s="4" t="s">
+      <c r="C189" s="2"/>
+    </row>
+    <row r="191" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A191" s="4" t="s">
         <v>123</v>
       </c>
-      <c r="B190" s="5" t="s">
+      <c r="B191" s="5" t="s">
         <v>124</v>
       </c>
-      <c r="C190" s="4"/>
-      <c r="D190" s="6"/>
-    </row>
-    <row r="191" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A191" s="1">
-        <v>1</v>
-      </c>
-      <c r="B191" t="s">
-        <v>125</v>
-      </c>
-      <c r="C191" s="2" t="s">
-        <v>2</v>
-      </c>
+      <c r="C191" s="4"/>
+      <c r="D191" s="6"/>
     </row>
     <row r="192" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A192" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B192" t="s">
-        <v>14</v>
+        <v>125</v>
       </c>
       <c r="C192" s="2" t="s">
         <v>2</v>
@@ -3563,10 +3567,10 @@
     </row>
     <row r="193" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A193" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B193" t="s">
-        <v>137</v>
+        <v>14</v>
       </c>
       <c r="C193" s="2" t="s">
         <v>2</v>
@@ -3574,10 +3578,10 @@
     </row>
     <row r="194" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A194" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B194" t="s">
-        <v>126</v>
+        <v>137</v>
       </c>
       <c r="C194" s="2" t="s">
         <v>2</v>
@@ -3585,29 +3589,29 @@
     </row>
     <row r="195" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A195" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B195" t="s">
-        <v>127</v>
+        <v>126</v>
+      </c>
+      <c r="C195" s="2" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="196" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A196" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B196" t="s">
-        <v>135</v>
-      </c>
-      <c r="C196" s="2" t="s">
-        <v>2</v>
+        <v>127</v>
       </c>
     </row>
     <row r="197" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A197" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B197" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C197" s="2" t="s">
         <v>2</v>
@@ -3615,10 +3619,10 @@
     </row>
     <row r="198" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A198" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B198" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="C198" s="2" t="s">
         <v>2</v>
@@ -3626,62 +3630,62 @@
     </row>
     <row r="199" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A199" s="1">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B199" t="s">
-        <v>139</v>
+        <v>138</v>
+      </c>
+      <c r="C199" s="2" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="200" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A200" s="1">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B200" t="s">
-        <v>140</v>
-      </c>
-      <c r="C200" s="2" t="s">
-        <v>2</v>
+        <v>139</v>
       </c>
     </row>
     <row r="201" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A201" s="1">
+        <v>10</v>
+      </c>
+      <c r="B201" t="s">
+        <v>140</v>
+      </c>
+      <c r="C201" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="202" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A202" s="1">
         <v>11</v>
       </c>
-      <c r="B201" t="s">
+      <c r="B202" t="s">
         <v>241</v>
       </c>
-      <c r="C201" s="2"/>
-      <c r="D201" s="7" t="s">
+      <c r="C202" s="2"/>
+      <c r="D202" s="7" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="203" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A203" s="4" t="s">
+    <row r="204" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A204" s="4" t="s">
         <v>141</v>
       </c>
-      <c r="B203" s="5" t="s">
+      <c r="B204" s="5" t="s">
         <v>142</v>
       </c>
-      <c r="C203" s="4"/>
-      <c r="D203" s="6"/>
-    </row>
-    <row r="204" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A204" s="1">
-        <v>1</v>
-      </c>
-      <c r="B204" t="s">
-        <v>125</v>
-      </c>
-      <c r="C204" s="2" t="s">
-        <v>2</v>
-      </c>
+      <c r="C204" s="4"/>
+      <c r="D204" s="6"/>
     </row>
     <row r="205" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A205" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B205" t="s">
-        <v>143</v>
+        <v>125</v>
       </c>
       <c r="C205" s="2" t="s">
         <v>2</v>
@@ -3689,10 +3693,10 @@
     </row>
     <row r="206" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A206" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B206" t="s">
-        <v>174</v>
+        <v>143</v>
       </c>
       <c r="C206" s="2" t="s">
         <v>2</v>
@@ -3700,10 +3704,10 @@
     </row>
     <row r="207" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A207" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B207" t="s">
-        <v>144</v>
+        <v>174</v>
       </c>
       <c r="C207" s="2" t="s">
         <v>2</v>
@@ -3711,10 +3715,10 @@
     </row>
     <row r="208" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A208" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B208" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C208" s="2" t="s">
         <v>2</v>
@@ -3722,10 +3726,10 @@
     </row>
     <row r="209" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A209" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B209" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C209" s="2" t="s">
         <v>2</v>
@@ -3733,10 +3737,10 @@
     </row>
     <row r="210" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A210" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B210" t="s">
-        <v>175</v>
+        <v>146</v>
       </c>
       <c r="C210" s="2" t="s">
         <v>2</v>
@@ -3744,10 +3748,10 @@
     </row>
     <row r="211" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A211" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B211" t="s">
-        <v>147</v>
+        <v>175</v>
       </c>
       <c r="C211" s="2" t="s">
         <v>2</v>
@@ -3755,10 +3759,10 @@
     </row>
     <row r="212" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A212" s="1">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B212" t="s">
-        <v>14</v>
+        <v>147</v>
       </c>
       <c r="C212" s="2" t="s">
         <v>2</v>
@@ -3766,52 +3770,52 @@
     </row>
     <row r="213" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A213" s="1">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B213" t="s">
-        <v>77</v>
-      </c>
-      <c r="C213" s="2"/>
+        <v>14</v>
+      </c>
+      <c r="C213" s="2" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="214" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A214" s="1">
+        <v>10</v>
+      </c>
+      <c r="B214" t="s">
+        <v>77</v>
+      </c>
+      <c r="C214" s="2"/>
+    </row>
+    <row r="215" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A215" s="1">
         <v>11</v>
       </c>
-      <c r="B214" t="s">
+      <c r="B215" t="s">
         <v>78</v>
       </c>
-      <c r="C214" s="2"/>
-    </row>
-    <row r="215" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C215" s="2"/>
     </row>
     <row r="216" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A216" s="4" t="s">
+      <c r="C216" s="2"/>
+    </row>
+    <row r="217" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A217" s="4" t="s">
         <v>148</v>
       </c>
-      <c r="B216" s="5" t="s">
+      <c r="B217" s="5" t="s">
         <v>158</v>
       </c>
-      <c r="C216" s="4"/>
-      <c r="D216" s="6"/>
-    </row>
-    <row r="217" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A217" s="1">
-        <v>1</v>
-      </c>
-      <c r="B217" t="s">
-        <v>125</v>
-      </c>
-      <c r="C217" s="2" t="s">
-        <v>2</v>
-      </c>
+      <c r="C217" s="4"/>
+      <c r="D217" s="6"/>
     </row>
     <row r="218" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A218" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B218" t="s">
-        <v>161</v>
+        <v>125</v>
       </c>
       <c r="C218" s="2" t="s">
         <v>2</v>
@@ -3819,10 +3823,10 @@
     </row>
     <row r="219" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A219" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B219" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C219" s="2" t="s">
         <v>2</v>
@@ -3830,10 +3834,10 @@
     </row>
     <row r="220" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A220" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B220" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="C220" s="2" t="s">
         <v>2</v>
@@ -3841,10 +3845,10 @@
     </row>
     <row r="221" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A221" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B221" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="C221" s="2" t="s">
         <v>2</v>
@@ -3852,10 +3856,10 @@
     </row>
     <row r="222" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A222" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B222" t="s">
-        <v>163</v>
+        <v>166</v>
       </c>
       <c r="C222" s="2" t="s">
         <v>2</v>
@@ -3863,10 +3867,10 @@
     </row>
     <row r="223" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A223" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B223" t="s">
-        <v>170</v>
+        <v>163</v>
       </c>
       <c r="C223" s="2" t="s">
         <v>2</v>
@@ -3874,10 +3878,10 @@
     </row>
     <row r="224" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A224" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B224" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="C224" s="2" t="s">
         <v>2</v>
@@ -3885,10 +3889,10 @@
     </row>
     <row r="225" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A225" s="1">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B225" t="s">
-        <v>165</v>
+        <v>169</v>
       </c>
       <c r="C225" s="2" t="s">
         <v>2</v>
@@ -3896,10 +3900,10 @@
     </row>
     <row r="226" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A226" s="1">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B226" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="C226" s="2" t="s">
         <v>2</v>
@@ -3907,10 +3911,10 @@
     </row>
     <row r="227" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A227" s="1">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B227" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C227" s="2" t="s">
         <v>2</v>
@@ -3918,10 +3922,10 @@
     </row>
     <row r="228" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A228" s="1">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B228" t="s">
-        <v>14</v>
+        <v>168</v>
       </c>
       <c r="C228" s="2" t="s">
         <v>2</v>
@@ -3929,49 +3933,49 @@
     </row>
     <row r="229" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A229" s="1">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B229" t="s">
-        <v>77</v>
-      </c>
-      <c r="C229" s="2"/>
+        <v>14</v>
+      </c>
+      <c r="C229" s="2" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="230" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A230" s="1">
+        <v>13</v>
+      </c>
+      <c r="B230" t="s">
+        <v>77</v>
+      </c>
+      <c r="C230" s="2"/>
+    </row>
+    <row r="231" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A231" s="1">
         <v>14</v>
       </c>
-      <c r="B230" t="s">
+      <c r="B231" t="s">
         <v>78</v>
       </c>
-      <c r="C230" s="2"/>
-    </row>
-    <row r="232" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A232" s="4" t="s">
+      <c r="C231" s="2"/>
+    </row>
+    <row r="233" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A233" s="4" t="s">
         <v>157</v>
       </c>
-      <c r="B232" s="5" t="s">
+      <c r="B233" s="5" t="s">
         <v>149</v>
       </c>
-      <c r="C232" s="4"/>
-      <c r="D232" s="6"/>
-    </row>
-    <row r="233" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A233" s="1">
-        <v>1</v>
-      </c>
-      <c r="B233" t="s">
-        <v>150</v>
-      </c>
-      <c r="C233" s="2" t="s">
-        <v>2</v>
-      </c>
+      <c r="C233" s="4"/>
+      <c r="D233" s="6"/>
     </row>
     <row r="234" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A234" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B234" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C234" s="2" t="s">
         <v>2</v>
@@ -3979,10 +3983,10 @@
     </row>
     <row r="235" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A235" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B235" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C235" s="2" t="s">
         <v>2</v>
@@ -3990,10 +3994,10 @@
     </row>
     <row r="236" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A236" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B236" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C236" s="2" t="s">
         <v>2</v>
@@ -4001,10 +4005,10 @@
     </row>
     <row r="237" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A237" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B237" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C237" s="2" t="s">
         <v>2</v>
@@ -4012,10 +4016,10 @@
     </row>
     <row r="238" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A238" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B238" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C238" s="2" t="s">
         <v>2</v>
@@ -4023,10 +4027,10 @@
     </row>
     <row r="239" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A239" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B239" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C239" s="2" t="s">
         <v>2</v>
@@ -4034,10 +4038,10 @@
     </row>
     <row r="240" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A240" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B240" t="s">
-        <v>14</v>
+        <v>156</v>
       </c>
       <c r="C240" s="2" t="s">
         <v>2</v>
@@ -4045,47 +4049,47 @@
     </row>
     <row r="241" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A241" s="1">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B241" t="s">
-        <v>77</v>
+        <v>14</v>
+      </c>
+      <c r="C241" s="2" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="242" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A242" s="1">
+        <v>9</v>
+      </c>
+      <c r="B242" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="243" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A243" s="1">
         <v>10</v>
       </c>
-      <c r="B242" t="s">
+      <c r="B243" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="244" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A244" s="4" t="s">
+    <row r="245" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A245" s="4" t="s">
         <v>159</v>
       </c>
-      <c r="B244" s="5" t="s">
+      <c r="B245" s="5" t="s">
         <v>160</v>
       </c>
-      <c r="C244" s="4"/>
-      <c r="D244" s="6"/>
-    </row>
-    <row r="245" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A245" s="1">
-        <v>1</v>
-      </c>
-      <c r="B245" t="s">
-        <v>171</v>
-      </c>
-      <c r="C245" s="2" t="s">
-        <v>2</v>
-      </c>
+      <c r="C245" s="4"/>
+      <c r="D245" s="6"/>
     </row>
     <row r="246" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A246" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B246" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C246" s="2" t="s">
         <v>2</v>
@@ -4093,10 +4097,10 @@
     </row>
     <row r="247" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A247" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B247" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C247" s="2" t="s">
         <v>2</v>
@@ -4104,10 +4108,10 @@
     </row>
     <row r="248" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A248" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B248" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="C248" s="2" t="s">
         <v>2</v>
@@ -4115,10 +4119,10 @@
     </row>
     <row r="249" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A249" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B249" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C249" s="2" t="s">
         <v>2</v>
@@ -4126,10 +4130,10 @@
     </row>
     <row r="250" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A250" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B250" t="s">
-        <v>14</v>
+        <v>177</v>
       </c>
       <c r="C250" s="2" t="s">
         <v>2</v>
@@ -4137,50 +4141,50 @@
     </row>
     <row r="251" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A251" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B251" t="s">
-        <v>77</v>
+        <v>14</v>
+      </c>
+      <c r="C251" s="2" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="252" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A252" s="1">
+        <v>7</v>
+      </c>
+      <c r="B252" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="253" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A253" s="1">
         <v>8</v>
       </c>
-      <c r="B252" t="s">
+      <c r="B253" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="253" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C253" s="2"/>
-    </row>
     <row r="254" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A254" s="4" t="s">
+      <c r="C254" s="2"/>
+    </row>
+    <row r="255" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A255" s="4" t="s">
         <v>178</v>
       </c>
-      <c r="B254" s="5" t="s">
+      <c r="B255" s="5" t="s">
         <v>179</v>
       </c>
-      <c r="C254" s="4"/>
-      <c r="D254" s="6"/>
-    </row>
-    <row r="255" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A255" s="1">
-        <v>1</v>
-      </c>
-      <c r="B255" t="s">
-        <v>125</v>
-      </c>
-      <c r="C255" s="2" t="s">
-        <v>2</v>
-      </c>
+      <c r="C255" s="4"/>
+      <c r="D255" s="6"/>
     </row>
     <row r="256" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A256" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B256" t="s">
-        <v>180</v>
+        <v>125</v>
       </c>
       <c r="C256" s="2" t="s">
         <v>2</v>
@@ -4188,10 +4192,10 @@
     </row>
     <row r="257" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A257" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B257" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C257" s="2" t="s">
         <v>2</v>
@@ -4199,10 +4203,10 @@
     </row>
     <row r="258" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A258" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B258" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C258" s="2" t="s">
         <v>2</v>
@@ -4210,10 +4214,10 @@
     </row>
     <row r="259" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A259" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B259" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C259" s="2" t="s">
         <v>2</v>
@@ -4221,10 +4225,10 @@
     </row>
     <row r="260" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A260" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B260" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C260" s="2" t="s">
         <v>2</v>
@@ -4232,10 +4236,10 @@
     </row>
     <row r="261" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A261" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B261" t="s">
-        <v>14</v>
+        <v>184</v>
       </c>
       <c r="C261" s="2" t="s">
         <v>2</v>
@@ -4243,47 +4247,47 @@
     </row>
     <row r="262" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A262" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B262" t="s">
-        <v>77</v>
+        <v>14</v>
+      </c>
+      <c r="C262" s="2" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="263" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A263" s="1">
+        <v>8</v>
+      </c>
+      <c r="B263" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="264" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A264" s="1">
         <v>9</v>
       </c>
-      <c r="B263" t="s">
+      <c r="B264" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="265" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A265" s="4" t="s">
+    <row r="266" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A266" s="4" t="s">
         <v>185</v>
       </c>
-      <c r="B265" s="5" t="s">
+      <c r="B266" s="5" t="s">
         <v>187</v>
       </c>
-      <c r="C265" s="4"/>
-      <c r="D265" s="6"/>
-    </row>
-    <row r="266" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A266" s="1">
-        <v>1</v>
-      </c>
-      <c r="B266" t="s">
-        <v>186</v>
-      </c>
-      <c r="C266" s="2" t="s">
-        <v>2</v>
-      </c>
+      <c r="C266" s="4"/>
+      <c r="D266" s="6"/>
     </row>
     <row r="267" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A267" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B267" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="C267" s="2" t="s">
         <v>2</v>
@@ -4291,10 +4295,10 @@
     </row>
     <row r="268" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A268" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B268" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C268" s="2" t="s">
         <v>2</v>
@@ -4302,10 +4306,10 @@
     </row>
     <row r="269" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A269" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B269" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C269" s="2" t="s">
         <v>2</v>
@@ -4313,10 +4317,10 @@
     </row>
     <row r="270" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A270" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B270" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C270" s="2" t="s">
         <v>2</v>
@@ -4324,10 +4328,10 @@
     </row>
     <row r="271" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A271" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B271" t="s">
-        <v>14</v>
+        <v>191</v>
       </c>
       <c r="C271" s="2" t="s">
         <v>2</v>
@@ -4335,47 +4339,47 @@
     </row>
     <row r="272" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A272" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B272" t="s">
-        <v>77</v>
+        <v>14</v>
+      </c>
+      <c r="C272" s="2" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="273" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A273" s="1">
+        <v>7</v>
+      </c>
+      <c r="B273" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="274" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A274" s="1">
         <v>8</v>
       </c>
-      <c r="B273" t="s">
+      <c r="B274" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="275" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A275" s="4" t="s">
+    <row r="276" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A276" s="4" t="s">
         <v>192</v>
       </c>
-      <c r="B275" s="5" t="s">
+      <c r="B276" s="5" t="s">
         <v>193</v>
       </c>
-      <c r="C275" s="4"/>
-      <c r="D275" s="6"/>
-    </row>
-    <row r="276" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A276" s="1">
-        <v>1</v>
-      </c>
-      <c r="B276" t="s">
-        <v>125</v>
-      </c>
-      <c r="C276" s="2" t="s">
-        <v>2</v>
-      </c>
+      <c r="C276" s="4"/>
+      <c r="D276" s="6"/>
     </row>
     <row r="277" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A277" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B277" t="s">
-        <v>194</v>
+        <v>125</v>
       </c>
       <c r="C277" s="2" t="s">
         <v>2</v>
@@ -4383,10 +4387,10 @@
     </row>
     <row r="278" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A278" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B278" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C278" s="2" t="s">
         <v>2</v>
@@ -4394,10 +4398,10 @@
     </row>
     <row r="279" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A279" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B279" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="C279" s="2" t="s">
         <v>2</v>
@@ -4405,10 +4409,10 @@
     </row>
     <row r="280" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A280" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B280" t="s">
-        <v>196</v>
+        <v>199</v>
       </c>
       <c r="C280" s="2" t="s">
         <v>2</v>
@@ -4416,10 +4420,10 @@
     </row>
     <row r="281" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A281" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B281" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C281" s="2" t="s">
         <v>2</v>
@@ -4427,10 +4431,10 @@
     </row>
     <row r="282" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A282" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B282" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C282" s="2" t="s">
         <v>2</v>
@@ -4438,10 +4442,10 @@
     </row>
     <row r="283" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A283" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B283" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="C283" s="2" t="s">
         <v>2</v>
@@ -4449,10 +4453,10 @@
     </row>
     <row r="284" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A284" s="1">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B284" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C284" s="2" t="s">
         <v>2</v>
@@ -4460,10 +4464,10 @@
     </row>
     <row r="285" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A285" s="1">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B285" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C285" s="2" t="s">
         <v>2</v>
@@ -4471,10 +4475,10 @@
     </row>
     <row r="286" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A286" s="1">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B286" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C286" s="2" t="s">
         <v>2</v>
@@ -4482,10 +4486,10 @@
     </row>
     <row r="287" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A287" s="1">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B287" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C287" s="2" t="s">
         <v>2</v>
@@ -4493,10 +4497,10 @@
     </row>
     <row r="288" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A288" s="1">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B288" t="s">
-        <v>14</v>
+        <v>204</v>
       </c>
       <c r="C288" s="2" t="s">
         <v>2</v>
@@ -4504,47 +4508,47 @@
     </row>
     <row r="289" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A289" s="1">
+        <v>13</v>
+      </c>
+      <c r="B289" t="s">
         <v>14</v>
       </c>
-      <c r="B289" t="s">
-        <v>77</v>
+      <c r="C289" s="2" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="290" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A290" s="1">
+        <v>14</v>
+      </c>
+      <c r="B290" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="291" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A291" s="1">
         <v>15</v>
       </c>
-      <c r="B290" t="s">
+      <c r="B291" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="292" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A292" s="4" t="s">
+    <row r="293" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A293" s="4" t="s">
         <v>205</v>
       </c>
-      <c r="B292" s="5" t="s">
+      <c r="B293" s="5" t="s">
         <v>206</v>
       </c>
-      <c r="C292" s="4"/>
-      <c r="D292" s="6"/>
-    </row>
-    <row r="293" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A293" s="1">
-        <v>1</v>
-      </c>
-      <c r="B293" t="s">
-        <v>125</v>
-      </c>
-      <c r="C293" s="2" t="s">
-        <v>2</v>
-      </c>
+      <c r="C293" s="4"/>
+      <c r="D293" s="6"/>
     </row>
     <row r="294" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A294" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B294" t="s">
-        <v>207</v>
+        <v>125</v>
       </c>
       <c r="C294" s="2" t="s">
         <v>2</v>
@@ -4552,10 +4556,10 @@
     </row>
     <row r="295" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A295" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B295" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C295" s="2" t="s">
         <v>2</v>
@@ -4563,10 +4567,10 @@
     </row>
     <row r="296" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A296" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B296" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C296" s="2" t="s">
         <v>2</v>
@@ -4574,10 +4578,10 @@
     </row>
     <row r="297" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A297" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B297" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C297" s="2" t="s">
         <v>2</v>
@@ -4585,10 +4589,10 @@
     </row>
     <row r="298" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A298" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B298" t="s">
-        <v>14</v>
+        <v>210</v>
       </c>
       <c r="C298" s="2" t="s">
         <v>2</v>
@@ -4596,47 +4600,47 @@
     </row>
     <row r="299" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A299" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B299" t="s">
-        <v>77</v>
+        <v>14</v>
+      </c>
+      <c r="C299" s="2" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="300" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A300" s="1">
+        <v>7</v>
+      </c>
+      <c r="B300" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="301" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A301" s="1">
         <v>8</v>
       </c>
-      <c r="B300" t="s">
+      <c r="B301" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="302" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A302" s="4" t="s">
+    <row r="303" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A303" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="B302" s="5" t="s">
+      <c r="B303" s="5" t="s">
         <v>212</v>
       </c>
-      <c r="C302" s="4"/>
-      <c r="D302" s="6"/>
-    </row>
-    <row r="303" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A303" s="1">
-        <v>1</v>
-      </c>
-      <c r="B303" t="s">
-        <v>213</v>
-      </c>
-      <c r="C303" s="2" t="s">
-        <v>2</v>
-      </c>
+      <c r="C303" s="4"/>
+      <c r="D303" s="6"/>
     </row>
     <row r="304" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A304" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B304" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C304" s="2" t="s">
         <v>2</v>
@@ -4644,10 +4648,10 @@
     </row>
     <row r="305" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A305" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B305" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C305" s="2" t="s">
         <v>2</v>
@@ -4655,10 +4659,10 @@
     </row>
     <row r="306" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A306" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B306" t="s">
-        <v>14</v>
+        <v>215</v>
       </c>
       <c r="C306" s="2" t="s">
         <v>2</v>
@@ -4666,49 +4670,49 @@
     </row>
     <row r="307" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A307" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B307" t="s">
-        <v>77</v>
-      </c>
-      <c r="C307" s="2"/>
+        <v>14</v>
+      </c>
+      <c r="C307" s="2" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="308" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A308" s="1">
+        <v>5</v>
+      </c>
+      <c r="B308" t="s">
+        <v>77</v>
+      </c>
+      <c r="C308" s="2"/>
+    </row>
+    <row r="309" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A309" s="1">
         <v>6</v>
       </c>
-      <c r="B308" t="s">
+      <c r="B309" t="s">
         <v>78</v>
       </c>
-      <c r="C308" s="2"/>
-    </row>
-    <row r="310" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A310" s="4" t="s">
+      <c r="C309" s="2"/>
+    </row>
+    <row r="311" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A311" s="4" t="s">
         <v>216</v>
       </c>
-      <c r="B310" s="5" t="s">
+      <c r="B311" s="5" t="s">
         <v>217</v>
       </c>
-      <c r="C310" s="4"/>
-      <c r="D310" s="6"/>
-    </row>
-    <row r="311" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A311" s="1">
-        <v>1</v>
-      </c>
-      <c r="B311" t="s">
-        <v>125</v>
-      </c>
-      <c r="C311" s="2" t="s">
-        <v>2</v>
-      </c>
+      <c r="C311" s="4"/>
+      <c r="D311" s="6"/>
     </row>
     <row r="312" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A312" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B312" t="s">
-        <v>218</v>
+        <v>125</v>
       </c>
       <c r="C312" s="2" t="s">
         <v>2</v>
@@ -4716,10 +4720,10 @@
     </row>
     <row r="313" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A313" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B313" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="C313" s="2" t="s">
         <v>2</v>
@@ -4727,10 +4731,10 @@
     </row>
     <row r="314" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A314" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B314" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C314" s="2" t="s">
         <v>2</v>
@@ -4738,10 +4742,10 @@
     </row>
     <row r="315" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A315" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B315" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="C315" s="2" t="s">
         <v>2</v>
@@ -4749,10 +4753,10 @@
     </row>
     <row r="316" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A316" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B316" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="C316" s="2" t="s">
         <v>2</v>
@@ -4760,10 +4764,10 @@
     </row>
     <row r="317" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A317" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B317" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="C317" s="2" t="s">
         <v>2</v>
@@ -4771,10 +4775,10 @@
     </row>
     <row r="318" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A318" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B318" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="C318" s="2" t="s">
         <v>2</v>
@@ -4782,10 +4786,10 @@
     </row>
     <row r="319" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A319" s="1">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B319" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C319" s="2" t="s">
         <v>2</v>
@@ -4793,10 +4797,10 @@
     </row>
     <row r="320" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A320" s="1">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B320" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C320" s="2" t="s">
         <v>2</v>
@@ -4804,10 +4808,10 @@
     </row>
     <row r="321" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A321" s="1">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B321" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C321" s="2" t="s">
         <v>2</v>
@@ -4815,10 +4819,10 @@
     </row>
     <row r="322" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A322" s="1">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B322" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="C322" s="2" t="s">
         <v>2</v>
@@ -4826,10 +4830,10 @@
     </row>
     <row r="323" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A323" s="1">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B323" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="C323" s="2" t="s">
         <v>2</v>
@@ -4837,10 +4841,10 @@
     </row>
     <row r="324" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A324" s="1">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B324" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="C324" s="2" t="s">
         <v>2</v>
@@ -4848,10 +4852,10 @@
     </row>
     <row r="325" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A325" s="1">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B325" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="C325" s="2" t="s">
         <v>2</v>
@@ -4859,10 +4863,10 @@
     </row>
     <row r="326" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A326" s="1">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B326" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C326" s="2" t="s">
         <v>2</v>
@@ -4870,10 +4874,10 @@
     </row>
     <row r="327" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A327" s="1">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B327" t="s">
-        <v>14</v>
+        <v>232</v>
       </c>
       <c r="C327" s="2" t="s">
         <v>2</v>
@@ -4881,23 +4885,34 @@
     </row>
     <row r="328" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A328" s="1">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B328" t="s">
-        <v>77</v>
+        <v>14</v>
+      </c>
+      <c r="C328" s="2" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="329" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A329" s="1">
+        <v>18</v>
+      </c>
+      <c r="B329" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="330" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A330" s="1">
         <v>19</v>
       </c>
-      <c r="B329" t="s">
+      <c r="B330" t="s">
         <v>78</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="9">
-    <mergeCell ref="A162:D162"/>
+    <mergeCell ref="A163:D163"/>
     <mergeCell ref="A72:D72"/>
     <mergeCell ref="A1:D1"/>
     <mergeCell ref="A8:D8"/>
@@ -4905,7 +4920,7 @@
     <mergeCell ref="A49:D49"/>
     <mergeCell ref="A67:D67"/>
     <mergeCell ref="A81:D81"/>
-    <mergeCell ref="A141:D141"/>
+    <mergeCell ref="A142:D142"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>